<commit_message>
docs: Solution of 1945. Sum of Digits of String After Convert
Leetcode Problem 1945. Sum of Digits of String After Convert is solved and the learnings from it are captured

URL: https://leetcode.com/problems/sum-of-digits-of-string-after-convert/description/
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B55DD8-204C-4686-8693-7B157873276C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A67672-FD0A-49D7-A695-D331C2105534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Format" sheetId="2" r:id="rId2"/>
+    <sheet name="A" sheetId="1" r:id="rId1"/>
+    <sheet name="S" sheetId="3" r:id="rId2"/>
+    <sheet name="Format" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="249">
   <si>
     <t>Title</t>
   </si>
@@ -604,6 +605,214 @@
   </si>
   <si>
     <t>The hash map requires O(n) space to store the elements</t>
+  </si>
+  <si>
+    <t>1945. Sum of Digits of String After Convert</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/sum-of-digits-of-string-after-convert/description/?envType=problem-list-v2&amp;envId=string</t>
+  </si>
+  <si>
+    <t>#include &lt;string&gt;</t>
+  </si>
+  <si>
+    <t>#include &lt;iostream&gt;</t>
+  </si>
+  <si>
+    <t>int getLucky(std::string s, int k) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int asciiVal;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std::string valOfStr;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (int i = 0; i &lt; s.length(); i++) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        asciiVal = (int)(s[i]-96);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        valOfStr = valOfStr + std::to_string(asciiVal);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std::cout &lt;&lt; valOfStr &lt;&lt; '\n';</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    long long strVal = std::stoll(valOfStr);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std::cout &lt;&lt; strVal &lt;&lt; '\n';</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   for (int j = 1; j &lt;= k; j++) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int sum=0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        while (strVal &gt; 0) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            sum += strVal % 10;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            strVal /= 10;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        strVal = sum;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        std::cout &lt;&lt; sum &lt;&lt; '\n';</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (j==k)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            return sum;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   return 0;</t>
+  </si>
+  <si>
+    <t>void main() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std::string str1 = "leetcode";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int val = 2;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int result = getLucky(str1, val);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std::cout &lt;&lt; result;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std::string str = "";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (char ch : s) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        str += std::to_string((ch - 'a') + 1);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    long long num = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (char c : str) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        num += c - '0';</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    while (k &gt; 1) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int sum = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        while (num &gt; 0) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            sum += num % 10;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            num /= 10;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        num = sum;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        k--;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    return num;</t>
+  </si>
+  <si>
+    <t>Brute Force</t>
+  </si>
+  <si>
+    <t>From Solution</t>
+  </si>
+  <si>
+    <t>For looping through characters in string,</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We can use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>for (char ch : s)</t>
+    </r>
+  </si>
+  <si>
+    <t>We can directly typcast char to int to get the ascii value</t>
+  </si>
+  <si>
+    <t>Since a starts at 97,we can subtract 96</t>
+  </si>
+  <si>
+    <t>toget alphabet value</t>
+  </si>
+  <si>
+    <t>To convert int to string, use std::to_string(&lt;integer&gt;)</t>
+  </si>
+  <si>
+    <t>Instead hardcoding subtraction 96</t>
+  </si>
+  <si>
+    <t>We can subtract character a with the character in string</t>
+  </si>
+  <si>
+    <t>and finally add 1, since we considered a also</t>
+  </si>
+  <si>
+    <t>To convert string to int, use std::stoi(&lt;string&gt;)</t>
+  </si>
+  <si>
+    <t>To convert string to long, use std::stol(&lt;string&gt;)</t>
+  </si>
+  <si>
+    <t>To convert string to long long, use std::stoll(&lt;string&gt;)</t>
+  </si>
+  <si>
+    <t>Any number in char format - '0'(ascii value of 0)</t>
+  </si>
+  <si>
+    <t>Similar to subtracting a in the previous loop</t>
+  </si>
+  <si>
+    <t>Thus we get the sum of the number here</t>
+  </si>
+  <si>
+    <t>Coded like this, as we need sum</t>
+  </si>
+  <si>
+    <t>If we need the exact same number, we can code like below</t>
+  </si>
+  <si>
+    <t>num = num * 10 + (c - '0');</t>
+  </si>
+  <si>
+    <t>If we need to do something n no of times</t>
+  </si>
+  <si>
+    <t>use while (n&gt;0) and decrement it for each loop</t>
   </si>
 </sst>
 </file>
@@ -1143,7 +1352,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1461,8 +1672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE6A8EE-45F0-4DFE-8B47-A80E55C53C69}">
   <dimension ref="B1:AP399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="AA213" sqref="AA213"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.77734375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -3277,14 +3488,13 @@
     </row>
     <row r="114" spans="2:42" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B114" s="54"/>
-      <c r="C114" s="61" t="s">
+      <c r="C114" s="53" t="s">
         <v>143</v>
       </c>
       <c r="AP114" s="55"/>
     </row>
     <row r="115" spans="2:42" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B115" s="54"/>
-      <c r="C115" s="61"/>
       <c r="AP115" s="55"/>
     </row>
     <row r="116" spans="2:42" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
@@ -6386,6 +6596,1270 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28504ADD-8E4E-436B-849F-525BA36E82D6}">
+  <dimension ref="A2:BQ41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="AA35" sqref="AA35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="15" width="4.77734375" style="53"/>
+    <col min="16" max="19" width="4.77734375" style="53" customWidth="1"/>
+    <col min="20" max="20" width="4.77734375" style="53"/>
+    <col min="21" max="26" width="4.77734375" style="53" customWidth="1"/>
+    <col min="27" max="27" width="8.88671875" style="53"/>
+    <col min="28" max="69" width="4.77734375" style="53"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:69" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="61" t="s">
+        <v>185</v>
+      </c>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="1"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="1"/>
+      <c r="BC2" s="1"/>
+      <c r="BD2" s="1"/>
+      <c r="BE2" s="1"/>
+      <c r="BF2" s="1"/>
+      <c r="BG2" s="1"/>
+      <c r="BH2" s="1"/>
+      <c r="BI2" s="1"/>
+      <c r="BJ2" s="1"/>
+      <c r="BK2" s="1"/>
+      <c r="BL2" s="1"/>
+      <c r="BM2" s="1"/>
+      <c r="BN2" s="1"/>
+      <c r="BO2" s="1"/>
+      <c r="BP2" s="1"/>
+      <c r="BQ2" s="1"/>
+    </row>
+    <row r="3" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B3" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC3" s="59" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B4" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="AC4" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="9"/>
+      <c r="AI4" s="9"/>
+      <c r="AJ4" s="9"/>
+      <c r="AK4" s="9"/>
+      <c r="AL4" s="9"/>
+      <c r="AM4" s="9"/>
+    </row>
+    <row r="5" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B5" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="AC5" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9"/>
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="9"/>
+      <c r="AK5" s="9"/>
+      <c r="AL5" s="9"/>
+      <c r="AM5" s="9"/>
+    </row>
+    <row r="6" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
+      <c r="AJ6" s="9"/>
+      <c r="AK6" s="9"/>
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="9"/>
+    </row>
+    <row r="7" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B7" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="AC7" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
+    </row>
+    <row r="8" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B8" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="AC8" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="9"/>
+      <c r="AK8" s="9"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="9"/>
+    </row>
+    <row r="9" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B9" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="AC9" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
+      <c r="AP9" s="53" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B10" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="AC10" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
+      <c r="AQ10" s="53" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B11" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="53" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AP11" s="53" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B12" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="53" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="9"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="9"/>
+      <c r="AQ12" s="53" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="P13" s="53" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="9"/>
+      <c r="AJ13" s="9"/>
+      <c r="AK13" s="9"/>
+      <c r="AL13" s="9"/>
+      <c r="AM13" s="9"/>
+      <c r="AQ13" s="53" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="53" t="s">
+        <v>234</v>
+      </c>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
+      <c r="AG14" s="9"/>
+      <c r="AH14" s="9"/>
+      <c r="AI14" s="9"/>
+      <c r="AJ14" s="9"/>
+      <c r="AK14" s="9"/>
+      <c r="AL14" s="9"/>
+      <c r="AM14" s="9"/>
+    </row>
+    <row r="15" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="AC15" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="9"/>
+      <c r="AJ15" s="9"/>
+      <c r="AK15" s="9"/>
+      <c r="AL15" s="9"/>
+      <c r="AM15" s="9"/>
+      <c r="AP15" s="53" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="B16" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="AC16" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="9"/>
+      <c r="AJ16" s="9"/>
+      <c r="AK16" s="9"/>
+      <c r="AL16" s="9"/>
+      <c r="AM16" s="9"/>
+      <c r="AP16" s="53" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="17" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B17" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="53" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC17" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9"/>
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="9"/>
+      <c r="AI17" s="9"/>
+      <c r="AJ17" s="9"/>
+      <c r="AK17" s="9"/>
+      <c r="AL17" s="9"/>
+      <c r="AM17" s="9"/>
+      <c r="AP17" s="53" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B18" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="53" t="s">
+        <v>239</v>
+      </c>
+      <c r="AC18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="9"/>
+      <c r="AI18" s="9"/>
+      <c r="AJ18" s="9"/>
+      <c r="AK18" s="9"/>
+      <c r="AL18" s="9"/>
+      <c r="AM18" s="9"/>
+      <c r="AP18" s="53" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="53" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="9"/>
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="9"/>
+      <c r="AL19" s="9"/>
+      <c r="AM19" s="9"/>
+      <c r="AP19" s="53" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="9"/>
+      <c r="AI20" s="9"/>
+      <c r="AJ20" s="9"/>
+      <c r="AK20" s="9"/>
+      <c r="AL20" s="9"/>
+      <c r="AM20" s="9"/>
+      <c r="AQ20" s="53" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="21" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="9"/>
+      <c r="AI21" s="9"/>
+      <c r="AJ21" s="9"/>
+      <c r="AK21" s="9"/>
+      <c r="AL21" s="9"/>
+      <c r="AM21" s="9"/>
+    </row>
+    <row r="22" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B22" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="AC22" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="9"/>
+      <c r="AG22" s="9"/>
+      <c r="AH22" s="9"/>
+      <c r="AI22" s="9"/>
+      <c r="AJ22" s="9"/>
+      <c r="AK22" s="9"/>
+      <c r="AL22" s="9"/>
+      <c r="AM22" s="9"/>
+      <c r="AP22" s="53" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B23" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="AC23" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="AD23" s="9"/>
+      <c r="AE23" s="9"/>
+      <c r="AF23" s="9"/>
+      <c r="AG23" s="9"/>
+      <c r="AH23" s="9"/>
+      <c r="AI23" s="9"/>
+      <c r="AJ23" s="9"/>
+      <c r="AK23" s="9"/>
+      <c r="AL23" s="9"/>
+      <c r="AM23" s="9"/>
+      <c r="AQ23" s="53" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="24" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B24" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="AC24" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="9"/>
+      <c r="AF24" s="9"/>
+      <c r="AG24" s="9"/>
+      <c r="AH24" s="9"/>
+      <c r="AI24" s="9"/>
+      <c r="AJ24" s="9"/>
+      <c r="AK24" s="9"/>
+      <c r="AL24" s="9"/>
+      <c r="AM24" s="9"/>
+    </row>
+    <row r="25" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B25" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="AC25" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="9"/>
+      <c r="AF25" s="9"/>
+      <c r="AG25" s="9"/>
+      <c r="AH25" s="9"/>
+      <c r="AI25" s="9"/>
+      <c r="AJ25" s="9"/>
+      <c r="AK25" s="9"/>
+      <c r="AL25" s="9"/>
+      <c r="AM25" s="9"/>
+    </row>
+    <row r="26" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B26" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="AC26" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9"/>
+      <c r="AF26" s="9"/>
+      <c r="AG26" s="9"/>
+      <c r="AH26" s="9"/>
+      <c r="AI26" s="9"/>
+      <c r="AJ26" s="9"/>
+      <c r="AK26" s="9"/>
+      <c r="AL26" s="9"/>
+      <c r="AM26" s="9"/>
+    </row>
+    <row r="27" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B27" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="AC27" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="9"/>
+      <c r="AG27" s="9"/>
+      <c r="AH27" s="9"/>
+      <c r="AI27" s="9"/>
+      <c r="AJ27" s="9"/>
+      <c r="AK27" s="9"/>
+      <c r="AL27" s="9"/>
+      <c r="AM27" s="9"/>
+    </row>
+    <row r="28" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B28" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="AC28" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="9"/>
+      <c r="AF28" s="9"/>
+      <c r="AG28" s="9"/>
+      <c r="AH28" s="9"/>
+      <c r="AI28" s="9"/>
+      <c r="AJ28" s="9"/>
+      <c r="AK28" s="9"/>
+      <c r="AL28" s="9"/>
+      <c r="AM28" s="9"/>
+    </row>
+    <row r="29" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B29" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="AC29" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="9"/>
+      <c r="AF29" s="9"/>
+      <c r="AG29" s="9"/>
+      <c r="AH29" s="9"/>
+      <c r="AI29" s="9"/>
+      <c r="AJ29" s="9"/>
+      <c r="AK29" s="9"/>
+      <c r="AL29" s="9"/>
+      <c r="AM29" s="9"/>
+    </row>
+    <row r="30" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B30" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="AC30" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="9"/>
+      <c r="AF30" s="9"/>
+      <c r="AG30" s="9"/>
+      <c r="AH30" s="9"/>
+      <c r="AI30" s="9"/>
+      <c r="AJ30" s="9"/>
+      <c r="AK30" s="9"/>
+      <c r="AL30" s="9"/>
+      <c r="AM30" s="9"/>
+    </row>
+    <row r="31" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B31" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="AC31" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="9"/>
+      <c r="AF31" s="9"/>
+      <c r="AG31" s="9"/>
+      <c r="AH31" s="9"/>
+      <c r="AI31" s="9"/>
+      <c r="AJ31" s="9"/>
+      <c r="AK31" s="9"/>
+      <c r="AL31" s="9"/>
+      <c r="AM31" s="9"/>
+    </row>
+    <row r="32" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="B32" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="AC32" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="9"/>
+      <c r="AF32" s="9"/>
+      <c r="AG32" s="9"/>
+      <c r="AH32" s="9"/>
+      <c r="AI32" s="9"/>
+      <c r="AJ32" s="9"/>
+      <c r="AK32" s="9"/>
+      <c r="AL32" s="9"/>
+      <c r="AM32" s="9"/>
+    </row>
+    <row r="33" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="B33" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="AC33" s="9"/>
+      <c r="AD33" s="9"/>
+      <c r="AE33" s="9"/>
+      <c r="AF33" s="9"/>
+      <c r="AG33" s="9"/>
+      <c r="AH33" s="9"/>
+      <c r="AI33" s="9"/>
+      <c r="AJ33" s="9"/>
+      <c r="AK33" s="9"/>
+      <c r="AL33" s="9"/>
+      <c r="AM33" s="9"/>
+    </row>
+    <row r="34" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="B34" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="AC34" s="9"/>
+      <c r="AD34" s="9"/>
+      <c r="AE34" s="9"/>
+      <c r="AF34" s="9"/>
+      <c r="AG34" s="9"/>
+      <c r="AH34" s="9"/>
+      <c r="AI34" s="9"/>
+      <c r="AJ34" s="9"/>
+      <c r="AK34" s="9"/>
+      <c r="AL34" s="9"/>
+      <c r="AM34" s="9"/>
+    </row>
+    <row r="35" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="AC35" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="AD35" s="9"/>
+      <c r="AE35" s="9"/>
+      <c r="AF35" s="9"/>
+      <c r="AG35" s="9"/>
+      <c r="AH35" s="9"/>
+      <c r="AI35" s="9"/>
+      <c r="AJ35" s="9"/>
+      <c r="AK35" s="9"/>
+      <c r="AL35" s="9"/>
+      <c r="AM35" s="9"/>
+    </row>
+    <row r="36" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="B36" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="AC36" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="AD36" s="9"/>
+      <c r="AE36" s="9"/>
+      <c r="AF36" s="9"/>
+      <c r="AG36" s="9"/>
+      <c r="AH36" s="9"/>
+      <c r="AI36" s="9"/>
+      <c r="AJ36" s="9"/>
+      <c r="AK36" s="9"/>
+      <c r="AL36" s="9"/>
+      <c r="AM36" s="9"/>
+    </row>
+    <row r="37" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="B37" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="AC37" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="AD37" s="9"/>
+      <c r="AE37" s="9"/>
+      <c r="AF37" s="9"/>
+      <c r="AG37" s="9"/>
+      <c r="AH37" s="9"/>
+      <c r="AI37" s="9"/>
+      <c r="AJ37" s="9"/>
+      <c r="AK37" s="9"/>
+      <c r="AL37" s="9"/>
+      <c r="AM37" s="9"/>
+    </row>
+    <row r="38" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="B38" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="AC38" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="AD38" s="9"/>
+      <c r="AE38" s="9"/>
+      <c r="AF38" s="9"/>
+      <c r="AG38" s="9"/>
+      <c r="AH38" s="9"/>
+      <c r="AI38" s="9"/>
+      <c r="AJ38" s="9"/>
+      <c r="AK38" s="9"/>
+      <c r="AL38" s="9"/>
+      <c r="AM38" s="9"/>
+    </row>
+    <row r="39" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="B39" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="AC39" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD39" s="9"/>
+      <c r="AE39" s="9"/>
+      <c r="AF39" s="9"/>
+      <c r="AG39" s="9"/>
+      <c r="AH39" s="9"/>
+      <c r="AI39" s="9"/>
+      <c r="AJ39" s="9"/>
+      <c r="AK39" s="9"/>
+      <c r="AL39" s="9"/>
+      <c r="AM39" s="9"/>
+    </row>
+    <row r="40" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="B40" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="AC40" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD40" s="9"/>
+      <c r="AE40" s="9"/>
+      <c r="AF40" s="9"/>
+      <c r="AG40" s="9"/>
+      <c r="AH40" s="9"/>
+      <c r="AI40" s="9"/>
+      <c r="AJ40" s="9"/>
+      <c r="AK40" s="9"/>
+      <c r="AL40" s="9"/>
+      <c r="AM40" s="9"/>
+    </row>
+    <row r="41" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="B41" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{9E8104E2-0B1A-498B-A07D-38DAF385409A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AB2F21-1695-41F3-AD6E-505367934BD2}">
   <dimension ref="B1:AP84"/>
   <sheetViews>

</xml_diff>

<commit_message>
docs: 28. Find the Index of the First Occurrence in a String
Leetcode problem 28. Find the Index of the First Occurrence in a String is solved and the learnings from this are captured

URL: https://leetcode.com/problems/find-the-index-of-the-first-occurrence-in-a-string/description/?envType=problem-list-v2&envId=string
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A67672-FD0A-49D7-A695-D331C2105534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B38296B-8774-4C43-B22F-5108FD126ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="352">
   <si>
     <t>Title</t>
   </si>
@@ -814,12 +814,503 @@
   <si>
     <t>use while (n&gt;0) and decrement it for each loop</t>
   </si>
+  <si>
+    <t>#include &lt;cstring&gt; // For strlen</t>
+  </si>
+  <si>
+    <t>int getLucky(const char* s, int k) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int initialSum = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // Compute the initial digit sum from the character values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (int i = 0; s[i] != '\0'; ++i) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int value = s[i] - 'a' + 1; // Convert character to 1-based alphabetical position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        while (value &gt; 0) {         // Add the digits of the value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            initialSum += value % 10;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            value /= 10;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // Perform k-1 iterations of digit summation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int sum = initialSum;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (int i = 1; i &lt; k; ++i) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int tempSum = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        while (sum &gt; 0) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            tempSum += sum % 10;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            sum /= 10;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        sum = tempSum; // Update the sum for the next iteration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    return sum;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    const char* s = "leetcode"; // C-string input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int k = 2;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std::cout &lt;&lt; "Lucky number: " &lt;&lt; getLucky(s, k) &lt;&lt; std::endl;</t>
+  </si>
+  <si>
+    <t>28. Find the Index of the First Occurrence in a String</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-the-index-of-the-first-occurrence-in-a-string/description/?envType=problem-list-v2&amp;envId=string</t>
+  </si>
+  <si>
+    <t>BRUTE FORCE</t>
+  </si>
+  <si>
+    <t>int strStr(std::string haystack, std::string needle) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int x = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (int i = 0; i &lt; haystack.length(); i++) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (haystack[i] == needle[0]) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            x = i;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            for (int j = 0; j &lt; needle.length(); j++) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                if (needle[j] != haystack[x]) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    break;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                else {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    if (j == needle.length()-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                        return i;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    x++;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    return -1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std::string substr = "etco";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int result = strStr(str1, substr);</t>
+  </si>
+  <si>
+    <t>for loop is not used as ch:str</t>
+  </si>
+  <si>
+    <t>as we need to return i</t>
+  </si>
+  <si>
+    <t>class Solution {</t>
+  </si>
+  <si>
+    <t>public:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int strStr(std::string haystack, std::string needle) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        for (int i = 0; i &lt;= haystack.length() - needle.length(); ++i) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            if (haystack.substr(i, needle.length()) == needle) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                return i;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return -1;</t>
+  </si>
+  <si>
+    <t>};</t>
+  </si>
+  <si>
+    <t>FROM SOLUTION</t>
+  </si>
+  <si>
+    <t>substr(&lt;position&gt;,&lt;length&gt;) to get the substring</t>
+  </si>
+  <si>
+    <t>The condition is haystack length - needle length, as beyond that it is not possible</t>
+  </si>
+  <si>
+    <t>FROM CHATGPT</t>
+  </si>
+  <si>
+    <t>Finding length for each iteration is costly</t>
+  </si>
+  <si>
+    <t>So save it in a variable</t>
+  </si>
+  <si>
+    <t>int needleLen = needle.length();</t>
+  </si>
+  <si>
+    <t>int haystackLen = haystack.length();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        for (int i = 0; i &lt;= haystackLen - needleLen; ++i) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            if (haystack.substr(i, needleLen) == needle) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int j = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            ++j;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (int i = 0; i &lt;= haystackLen - needleLen; ++i) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        while (j &lt; needleLen &amp;&amp; haystack[i + j] == needle[j]) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (j == needleLen) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            return i;</t>
+  </si>
+  <si>
+    <t>Another way of finding substring using for loop without substr</t>
+  </si>
+  <si>
+    <t>By directly comparing characters in the while loop, you avoid the overhead of creating temporary strings with substr</t>
+  </si>
+  <si>
+    <t>std::vector&lt;int&gt; indices;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            indices.push_back(i);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return indices;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>std::vector&lt;int&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> strStr(std::string haystack, std::string needle) {</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">To get all the occurances, </t>
+  </si>
+  <si>
+    <t>initialise a vector</t>
+  </si>
+  <si>
+    <t>store the index in that vector instead returning it</t>
+  </si>
+  <si>
+    <t>return the vector</t>
+  </si>
+  <si>
+    <t>change the func return typ as it returs vector</t>
+  </si>
+  <si>
+    <t>Change in calling place also according to return type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std::string haystack = "subissubis";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std::string needle = "is";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std::cout &lt;&lt; "Indices of all occurrences: ";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for (int index : result) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        std::cout &lt;&lt; index &lt;&lt; " ";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std::vector&lt;int&gt; result = strStr(haystack, needle);</t>
+  </si>
+  <si>
+    <t>Modified  in calling place</t>
+  </si>
+  <si>
+    <t>Print statement made in loop as it is a vector</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>std::vector&lt;int&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> result = strStr(haystack, needle);</t>
+    </r>
+  </si>
+  <si>
+    <t>FROM CHATGPT(For C-String)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">int needleLen = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>strlen(needle)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">int haystackLen = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>strlen(haystack)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <t>We have to use strlen(&lt;string&gt;) for C-string</t>
+  </si>
+  <si>
+    <t>and &lt;string&gt;.length() for String</t>
+  </si>
+  <si>
+    <t>as String is like an object</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>char*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> needle = "is";</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>char*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> haystack = "subissubis";</t>
+    </r>
+  </si>
+  <si>
+    <t>Datatype changed fron std::string to char*</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    std::vector&lt;int&gt; strStr(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>char*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> haystack, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>char*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> needle) {</t>
+    </r>
+  </si>
+  <si>
+    <t>Datatype changed</t>
+  </si>
+  <si>
+    <t>We can also use char [] here instead char*</t>
+  </si>
+  <si>
+    <t>Use char* if you are working with string literals, dynamic memory, or passing strings to functions for flexibility</t>
+  </si>
+  <si>
+    <t>Use char arrays when you need local, writable storage with a fixed size</t>
+  </si>
+  <si>
+    <t>Based on these stuffs, we used char* here</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -982,6 +1473,21 @@
       <u/>
       <sz val="16"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFFFF00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1190,7 +1696,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1353,6 +1859,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6597,10 +7110,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28504ADD-8E4E-436B-849F-525BA36E82D6}">
-  <dimension ref="A2:BQ41"/>
+  <dimension ref="A2:FV76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="AA35" sqref="AA35"/>
+    <sheetView tabSelected="1" topLeftCell="EJ42" workbookViewId="0">
+      <selection activeCell="EV49" sqref="EV49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -6610,10 +7123,14 @@
     <col min="20" max="20" width="4.77734375" style="53"/>
     <col min="21" max="26" width="4.77734375" style="53" customWidth="1"/>
     <col min="27" max="27" width="8.88671875" style="53"/>
-    <col min="28" max="69" width="4.77734375" style="53"/>
+    <col min="28" max="59" width="4.77734375" style="53"/>
+    <col min="60" max="69" width="5.21875" style="53" customWidth="1"/>
+    <col min="70" max="173" width="5.21875" customWidth="1"/>
+    <col min="174" max="178" width="5.21875" style="53" customWidth="1"/>
+    <col min="179" max="180" width="5.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2" s="7" t="s">
         <v>184</v>
@@ -6688,7 +7205,7 @@
       <c r="BP2" s="1"/>
       <c r="BQ2" s="1"/>
     </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B3" s="59" t="s">
         <v>227</v>
       </c>
@@ -6696,7 +7213,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B4" s="9" t="s">
         <v>186</v>
       </c>
@@ -6725,8 +7242,26 @@
       <c r="AK4" s="9"/>
       <c r="AL4" s="9"/>
       <c r="AM4" s="9"/>
-    </row>
-    <row r="5" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="BF4" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="BG4" s="9"/>
+      <c r="BH4" s="9"/>
+      <c r="BI4" s="9"/>
+      <c r="BJ4" s="9"/>
+      <c r="BK4" s="9"/>
+      <c r="BL4" s="9"/>
+      <c r="BM4" s="9"/>
+      <c r="BN4" s="9"/>
+      <c r="BO4" s="9"/>
+      <c r="BP4" s="9"/>
+      <c r="BQ4" s="9"/>
+      <c r="BR4" s="9"/>
+      <c r="BS4" s="9"/>
+      <c r="BT4" s="9"/>
+      <c r="BU4" s="9"/>
+    </row>
+    <row r="5" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B5" s="9" t="s">
         <v>187</v>
       </c>
@@ -6755,8 +7290,26 @@
       <c r="AK5" s="9"/>
       <c r="AL5" s="9"/>
       <c r="AM5" s="9"/>
-    </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="BF5" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="BG5" s="9"/>
+      <c r="BH5" s="9"/>
+      <c r="BI5" s="9"/>
+      <c r="BJ5" s="9"/>
+      <c r="BK5" s="9"/>
+      <c r="BL5" s="9"/>
+      <c r="BM5" s="9"/>
+      <c r="BN5" s="9"/>
+      <c r="BO5" s="9"/>
+      <c r="BP5" s="9"/>
+      <c r="BQ5" s="9"/>
+      <c r="BR5" s="9"/>
+      <c r="BS5" s="9"/>
+      <c r="BT5" s="9"/>
+      <c r="BU5" s="9"/>
+    </row>
+    <row r="6" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -6781,8 +7334,24 @@
       <c r="AK6" s="9"/>
       <c r="AL6" s="9"/>
       <c r="AM6" s="9"/>
-    </row>
-    <row r="7" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="BF6" s="9"/>
+      <c r="BG6" s="9"/>
+      <c r="BH6" s="9"/>
+      <c r="BI6" s="9"/>
+      <c r="BJ6" s="9"/>
+      <c r="BK6" s="9"/>
+      <c r="BL6" s="9"/>
+      <c r="BM6" s="9"/>
+      <c r="BN6" s="9"/>
+      <c r="BO6" s="9"/>
+      <c r="BP6" s="9"/>
+      <c r="BQ6" s="9"/>
+      <c r="BR6" s="9"/>
+      <c r="BS6" s="9"/>
+      <c r="BT6" s="9"/>
+      <c r="BU6" s="9"/>
+    </row>
+    <row r="7" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B7" s="9" t="s">
         <v>188</v>
       </c>
@@ -6811,8 +7380,26 @@
       <c r="AK7" s="9"/>
       <c r="AL7" s="9"/>
       <c r="AM7" s="9"/>
-    </row>
-    <row r="8" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="BF7" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="BG7" s="9"/>
+      <c r="BH7" s="9"/>
+      <c r="BI7" s="9"/>
+      <c r="BJ7" s="9"/>
+      <c r="BK7" s="9"/>
+      <c r="BL7" s="9"/>
+      <c r="BM7" s="9"/>
+      <c r="BN7" s="9"/>
+      <c r="BO7" s="9"/>
+      <c r="BP7" s="9"/>
+      <c r="BQ7" s="9"/>
+      <c r="BR7" s="9"/>
+      <c r="BS7" s="9"/>
+      <c r="BT7" s="9"/>
+      <c r="BU7" s="9"/>
+    </row>
+    <row r="8" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B8" s="9" t="s">
         <v>189</v>
       </c>
@@ -6841,8 +7428,26 @@
       <c r="AK8" s="9"/>
       <c r="AL8" s="9"/>
       <c r="AM8" s="9"/>
-    </row>
-    <row r="9" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="BF8" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="BG8" s="9"/>
+      <c r="BH8" s="9"/>
+      <c r="BI8" s="9"/>
+      <c r="BJ8" s="9"/>
+      <c r="BK8" s="9"/>
+      <c r="BL8" s="9"/>
+      <c r="BM8" s="9"/>
+      <c r="BN8" s="9"/>
+      <c r="BO8" s="9"/>
+      <c r="BP8" s="9"/>
+      <c r="BQ8" s="9"/>
+      <c r="BR8" s="9"/>
+      <c r="BS8" s="9"/>
+      <c r="BT8" s="9"/>
+      <c r="BU8" s="9"/>
+    </row>
+    <row r="9" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B9" s="9" t="s">
         <v>190</v>
       </c>
@@ -6874,8 +7479,24 @@
       <c r="AP9" s="53" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="10" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="BF9" s="9"/>
+      <c r="BG9" s="9"/>
+      <c r="BH9" s="9"/>
+      <c r="BI9" s="9"/>
+      <c r="BJ9" s="9"/>
+      <c r="BK9" s="9"/>
+      <c r="BL9" s="9"/>
+      <c r="BM9" s="9"/>
+      <c r="BN9" s="9"/>
+      <c r="BO9" s="9"/>
+      <c r="BP9" s="9"/>
+      <c r="BQ9" s="9"/>
+      <c r="BR9" s="9"/>
+      <c r="BS9" s="9"/>
+      <c r="BT9" s="9"/>
+      <c r="BU9" s="9"/>
+    </row>
+    <row r="10" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B10" s="9" t="s">
         <v>191</v>
       </c>
@@ -6907,8 +7528,26 @@
       <c r="AQ10" s="53" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="11" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="BF10" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="BG10" s="9"/>
+      <c r="BH10" s="9"/>
+      <c r="BI10" s="9"/>
+      <c r="BJ10" s="9"/>
+      <c r="BK10" s="9"/>
+      <c r="BL10" s="9"/>
+      <c r="BM10" s="9"/>
+      <c r="BN10" s="9"/>
+      <c r="BO10" s="9"/>
+      <c r="BP10" s="9"/>
+      <c r="BQ10" s="9"/>
+      <c r="BR10" s="9"/>
+      <c r="BS10" s="9"/>
+      <c r="BT10" s="9"/>
+      <c r="BU10" s="9"/>
+    </row>
+    <row r="11" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B11" s="9" t="s">
         <v>192</v>
       </c>
@@ -6943,8 +7582,26 @@
       <c r="AP11" s="53" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="12" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="BF11" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="BG11" s="9"/>
+      <c r="BH11" s="9"/>
+      <c r="BI11" s="9"/>
+      <c r="BJ11" s="9"/>
+      <c r="BK11" s="9"/>
+      <c r="BL11" s="9"/>
+      <c r="BM11" s="9"/>
+      <c r="BN11" s="9"/>
+      <c r="BO11" s="9"/>
+      <c r="BP11" s="9"/>
+      <c r="BQ11" s="9"/>
+      <c r="BR11" s="9"/>
+      <c r="BS11" s="9"/>
+      <c r="BT11" s="9"/>
+      <c r="BU11" s="9"/>
+    </row>
+    <row r="12" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B12" s="9" t="s">
         <v>193</v>
       </c>
@@ -6977,8 +7634,26 @@
       <c r="AQ12" s="53" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="13" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="BF12" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="BG12" s="9"/>
+      <c r="BH12" s="9"/>
+      <c r="BI12" s="9"/>
+      <c r="BJ12" s="9"/>
+      <c r="BK12" s="9"/>
+      <c r="BL12" s="9"/>
+      <c r="BM12" s="9"/>
+      <c r="BN12" s="9"/>
+      <c r="BO12" s="9"/>
+      <c r="BP12" s="9"/>
+      <c r="BQ12" s="9"/>
+      <c r="BR12" s="9"/>
+      <c r="BS12" s="9"/>
+      <c r="BT12" s="9"/>
+      <c r="BU12" s="9"/>
+    </row>
+    <row r="13" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B13" s="9" t="s">
         <v>48</v>
       </c>
@@ -7011,8 +7686,26 @@
       <c r="AQ13" s="53" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="14" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="BF13" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="BG13" s="9"/>
+      <c r="BH13" s="9"/>
+      <c r="BI13" s="9"/>
+      <c r="BJ13" s="9"/>
+      <c r="BK13" s="9"/>
+      <c r="BL13" s="9"/>
+      <c r="BM13" s="9"/>
+      <c r="BN13" s="9"/>
+      <c r="BO13" s="9"/>
+      <c r="BP13" s="9"/>
+      <c r="BQ13" s="9"/>
+      <c r="BR13" s="9"/>
+      <c r="BS13" s="9"/>
+      <c r="BT13" s="9"/>
+      <c r="BU13" s="9"/>
+    </row>
+    <row r="14" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -7040,8 +7733,26 @@
       <c r="AK14" s="9"/>
       <c r="AL14" s="9"/>
       <c r="AM14" s="9"/>
-    </row>
-    <row r="15" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="BF14" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="BG14" s="9"/>
+      <c r="BH14" s="9"/>
+      <c r="BI14" s="9"/>
+      <c r="BJ14" s="9"/>
+      <c r="BK14" s="9"/>
+      <c r="BL14" s="9"/>
+      <c r="BM14" s="9"/>
+      <c r="BN14" s="9"/>
+      <c r="BO14" s="9"/>
+      <c r="BP14" s="9"/>
+      <c r="BQ14" s="9"/>
+      <c r="BR14" s="9"/>
+      <c r="BS14" s="9"/>
+      <c r="BT14" s="9"/>
+      <c r="BU14" s="9"/>
+    </row>
+    <row r="15" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -7071,8 +7782,26 @@
       <c r="AP15" s="53" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="16" spans="1:69" x14ac:dyDescent="0.4">
+      <c r="BF15" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="BG15" s="9"/>
+      <c r="BH15" s="9"/>
+      <c r="BI15" s="9"/>
+      <c r="BJ15" s="9"/>
+      <c r="BK15" s="9"/>
+      <c r="BL15" s="9"/>
+      <c r="BM15" s="9"/>
+      <c r="BN15" s="9"/>
+      <c r="BO15" s="9"/>
+      <c r="BP15" s="9"/>
+      <c r="BQ15" s="9"/>
+      <c r="BR15" s="9"/>
+      <c r="BS15" s="9"/>
+      <c r="BT15" s="9"/>
+      <c r="BU15" s="9"/>
+    </row>
+    <row r="16" spans="1:73" x14ac:dyDescent="0.4">
       <c r="B16" s="9" t="s">
         <v>194</v>
       </c>
@@ -7104,8 +7833,26 @@
       <c r="AP16" s="53" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="17" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF16" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="BG16" s="9"/>
+      <c r="BH16" s="9"/>
+      <c r="BI16" s="9"/>
+      <c r="BJ16" s="9"/>
+      <c r="BK16" s="9"/>
+      <c r="BL16" s="9"/>
+      <c r="BM16" s="9"/>
+      <c r="BN16" s="9"/>
+      <c r="BO16" s="9"/>
+      <c r="BP16" s="9"/>
+      <c r="BQ16" s="9"/>
+      <c r="BR16" s="9"/>
+      <c r="BS16" s="9"/>
+      <c r="BT16" s="9"/>
+      <c r="BU16" s="9"/>
+    </row>
+    <row r="17" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B17" s="9" t="s">
         <v>195</v>
       </c>
@@ -7140,8 +7887,26 @@
       <c r="AP17" s="53" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="18" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="BG17" s="9"/>
+      <c r="BH17" s="9"/>
+      <c r="BI17" s="9"/>
+      <c r="BJ17" s="9"/>
+      <c r="BK17" s="9"/>
+      <c r="BL17" s="9"/>
+      <c r="BM17" s="9"/>
+      <c r="BN17" s="9"/>
+      <c r="BO17" s="9"/>
+      <c r="BP17" s="9"/>
+      <c r="BQ17" s="9"/>
+      <c r="BR17" s="9"/>
+      <c r="BS17" s="9"/>
+      <c r="BT17" s="9"/>
+      <c r="BU17" s="9"/>
+    </row>
+    <row r="18" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B18" s="9" t="s">
         <v>196</v>
       </c>
@@ -7176,8 +7941,24 @@
       <c r="AP18" s="53" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="19" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF18" s="9"/>
+      <c r="BG18" s="9"/>
+      <c r="BH18" s="9"/>
+      <c r="BI18" s="9"/>
+      <c r="BJ18" s="9"/>
+      <c r="BK18" s="9"/>
+      <c r="BL18" s="9"/>
+      <c r="BM18" s="9"/>
+      <c r="BN18" s="9"/>
+      <c r="BO18" s="9"/>
+      <c r="BP18" s="9"/>
+      <c r="BQ18" s="9"/>
+      <c r="BR18" s="9"/>
+      <c r="BS18" s="9"/>
+      <c r="BT18" s="9"/>
+      <c r="BU18" s="9"/>
+    </row>
+    <row r="19" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -7208,8 +7989,26 @@
       <c r="AP19" s="53" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="20" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF19" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="BG19" s="9"/>
+      <c r="BH19" s="9"/>
+      <c r="BI19" s="9"/>
+      <c r="BJ19" s="9"/>
+      <c r="BK19" s="9"/>
+      <c r="BL19" s="9"/>
+      <c r="BM19" s="9"/>
+      <c r="BN19" s="9"/>
+      <c r="BO19" s="9"/>
+      <c r="BP19" s="9"/>
+      <c r="BQ19" s="9"/>
+      <c r="BR19" s="9"/>
+      <c r="BS19" s="9"/>
+      <c r="BT19" s="9"/>
+      <c r="BU19" s="9"/>
+    </row>
+    <row r="20" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -7237,8 +8036,26 @@
       <c r="AQ20" s="53" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="21" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF20" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="BG20" s="9"/>
+      <c r="BH20" s="9"/>
+      <c r="BI20" s="9"/>
+      <c r="BJ20" s="9"/>
+      <c r="BK20" s="9"/>
+      <c r="BL20" s="9"/>
+      <c r="BM20" s="9"/>
+      <c r="BN20" s="9"/>
+      <c r="BO20" s="9"/>
+      <c r="BP20" s="9"/>
+      <c r="BQ20" s="9"/>
+      <c r="BR20" s="9"/>
+      <c r="BS20" s="9"/>
+      <c r="BT20" s="9"/>
+      <c r="BU20" s="9"/>
+    </row>
+    <row r="21" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -7263,8 +8080,26 @@
       <c r="AK21" s="9"/>
       <c r="AL21" s="9"/>
       <c r="AM21" s="9"/>
-    </row>
-    <row r="22" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF21" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="BG21" s="9"/>
+      <c r="BH21" s="9"/>
+      <c r="BI21" s="9"/>
+      <c r="BJ21" s="9"/>
+      <c r="BK21" s="9"/>
+      <c r="BL21" s="9"/>
+      <c r="BM21" s="9"/>
+      <c r="BN21" s="9"/>
+      <c r="BO21" s="9"/>
+      <c r="BP21" s="9"/>
+      <c r="BQ21" s="9"/>
+      <c r="BR21" s="9"/>
+      <c r="BS21" s="9"/>
+      <c r="BT21" s="9"/>
+      <c r="BU21" s="9"/>
+    </row>
+    <row r="22" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B22" s="9" t="s">
         <v>197</v>
       </c>
@@ -7296,8 +8131,26 @@
       <c r="AP22" s="53" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="23" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF22" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="BG22" s="9"/>
+      <c r="BH22" s="9"/>
+      <c r="BI22" s="9"/>
+      <c r="BJ22" s="9"/>
+      <c r="BK22" s="9"/>
+      <c r="BL22" s="9"/>
+      <c r="BM22" s="9"/>
+      <c r="BN22" s="9"/>
+      <c r="BO22" s="9"/>
+      <c r="BP22" s="9"/>
+      <c r="BQ22" s="9"/>
+      <c r="BR22" s="9"/>
+      <c r="BS22" s="9"/>
+      <c r="BT22" s="9"/>
+      <c r="BU22" s="9"/>
+    </row>
+    <row r="23" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B23" s="9" t="s">
         <v>198</v>
       </c>
@@ -7329,8 +8182,26 @@
       <c r="AQ23" s="53" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="24" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF23" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="BG23" s="9"/>
+      <c r="BH23" s="9"/>
+      <c r="BI23" s="9"/>
+      <c r="BJ23" s="9"/>
+      <c r="BK23" s="9"/>
+      <c r="BL23" s="9"/>
+      <c r="BM23" s="9"/>
+      <c r="BN23" s="9"/>
+      <c r="BO23" s="9"/>
+      <c r="BP23" s="9"/>
+      <c r="BQ23" s="9"/>
+      <c r="BR23" s="9"/>
+      <c r="BS23" s="9"/>
+      <c r="BT23" s="9"/>
+      <c r="BU23" s="9"/>
+    </row>
+    <row r="24" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B24" s="9" t="s">
         <v>199</v>
       </c>
@@ -7359,8 +8230,26 @@
       <c r="AK24" s="9"/>
       <c r="AL24" s="9"/>
       <c r="AM24" s="9"/>
-    </row>
-    <row r="25" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF24" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="BG24" s="9"/>
+      <c r="BH24" s="9"/>
+      <c r="BI24" s="9"/>
+      <c r="BJ24" s="9"/>
+      <c r="BK24" s="9"/>
+      <c r="BL24" s="9"/>
+      <c r="BM24" s="9"/>
+      <c r="BN24" s="9"/>
+      <c r="BO24" s="9"/>
+      <c r="BP24" s="9"/>
+      <c r="BQ24" s="9"/>
+      <c r="BR24" s="9"/>
+      <c r="BS24" s="9"/>
+      <c r="BT24" s="9"/>
+      <c r="BU24" s="9"/>
+    </row>
+    <row r="25" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B25" s="9" t="s">
         <v>200</v>
       </c>
@@ -7389,8 +8278,26 @@
       <c r="AK25" s="9"/>
       <c r="AL25" s="9"/>
       <c r="AM25" s="9"/>
-    </row>
-    <row r="26" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF25" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="BG25" s="9"/>
+      <c r="BH25" s="9"/>
+      <c r="BI25" s="9"/>
+      <c r="BJ25" s="9"/>
+      <c r="BK25" s="9"/>
+      <c r="BL25" s="9"/>
+      <c r="BM25" s="9"/>
+      <c r="BN25" s="9"/>
+      <c r="BO25" s="9"/>
+      <c r="BP25" s="9"/>
+      <c r="BQ25" s="9"/>
+      <c r="BR25" s="9"/>
+      <c r="BS25" s="9"/>
+      <c r="BT25" s="9"/>
+      <c r="BU25" s="9"/>
+    </row>
+    <row r="26" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B26" s="9" t="s">
         <v>201</v>
       </c>
@@ -7419,8 +8326,26 @@
       <c r="AK26" s="9"/>
       <c r="AL26" s="9"/>
       <c r="AM26" s="9"/>
-    </row>
-    <row r="27" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF26" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="BG26" s="9"/>
+      <c r="BH26" s="9"/>
+      <c r="BI26" s="9"/>
+      <c r="BJ26" s="9"/>
+      <c r="BK26" s="9"/>
+      <c r="BL26" s="9"/>
+      <c r="BM26" s="9"/>
+      <c r="BN26" s="9"/>
+      <c r="BO26" s="9"/>
+      <c r="BP26" s="9"/>
+      <c r="BQ26" s="9"/>
+      <c r="BR26" s="9"/>
+      <c r="BS26" s="9"/>
+      <c r="BT26" s="9"/>
+      <c r="BU26" s="9"/>
+    </row>
+    <row r="27" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B27" s="9" t="s">
         <v>202</v>
       </c>
@@ -7449,8 +8374,26 @@
       <c r="AK27" s="9"/>
       <c r="AL27" s="9"/>
       <c r="AM27" s="9"/>
-    </row>
-    <row r="28" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF27" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="BG27" s="9"/>
+      <c r="BH27" s="9"/>
+      <c r="BI27" s="9"/>
+      <c r="BJ27" s="9"/>
+      <c r="BK27" s="9"/>
+      <c r="BL27" s="9"/>
+      <c r="BM27" s="9"/>
+      <c r="BN27" s="9"/>
+      <c r="BO27" s="9"/>
+      <c r="BP27" s="9"/>
+      <c r="BQ27" s="9"/>
+      <c r="BR27" s="9"/>
+      <c r="BS27" s="9"/>
+      <c r="BT27" s="9"/>
+      <c r="BU27" s="9"/>
+    </row>
+    <row r="28" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B28" s="9" t="s">
         <v>203</v>
       </c>
@@ -7479,8 +8422,26 @@
       <c r="AK28" s="9"/>
       <c r="AL28" s="9"/>
       <c r="AM28" s="9"/>
-    </row>
-    <row r="29" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF28" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="BG28" s="9"/>
+      <c r="BH28" s="9"/>
+      <c r="BI28" s="9"/>
+      <c r="BJ28" s="9"/>
+      <c r="BK28" s="9"/>
+      <c r="BL28" s="9"/>
+      <c r="BM28" s="9"/>
+      <c r="BN28" s="9"/>
+      <c r="BO28" s="9"/>
+      <c r="BP28" s="9"/>
+      <c r="BQ28" s="9"/>
+      <c r="BR28" s="9"/>
+      <c r="BS28" s="9"/>
+      <c r="BT28" s="9"/>
+      <c r="BU28" s="9"/>
+    </row>
+    <row r="29" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B29" s="9" t="s">
         <v>204</v>
       </c>
@@ -7509,8 +8470,24 @@
       <c r="AK29" s="9"/>
       <c r="AL29" s="9"/>
       <c r="AM29" s="9"/>
-    </row>
-    <row r="30" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF29" s="9"/>
+      <c r="BG29" s="9"/>
+      <c r="BH29" s="9"/>
+      <c r="BI29" s="9"/>
+      <c r="BJ29" s="9"/>
+      <c r="BK29" s="9"/>
+      <c r="BL29" s="9"/>
+      <c r="BM29" s="9"/>
+      <c r="BN29" s="9"/>
+      <c r="BO29" s="9"/>
+      <c r="BP29" s="9"/>
+      <c r="BQ29" s="9"/>
+      <c r="BR29" s="9"/>
+      <c r="BS29" s="9"/>
+      <c r="BT29" s="9"/>
+      <c r="BU29" s="9"/>
+    </row>
+    <row r="30" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B30" s="9" t="s">
         <v>205</v>
       </c>
@@ -7539,8 +8516,26 @@
       <c r="AK30" s="9"/>
       <c r="AL30" s="9"/>
       <c r="AM30" s="9"/>
-    </row>
-    <row r="31" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF30" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="BG30" s="9"/>
+      <c r="BH30" s="9"/>
+      <c r="BI30" s="9"/>
+      <c r="BJ30" s="9"/>
+      <c r="BK30" s="9"/>
+      <c r="BL30" s="9"/>
+      <c r="BM30" s="9"/>
+      <c r="BN30" s="9"/>
+      <c r="BO30" s="9"/>
+      <c r="BP30" s="9"/>
+      <c r="BQ30" s="9"/>
+      <c r="BR30" s="9"/>
+      <c r="BS30" s="9"/>
+      <c r="BT30" s="9"/>
+      <c r="BU30" s="9"/>
+    </row>
+    <row r="31" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B31" s="9" t="s">
         <v>206</v>
       </c>
@@ -7569,8 +8564,26 @@
       <c r="AK31" s="9"/>
       <c r="AL31" s="9"/>
       <c r="AM31" s="9"/>
-    </row>
-    <row r="32" spans="2:43" x14ac:dyDescent="0.4">
+      <c r="BF31" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="BG31" s="9"/>
+      <c r="BH31" s="9"/>
+      <c r="BI31" s="9"/>
+      <c r="BJ31" s="9"/>
+      <c r="BK31" s="9"/>
+      <c r="BL31" s="9"/>
+      <c r="BM31" s="9"/>
+      <c r="BN31" s="9"/>
+      <c r="BO31" s="9"/>
+      <c r="BP31" s="9"/>
+      <c r="BQ31" s="9"/>
+      <c r="BR31" s="9"/>
+      <c r="BS31" s="9"/>
+      <c r="BT31" s="9"/>
+      <c r="BU31" s="9"/>
+    </row>
+    <row r="32" spans="2:73" x14ac:dyDescent="0.4">
       <c r="B32" s="9" t="s">
         <v>48</v>
       </c>
@@ -7599,8 +8612,24 @@
       <c r="AK32" s="9"/>
       <c r="AL32" s="9"/>
       <c r="AM32" s="9"/>
-    </row>
-    <row r="33" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="BF32" s="9"/>
+      <c r="BG32" s="9"/>
+      <c r="BH32" s="9"/>
+      <c r="BI32" s="9"/>
+      <c r="BJ32" s="9"/>
+      <c r="BK32" s="9"/>
+      <c r="BL32" s="9"/>
+      <c r="BM32" s="9"/>
+      <c r="BN32" s="9"/>
+      <c r="BO32" s="9"/>
+      <c r="BP32" s="9"/>
+      <c r="BQ32" s="9"/>
+      <c r="BR32" s="9"/>
+      <c r="BS32" s="9"/>
+      <c r="BT32" s="9"/>
+      <c r="BU32" s="9"/>
+    </row>
+    <row r="33" spans="2:174" x14ac:dyDescent="0.4">
       <c r="B33" s="9" t="s">
         <v>207</v>
       </c>
@@ -7627,8 +8656,26 @@
       <c r="AK33" s="9"/>
       <c r="AL33" s="9"/>
       <c r="AM33" s="9"/>
-    </row>
-    <row r="34" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="BF33" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="BG33" s="9"/>
+      <c r="BH33" s="9"/>
+      <c r="BI33" s="9"/>
+      <c r="BJ33" s="9"/>
+      <c r="BK33" s="9"/>
+      <c r="BL33" s="9"/>
+      <c r="BM33" s="9"/>
+      <c r="BN33" s="9"/>
+      <c r="BO33" s="9"/>
+      <c r="BP33" s="9"/>
+      <c r="BQ33" s="9"/>
+      <c r="BR33" s="9"/>
+      <c r="BS33" s="9"/>
+      <c r="BT33" s="9"/>
+      <c r="BU33" s="9"/>
+    </row>
+    <row r="34" spans="2:174" x14ac:dyDescent="0.4">
       <c r="B34" s="9" t="s">
         <v>46</v>
       </c>
@@ -7655,8 +8702,26 @@
       <c r="AK34" s="9"/>
       <c r="AL34" s="9"/>
       <c r="AM34" s="9"/>
-    </row>
-    <row r="35" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="BF34" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="BG34" s="9"/>
+      <c r="BH34" s="9"/>
+      <c r="BI34" s="9"/>
+      <c r="BJ34" s="9"/>
+      <c r="BK34" s="9"/>
+      <c r="BL34" s="9"/>
+      <c r="BM34" s="9"/>
+      <c r="BN34" s="9"/>
+      <c r="BO34" s="9"/>
+      <c r="BP34" s="9"/>
+      <c r="BQ34" s="9"/>
+      <c r="BR34" s="9"/>
+      <c r="BS34" s="9"/>
+      <c r="BT34" s="9"/>
+      <c r="BU34" s="9"/>
+    </row>
+    <row r="35" spans="2:174" x14ac:dyDescent="0.4">
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
@@ -7683,8 +8748,26 @@
       <c r="AK35" s="9"/>
       <c r="AL35" s="9"/>
       <c r="AM35" s="9"/>
-    </row>
-    <row r="36" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="BF35" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="BG35" s="9"/>
+      <c r="BH35" s="9"/>
+      <c r="BI35" s="9"/>
+      <c r="BJ35" s="9"/>
+      <c r="BK35" s="9"/>
+      <c r="BL35" s="9"/>
+      <c r="BM35" s="9"/>
+      <c r="BN35" s="9"/>
+      <c r="BO35" s="9"/>
+      <c r="BP35" s="9"/>
+      <c r="BQ35" s="9"/>
+      <c r="BR35" s="9"/>
+      <c r="BS35" s="9"/>
+      <c r="BT35" s="9"/>
+      <c r="BU35" s="9"/>
+    </row>
+    <row r="36" spans="2:174" x14ac:dyDescent="0.4">
       <c r="B36" s="9" t="s">
         <v>208</v>
       </c>
@@ -7713,8 +8796,26 @@
       <c r="AK36" s="9"/>
       <c r="AL36" s="9"/>
       <c r="AM36" s="9"/>
-    </row>
-    <row r="37" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="BF36" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="BG36" s="9"/>
+      <c r="BH36" s="9"/>
+      <c r="BI36" s="9"/>
+      <c r="BJ36" s="9"/>
+      <c r="BK36" s="9"/>
+      <c r="BL36" s="9"/>
+      <c r="BM36" s="9"/>
+      <c r="BN36" s="9"/>
+      <c r="BO36" s="9"/>
+      <c r="BP36" s="9"/>
+      <c r="BQ36" s="9"/>
+      <c r="BR36" s="9"/>
+      <c r="BS36" s="9"/>
+      <c r="BT36" s="9"/>
+      <c r="BU36" s="9"/>
+    </row>
+    <row r="37" spans="2:174" x14ac:dyDescent="0.4">
       <c r="B37" s="9" t="s">
         <v>209</v>
       </c>
@@ -7743,8 +8844,26 @@
       <c r="AK37" s="9"/>
       <c r="AL37" s="9"/>
       <c r="AM37" s="9"/>
-    </row>
-    <row r="38" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="BF37" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="BG37" s="9"/>
+      <c r="BH37" s="9"/>
+      <c r="BI37" s="9"/>
+      <c r="BJ37" s="9"/>
+      <c r="BK37" s="9"/>
+      <c r="BL37" s="9"/>
+      <c r="BM37" s="9"/>
+      <c r="BN37" s="9"/>
+      <c r="BO37" s="9"/>
+      <c r="BP37" s="9"/>
+      <c r="BQ37" s="9"/>
+      <c r="BR37" s="9"/>
+      <c r="BS37" s="9"/>
+      <c r="BT37" s="9"/>
+      <c r="BU37" s="9"/>
+    </row>
+    <row r="38" spans="2:174" x14ac:dyDescent="0.4">
       <c r="B38" s="9" t="s">
         <v>210</v>
       </c>
@@ -7773,8 +8892,26 @@
       <c r="AK38" s="9"/>
       <c r="AL38" s="9"/>
       <c r="AM38" s="9"/>
-    </row>
-    <row r="39" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="BF38" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="BG38" s="9"/>
+      <c r="BH38" s="9"/>
+      <c r="BI38" s="9"/>
+      <c r="BJ38" s="9"/>
+      <c r="BK38" s="9"/>
+      <c r="BL38" s="9"/>
+      <c r="BM38" s="9"/>
+      <c r="BN38" s="9"/>
+      <c r="BO38" s="9"/>
+      <c r="BP38" s="9"/>
+      <c r="BQ38" s="9"/>
+      <c r="BR38" s="9"/>
+      <c r="BS38" s="9"/>
+      <c r="BT38" s="9"/>
+      <c r="BU38" s="9"/>
+    </row>
+    <row r="39" spans="2:174" x14ac:dyDescent="0.4">
       <c r="B39" s="9" t="s">
         <v>211</v>
       </c>
@@ -7804,7 +8941,7 @@
       <c r="AL39" s="9"/>
       <c r="AM39" s="9"/>
     </row>
-    <row r="40" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:174" x14ac:dyDescent="0.4">
       <c r="B40" s="9" t="s">
         <v>212</v>
       </c>
@@ -7834,7 +8971,7 @@
       <c r="AL40" s="9"/>
       <c r="AM40" s="9"/>
     </row>
-    <row r="41" spans="2:39" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:174" x14ac:dyDescent="0.4">
       <c r="B41" s="9" t="s">
         <v>46</v>
       </c>
@@ -7851,9 +8988,2529 @@
       <c r="M41" s="9"/>
       <c r="N41" s="9"/>
     </row>
+    <row r="43" spans="2:174" x14ac:dyDescent="0.4">
+      <c r="B43" s="59" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q43" s="62" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="44" spans="2:174" x14ac:dyDescent="0.4">
+      <c r="B44" s="59" t="s">
+        <v>272</v>
+      </c>
+      <c r="W44" s="59" t="s">
+        <v>300</v>
+      </c>
+      <c r="BH44" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="BR44" s="53"/>
+      <c r="BS44" s="53"/>
+      <c r="BT44" s="53"/>
+      <c r="BU44" s="53"/>
+      <c r="BV44" s="53"/>
+      <c r="CG44" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="CH44" s="53"/>
+      <c r="CI44" s="53"/>
+      <c r="CJ44" s="53"/>
+      <c r="CK44" s="53"/>
+      <c r="CL44" s="53"/>
+      <c r="CM44" s="53"/>
+      <c r="CN44" s="53"/>
+      <c r="CO44" s="53"/>
+      <c r="CP44" s="53"/>
+      <c r="CQ44" s="53"/>
+      <c r="CR44" s="53"/>
+      <c r="CS44" s="53"/>
+      <c r="CT44" s="53"/>
+      <c r="CU44" s="53"/>
+      <c r="DX44" s="59" t="s">
+        <v>303</v>
+      </c>
+      <c r="DY44" s="53"/>
+      <c r="DZ44" s="53"/>
+      <c r="EA44" s="53"/>
+      <c r="EB44" s="53"/>
+      <c r="EC44" s="53"/>
+      <c r="ED44" s="53"/>
+      <c r="EE44" s="53"/>
+      <c r="EF44" s="53"/>
+      <c r="EG44" s="53"/>
+      <c r="EH44" s="53"/>
+      <c r="EI44" s="53"/>
+      <c r="EJ44" s="53"/>
+      <c r="EK44" s="53"/>
+      <c r="EL44" s="53"/>
+      <c r="FA44" s="59" t="s">
+        <v>337</v>
+      </c>
+      <c r="FB44" s="53"/>
+      <c r="FC44" s="53"/>
+      <c r="FD44" s="53"/>
+      <c r="FE44" s="53"/>
+      <c r="FF44" s="53"/>
+      <c r="FG44" s="53"/>
+      <c r="FH44" s="53"/>
+      <c r="FI44" s="53"/>
+      <c r="FJ44" s="53"/>
+      <c r="FK44" s="53"/>
+      <c r="FL44" s="53"/>
+      <c r="FM44" s="53"/>
+      <c r="FN44" s="53"/>
+      <c r="FO44" s="53"/>
+    </row>
+    <row r="45" spans="2:174" x14ac:dyDescent="0.4">
+      <c r="B45" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
+      <c r="W45" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="X45" s="9"/>
+      <c r="Y45" s="9"/>
+      <c r="Z45" s="9"/>
+      <c r="AA45" s="9"/>
+      <c r="AB45" s="9"/>
+      <c r="AC45" s="9"/>
+      <c r="AD45" s="9"/>
+      <c r="AE45" s="9"/>
+      <c r="AF45" s="9"/>
+      <c r="AG45" s="9"/>
+      <c r="AH45" s="9"/>
+      <c r="AI45" s="9"/>
+      <c r="AJ45" s="9"/>
+      <c r="AK45" s="9"/>
+      <c r="BH45" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="BI45" s="9"/>
+      <c r="BJ45" s="9"/>
+      <c r="BK45" s="9"/>
+      <c r="BL45" s="9"/>
+      <c r="BM45" s="9"/>
+      <c r="BN45" s="9"/>
+      <c r="BO45" s="9"/>
+      <c r="BP45" s="9"/>
+      <c r="BQ45" s="9"/>
+      <c r="BR45" s="9"/>
+      <c r="BS45" s="9"/>
+      <c r="BT45" s="9"/>
+      <c r="BU45" s="9"/>
+      <c r="BV45" s="9"/>
+      <c r="CG45" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="CH45" s="9"/>
+      <c r="CI45" s="9"/>
+      <c r="CJ45" s="9"/>
+      <c r="CK45" s="9"/>
+      <c r="CL45" s="9"/>
+      <c r="CM45" s="9"/>
+      <c r="CN45" s="9"/>
+      <c r="CO45" s="9"/>
+      <c r="CP45" s="9"/>
+      <c r="CQ45" s="9"/>
+      <c r="CR45" s="9"/>
+      <c r="CS45" s="9"/>
+      <c r="CT45" s="9"/>
+      <c r="CU45" s="9"/>
+      <c r="DX45" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="DY45" s="9"/>
+      <c r="DZ45" s="9"/>
+      <c r="EA45" s="9"/>
+      <c r="EB45" s="9"/>
+      <c r="EC45" s="9"/>
+      <c r="ED45" s="9"/>
+      <c r="EE45" s="9"/>
+      <c r="EF45" s="9"/>
+      <c r="EG45" s="9"/>
+      <c r="EH45" s="9"/>
+      <c r="EI45" s="9"/>
+      <c r="EJ45" s="9"/>
+      <c r="EK45" s="9"/>
+      <c r="EL45" s="9"/>
+      <c r="FA45" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="FB45" s="9"/>
+      <c r="FC45" s="9"/>
+      <c r="FD45" s="9"/>
+      <c r="FE45" s="9"/>
+      <c r="FF45" s="9"/>
+      <c r="FG45" s="9"/>
+      <c r="FH45" s="9"/>
+      <c r="FI45" s="9"/>
+      <c r="FJ45" s="9"/>
+      <c r="FK45" s="9"/>
+      <c r="FL45" s="9"/>
+      <c r="FM45" s="9"/>
+      <c r="FN45" s="9"/>
+      <c r="FO45" s="9"/>
+      <c r="FP45" s="9"/>
+      <c r="FQ45" s="9"/>
+    </row>
+    <row r="46" spans="2:174" x14ac:dyDescent="0.4">
+      <c r="B46" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="W46" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="X46" s="9"/>
+      <c r="Y46" s="9"/>
+      <c r="Z46" s="9"/>
+      <c r="AA46" s="9"/>
+      <c r="AB46" s="9"/>
+      <c r="AC46" s="9"/>
+      <c r="AD46" s="9"/>
+      <c r="AE46" s="9"/>
+      <c r="AF46" s="9"/>
+      <c r="AG46" s="9"/>
+      <c r="AH46" s="9"/>
+      <c r="AI46" s="9"/>
+      <c r="AJ46" s="9"/>
+      <c r="AK46" s="9"/>
+      <c r="BH46" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="BI46" s="9"/>
+      <c r="BJ46" s="9"/>
+      <c r="BK46" s="9"/>
+      <c r="BL46" s="9"/>
+      <c r="BM46" s="9"/>
+      <c r="BN46" s="9"/>
+      <c r="BO46" s="9"/>
+      <c r="BP46" s="9"/>
+      <c r="BQ46" s="9"/>
+      <c r="BR46" s="9"/>
+      <c r="BS46" s="9"/>
+      <c r="BT46" s="9"/>
+      <c r="BU46" s="9"/>
+      <c r="BV46" s="9"/>
+      <c r="CG46" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="CH46" s="9"/>
+      <c r="CI46" s="9"/>
+      <c r="CJ46" s="9"/>
+      <c r="CK46" s="9"/>
+      <c r="CL46" s="9"/>
+      <c r="CM46" s="9"/>
+      <c r="CN46" s="9"/>
+      <c r="CO46" s="9"/>
+      <c r="CP46" s="9"/>
+      <c r="CQ46" s="9"/>
+      <c r="CR46" s="9"/>
+      <c r="CS46" s="9"/>
+      <c r="CT46" s="9"/>
+      <c r="CU46" s="9"/>
+      <c r="DX46" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="DY46" s="9"/>
+      <c r="DZ46" s="9"/>
+      <c r="EA46" s="9"/>
+      <c r="EB46" s="9"/>
+      <c r="EC46" s="9"/>
+      <c r="ED46" s="9"/>
+      <c r="EE46" s="9"/>
+      <c r="EF46" s="9"/>
+      <c r="EG46" s="9"/>
+      <c r="EH46" s="9"/>
+      <c r="EI46" s="9"/>
+      <c r="EJ46" s="9"/>
+      <c r="EK46" s="9"/>
+      <c r="EL46" s="9"/>
+      <c r="FA46" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="FB46" s="9"/>
+      <c r="FC46" s="9"/>
+      <c r="FD46" s="9"/>
+      <c r="FE46" s="9"/>
+      <c r="FF46" s="9"/>
+      <c r="FG46" s="9"/>
+      <c r="FH46" s="9"/>
+      <c r="FI46" s="9"/>
+      <c r="FJ46" s="9"/>
+      <c r="FK46" s="9"/>
+      <c r="FL46" s="9"/>
+      <c r="FM46" s="9"/>
+      <c r="FN46" s="9"/>
+      <c r="FO46" s="9"/>
+      <c r="FP46" s="9"/>
+      <c r="FQ46" s="9"/>
+    </row>
+    <row r="47" spans="2:174" x14ac:dyDescent="0.4">
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="W47" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="X47" s="9"/>
+      <c r="Y47" s="9"/>
+      <c r="Z47" s="9"/>
+      <c r="AA47" s="9"/>
+      <c r="AB47" s="9"/>
+      <c r="AC47" s="9"/>
+      <c r="AD47" s="9"/>
+      <c r="AE47" s="9"/>
+      <c r="AF47" s="9"/>
+      <c r="AG47" s="9"/>
+      <c r="AH47" s="9"/>
+      <c r="AI47" s="9"/>
+      <c r="AJ47" s="9"/>
+      <c r="AK47" s="9"/>
+      <c r="BH47" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="BI47" s="9"/>
+      <c r="BJ47" s="9"/>
+      <c r="BK47" s="9"/>
+      <c r="BL47" s="9"/>
+      <c r="BM47" s="9"/>
+      <c r="BN47" s="9"/>
+      <c r="BO47" s="9"/>
+      <c r="BP47" s="9"/>
+      <c r="BQ47" s="9"/>
+      <c r="BR47" s="9"/>
+      <c r="BS47" s="9"/>
+      <c r="BT47" s="9"/>
+      <c r="BU47" s="9"/>
+      <c r="BV47" s="9"/>
+      <c r="CG47" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="CH47" s="9"/>
+      <c r="CI47" s="9"/>
+      <c r="CJ47" s="9"/>
+      <c r="CK47" s="9"/>
+      <c r="CL47" s="9"/>
+      <c r="CM47" s="9"/>
+      <c r="CN47" s="9"/>
+      <c r="CO47" s="9"/>
+      <c r="CP47" s="9"/>
+      <c r="CQ47" s="9"/>
+      <c r="CR47" s="9"/>
+      <c r="CS47" s="9"/>
+      <c r="CT47" s="9"/>
+      <c r="CU47" s="9"/>
+      <c r="DX47" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="DY47" s="9"/>
+      <c r="DZ47" s="9"/>
+      <c r="EA47" s="9"/>
+      <c r="EB47" s="9"/>
+      <c r="EC47" s="9"/>
+      <c r="ED47" s="9"/>
+      <c r="EE47" s="9"/>
+      <c r="EF47" s="9"/>
+      <c r="EG47" s="9"/>
+      <c r="EH47" s="9"/>
+      <c r="EI47" s="9"/>
+      <c r="EJ47" s="9"/>
+      <c r="EK47" s="9"/>
+      <c r="EL47" s="9"/>
+      <c r="EM47" s="53" t="s">
+        <v>322</v>
+      </c>
+      <c r="EN47" s="53"/>
+      <c r="FA47" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="FB47" s="9"/>
+      <c r="FC47" s="9"/>
+      <c r="FD47" s="9"/>
+      <c r="FE47" s="9"/>
+      <c r="FF47" s="9"/>
+      <c r="FG47" s="9"/>
+      <c r="FH47" s="9"/>
+      <c r="FI47" s="9"/>
+      <c r="FJ47" s="9"/>
+      <c r="FK47" s="9"/>
+      <c r="FL47" s="9"/>
+      <c r="FM47" s="9"/>
+      <c r="FN47" s="9"/>
+      <c r="FO47" s="9"/>
+      <c r="FP47" s="9"/>
+      <c r="FQ47" s="9"/>
+      <c r="FR47" s="53" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="48" spans="2:174" x14ac:dyDescent="0.4">
+      <c r="B48" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="W48" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="X48" s="9"/>
+      <c r="Y48" s="9"/>
+      <c r="Z48" s="9"/>
+      <c r="AA48" s="9"/>
+      <c r="AB48" s="9"/>
+      <c r="AC48" s="9"/>
+      <c r="AD48" s="9"/>
+      <c r="AE48" s="9"/>
+      <c r="AF48" s="9"/>
+      <c r="AG48" s="9"/>
+      <c r="AH48" s="9"/>
+      <c r="AI48" s="9"/>
+      <c r="AJ48" s="9"/>
+      <c r="AK48" s="9"/>
+      <c r="AM48" s="53" t="s">
+        <v>302</v>
+      </c>
+      <c r="BH48" s="9"/>
+      <c r="BI48" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="BJ48" s="9"/>
+      <c r="BK48" s="9"/>
+      <c r="BL48" s="9"/>
+      <c r="BM48" s="9"/>
+      <c r="BN48" s="9"/>
+      <c r="BO48" s="9"/>
+      <c r="BP48" s="9"/>
+      <c r="BQ48" s="9"/>
+      <c r="BR48" s="9"/>
+      <c r="BS48" s="9"/>
+      <c r="BT48" s="9"/>
+      <c r="BU48" s="9"/>
+      <c r="BV48" s="9"/>
+      <c r="BW48" s="53" t="s">
+        <v>304</v>
+      </c>
+      <c r="BX48" s="53"/>
+      <c r="CG48" s="9"/>
+      <c r="CH48" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="CI48" s="9"/>
+      <c r="CJ48" s="9"/>
+      <c r="CK48" s="9"/>
+      <c r="CL48" s="9"/>
+      <c r="CM48" s="9"/>
+      <c r="CN48" s="9"/>
+      <c r="CO48" s="9"/>
+      <c r="CP48" s="9"/>
+      <c r="CQ48" s="9"/>
+      <c r="CR48" s="9"/>
+      <c r="CS48" s="9"/>
+      <c r="CT48" s="9"/>
+      <c r="CU48" s="9"/>
+      <c r="DX48" s="9"/>
+      <c r="DY48" s="63" t="s">
+        <v>318</v>
+      </c>
+      <c r="DZ48" s="9"/>
+      <c r="EA48" s="9"/>
+      <c r="EB48" s="9"/>
+      <c r="EC48" s="9"/>
+      <c r="ED48" s="9"/>
+      <c r="EE48" s="9"/>
+      <c r="EF48" s="9"/>
+      <c r="EG48" s="9"/>
+      <c r="EH48" s="9"/>
+      <c r="EI48" s="9"/>
+      <c r="EJ48" s="9"/>
+      <c r="EK48" s="9"/>
+      <c r="EL48" s="9"/>
+      <c r="EM48" s="53"/>
+      <c r="EN48" s="53" t="s">
+        <v>323</v>
+      </c>
+      <c r="FA48" s="9"/>
+      <c r="FB48" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="FC48" s="9"/>
+      <c r="FD48" s="9"/>
+      <c r="FE48" s="9"/>
+      <c r="FF48" s="9"/>
+      <c r="FG48" s="9"/>
+      <c r="FH48" s="9"/>
+      <c r="FI48" s="9"/>
+      <c r="FJ48" s="9"/>
+      <c r="FK48" s="9"/>
+      <c r="FL48" s="9"/>
+      <c r="FM48" s="9"/>
+      <c r="FN48" s="9"/>
+      <c r="FO48" s="9"/>
+      <c r="FP48" s="9"/>
+      <c r="FQ48" s="9"/>
+    </row>
+    <row r="49" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B49" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="9"/>
+      <c r="W49" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="X49" s="9"/>
+      <c r="Y49" s="9"/>
+      <c r="Z49" s="9"/>
+      <c r="AA49" s="9"/>
+      <c r="AB49" s="9"/>
+      <c r="AC49" s="9"/>
+      <c r="AD49" s="9"/>
+      <c r="AE49" s="9"/>
+      <c r="AF49" s="9"/>
+      <c r="AG49" s="9"/>
+      <c r="AH49" s="9"/>
+      <c r="AI49" s="9"/>
+      <c r="AJ49" s="9"/>
+      <c r="AK49" s="9"/>
+      <c r="AM49" s="53" t="s">
+        <v>301</v>
+      </c>
+      <c r="BH49" s="9"/>
+      <c r="BI49" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="BJ49" s="9"/>
+      <c r="BK49" s="9"/>
+      <c r="BL49" s="9"/>
+      <c r="BM49" s="9"/>
+      <c r="BN49" s="9"/>
+      <c r="BO49" s="9"/>
+      <c r="BP49" s="9"/>
+      <c r="BQ49" s="9"/>
+      <c r="BR49" s="9"/>
+      <c r="BS49" s="9"/>
+      <c r="BT49" s="9"/>
+      <c r="BU49" s="9"/>
+      <c r="BV49" s="9"/>
+      <c r="BW49" s="53"/>
+      <c r="BX49" s="53" t="s">
+        <v>305</v>
+      </c>
+      <c r="CG49" s="9"/>
+      <c r="CH49" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="CI49" s="9"/>
+      <c r="CJ49" s="9"/>
+      <c r="CK49" s="9"/>
+      <c r="CL49" s="9"/>
+      <c r="CM49" s="9"/>
+      <c r="CN49" s="9"/>
+      <c r="CO49" s="9"/>
+      <c r="CP49" s="9"/>
+      <c r="CQ49" s="9"/>
+      <c r="CR49" s="9"/>
+      <c r="CS49" s="9"/>
+      <c r="CT49" s="9"/>
+      <c r="CU49" s="9"/>
+      <c r="DX49" s="9"/>
+      <c r="DY49" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="DZ49" s="9"/>
+      <c r="EA49" s="9"/>
+      <c r="EB49" s="9"/>
+      <c r="EC49" s="9"/>
+      <c r="ED49" s="9"/>
+      <c r="EE49" s="9"/>
+      <c r="EF49" s="9"/>
+      <c r="EG49" s="9"/>
+      <c r="EH49" s="9"/>
+      <c r="EI49" s="9"/>
+      <c r="EJ49" s="9"/>
+      <c r="EK49" s="9"/>
+      <c r="EL49" s="9"/>
+      <c r="EM49" s="53"/>
+      <c r="EN49" s="53" t="s">
+        <v>324</v>
+      </c>
+      <c r="FA49" s="9"/>
+      <c r="FB49" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="FC49" s="9"/>
+      <c r="FD49" s="9"/>
+      <c r="FE49" s="9"/>
+      <c r="FF49" s="9"/>
+      <c r="FG49" s="9"/>
+      <c r="FH49" s="9"/>
+      <c r="FI49" s="9"/>
+      <c r="FJ49" s="9"/>
+      <c r="FK49" s="9"/>
+      <c r="FL49" s="9"/>
+      <c r="FM49" s="9"/>
+      <c r="FN49" s="9"/>
+      <c r="FO49" s="9"/>
+      <c r="FP49" s="9"/>
+      <c r="FQ49" s="9"/>
+      <c r="FR49" s="53" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="50" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B50" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="53" t="s">
+        <v>290</v>
+      </c>
+      <c r="W50" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="X50" s="9"/>
+      <c r="Y50" s="9"/>
+      <c r="Z50" s="9"/>
+      <c r="AA50" s="9"/>
+      <c r="AB50" s="9"/>
+      <c r="AC50" s="9"/>
+      <c r="AD50" s="9"/>
+      <c r="AE50" s="9"/>
+      <c r="AF50" s="9"/>
+      <c r="AG50" s="9"/>
+      <c r="AH50" s="9"/>
+      <c r="AI50" s="9"/>
+      <c r="AJ50" s="9"/>
+      <c r="AK50" s="9"/>
+      <c r="BH50" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="BI50" s="9"/>
+      <c r="BJ50" s="9"/>
+      <c r="BK50" s="9"/>
+      <c r="BL50" s="9"/>
+      <c r="BM50" s="9"/>
+      <c r="BN50" s="9"/>
+      <c r="BO50" s="9"/>
+      <c r="BP50" s="9"/>
+      <c r="BQ50" s="9"/>
+      <c r="BR50" s="9"/>
+      <c r="BS50" s="9"/>
+      <c r="BT50" s="9"/>
+      <c r="BU50" s="9"/>
+      <c r="BV50" s="9"/>
+      <c r="BW50" s="53"/>
+      <c r="BX50" s="53"/>
+      <c r="CG50" s="9"/>
+      <c r="CH50" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="CI50" s="9"/>
+      <c r="CJ50" s="9"/>
+      <c r="CK50" s="9"/>
+      <c r="CL50" s="9"/>
+      <c r="CM50" s="9"/>
+      <c r="CN50" s="9"/>
+      <c r="CO50" s="9"/>
+      <c r="CP50" s="9"/>
+      <c r="CQ50" s="9"/>
+      <c r="CR50" s="9"/>
+      <c r="CS50" s="9"/>
+      <c r="CT50" s="9"/>
+      <c r="CU50" s="9"/>
+      <c r="CV50" s="53" t="s">
+        <v>316</v>
+      </c>
+      <c r="DX50" s="9"/>
+      <c r="DY50" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="DZ50" s="9"/>
+      <c r="EA50" s="9"/>
+      <c r="EB50" s="9"/>
+      <c r="EC50" s="9"/>
+      <c r="ED50" s="9"/>
+      <c r="EE50" s="9"/>
+      <c r="EF50" s="9"/>
+      <c r="EG50" s="9"/>
+      <c r="EH50" s="9"/>
+      <c r="EI50" s="9"/>
+      <c r="EJ50" s="9"/>
+      <c r="EK50" s="9"/>
+      <c r="EL50" s="9"/>
+      <c r="EM50" s="53"/>
+      <c r="EN50" s="53" t="s">
+        <v>325</v>
+      </c>
+      <c r="FA50" s="9"/>
+      <c r="FB50" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="FC50" s="9"/>
+      <c r="FD50" s="9"/>
+      <c r="FE50" s="9"/>
+      <c r="FF50" s="9"/>
+      <c r="FG50" s="9"/>
+      <c r="FH50" s="9"/>
+      <c r="FI50" s="9"/>
+      <c r="FJ50" s="9"/>
+      <c r="FK50" s="9"/>
+      <c r="FL50" s="9"/>
+      <c r="FM50" s="9"/>
+      <c r="FN50" s="9"/>
+      <c r="FO50" s="9"/>
+      <c r="FP50" s="9"/>
+      <c r="FQ50" s="9"/>
+      <c r="FS50" s="53" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="51" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B51" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+      <c r="P51" s="53" t="s">
+        <v>291</v>
+      </c>
+      <c r="W51" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="X51" s="9"/>
+      <c r="Y51" s="9"/>
+      <c r="Z51" s="9"/>
+      <c r="AA51" s="9"/>
+      <c r="AB51" s="9"/>
+      <c r="AC51" s="9"/>
+      <c r="AD51" s="9"/>
+      <c r="AE51" s="9"/>
+      <c r="AF51" s="9"/>
+      <c r="AG51" s="9"/>
+      <c r="AH51" s="9"/>
+      <c r="AI51" s="9"/>
+      <c r="AJ51" s="9"/>
+      <c r="AK51" s="9"/>
+      <c r="BH51" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="BI51" s="9"/>
+      <c r="BJ51" s="9"/>
+      <c r="BK51" s="9"/>
+      <c r="BL51" s="9"/>
+      <c r="BM51" s="9"/>
+      <c r="BN51" s="9"/>
+      <c r="BO51" s="9"/>
+      <c r="BP51" s="9"/>
+      <c r="BQ51" s="9"/>
+      <c r="BR51" s="9"/>
+      <c r="BS51" s="9"/>
+      <c r="BT51" s="9"/>
+      <c r="BU51" s="9"/>
+      <c r="BV51" s="9"/>
+      <c r="BW51" s="53"/>
+      <c r="BX51" s="53"/>
+      <c r="CG51" s="9"/>
+      <c r="CH51" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="CI51" s="9"/>
+      <c r="CJ51" s="9"/>
+      <c r="CK51" s="9"/>
+      <c r="CL51" s="9"/>
+      <c r="CM51" s="9"/>
+      <c r="CN51" s="9"/>
+      <c r="CO51" s="9"/>
+      <c r="CP51" s="9"/>
+      <c r="CQ51" s="9"/>
+      <c r="CR51" s="9"/>
+      <c r="CS51" s="9"/>
+      <c r="CT51" s="9"/>
+      <c r="CU51" s="9"/>
+      <c r="CV51" s="53" t="s">
+        <v>317</v>
+      </c>
+      <c r="DX51" s="9"/>
+      <c r="DY51" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="DZ51" s="9"/>
+      <c r="EA51" s="9"/>
+      <c r="EB51" s="9"/>
+      <c r="EC51" s="9"/>
+      <c r="ED51" s="9"/>
+      <c r="EE51" s="9"/>
+      <c r="EF51" s="9"/>
+      <c r="EG51" s="9"/>
+      <c r="EH51" s="9"/>
+      <c r="EI51" s="9"/>
+      <c r="EJ51" s="9"/>
+      <c r="EK51" s="9"/>
+      <c r="EL51" s="9"/>
+      <c r="EM51" s="53"/>
+      <c r="EN51" s="53" t="s">
+        <v>326</v>
+      </c>
+      <c r="FA51" s="9"/>
+      <c r="FB51" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="FC51" s="9"/>
+      <c r="FD51" s="9"/>
+      <c r="FE51" s="9"/>
+      <c r="FF51" s="9"/>
+      <c r="FG51" s="9"/>
+      <c r="FH51" s="9"/>
+      <c r="FI51" s="9"/>
+      <c r="FJ51" s="9"/>
+      <c r="FK51" s="9"/>
+      <c r="FL51" s="9"/>
+      <c r="FM51" s="9"/>
+      <c r="FN51" s="9"/>
+      <c r="FO51" s="9"/>
+      <c r="FP51" s="9"/>
+      <c r="FQ51" s="9"/>
+      <c r="FS51" s="53" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="52" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B52" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9"/>
+      <c r="W52" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="X52" s="9"/>
+      <c r="Y52" s="9"/>
+      <c r="Z52" s="9"/>
+      <c r="AA52" s="9"/>
+      <c r="AB52" s="9"/>
+      <c r="AC52" s="9"/>
+      <c r="AD52" s="9"/>
+      <c r="AE52" s="9"/>
+      <c r="AF52" s="9"/>
+      <c r="AG52" s="9"/>
+      <c r="AH52" s="9"/>
+      <c r="AI52" s="9"/>
+      <c r="AJ52" s="9"/>
+      <c r="AK52" s="9"/>
+      <c r="BH52" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="BI52" s="9"/>
+      <c r="BJ52" s="9"/>
+      <c r="BK52" s="9"/>
+      <c r="BL52" s="9"/>
+      <c r="BM52" s="9"/>
+      <c r="BN52" s="9"/>
+      <c r="BO52" s="9"/>
+      <c r="BP52" s="9"/>
+      <c r="BQ52" s="9"/>
+      <c r="BR52" s="9"/>
+      <c r="BS52" s="9"/>
+      <c r="BT52" s="9"/>
+      <c r="BU52" s="9"/>
+      <c r="BV52" s="9"/>
+      <c r="BW52" s="53"/>
+      <c r="BX52" s="53"/>
+      <c r="CG52" s="9"/>
+      <c r="CH52" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="CI52" s="9"/>
+      <c r="CJ52" s="9"/>
+      <c r="CK52" s="9"/>
+      <c r="CL52" s="9"/>
+      <c r="CM52" s="9"/>
+      <c r="CN52" s="9"/>
+      <c r="CO52" s="9"/>
+      <c r="CP52" s="9"/>
+      <c r="CQ52" s="9"/>
+      <c r="CR52" s="9"/>
+      <c r="CS52" s="9"/>
+      <c r="CT52" s="9"/>
+      <c r="CU52" s="9"/>
+      <c r="DX52" s="9"/>
+      <c r="DY52" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="DZ52" s="9"/>
+      <c r="EA52" s="9"/>
+      <c r="EB52" s="9"/>
+      <c r="EC52" s="9"/>
+      <c r="ED52" s="9"/>
+      <c r="EE52" s="9"/>
+      <c r="EF52" s="9"/>
+      <c r="EG52" s="9"/>
+      <c r="EH52" s="9"/>
+      <c r="EI52" s="9"/>
+      <c r="EJ52" s="9"/>
+      <c r="EK52" s="9"/>
+      <c r="EL52" s="9"/>
+      <c r="EM52" s="53"/>
+      <c r="EN52" s="53" t="s">
+        <v>327</v>
+      </c>
+      <c r="FA52" s="9"/>
+      <c r="FB52" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="FC52" s="9"/>
+      <c r="FD52" s="9"/>
+      <c r="FE52" s="9"/>
+      <c r="FF52" s="9"/>
+      <c r="FG52" s="9"/>
+      <c r="FH52" s="9"/>
+      <c r="FI52" s="9"/>
+      <c r="FJ52" s="9"/>
+      <c r="FK52" s="9"/>
+      <c r="FL52" s="9"/>
+      <c r="FM52" s="9"/>
+      <c r="FN52" s="9"/>
+      <c r="FO52" s="9"/>
+      <c r="FP52" s="9"/>
+      <c r="FQ52" s="9"/>
+    </row>
+    <row r="53" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B53" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+      <c r="W53" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="X53" s="9"/>
+      <c r="Y53" s="9"/>
+      <c r="Z53" s="9"/>
+      <c r="AA53" s="9"/>
+      <c r="AB53" s="9"/>
+      <c r="AC53" s="9"/>
+      <c r="AD53" s="9"/>
+      <c r="AE53" s="9"/>
+      <c r="AF53" s="9"/>
+      <c r="AG53" s="9"/>
+      <c r="AH53" s="9"/>
+      <c r="AI53" s="9"/>
+      <c r="AJ53" s="9"/>
+      <c r="AK53" s="9"/>
+      <c r="BH53" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="BI53" s="9"/>
+      <c r="BJ53" s="9"/>
+      <c r="BK53" s="9"/>
+      <c r="BL53" s="9"/>
+      <c r="BM53" s="9"/>
+      <c r="BN53" s="9"/>
+      <c r="BO53" s="9"/>
+      <c r="BP53" s="9"/>
+      <c r="BQ53" s="9"/>
+      <c r="BR53" s="9"/>
+      <c r="BS53" s="9"/>
+      <c r="BT53" s="9"/>
+      <c r="BU53" s="9"/>
+      <c r="BV53" s="9"/>
+      <c r="BW53" s="53"/>
+      <c r="BX53" s="53"/>
+      <c r="CG53" s="9"/>
+      <c r="CH53" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="CI53" s="9"/>
+      <c r="CJ53" s="9"/>
+      <c r="CK53" s="9"/>
+      <c r="CL53" s="9"/>
+      <c r="CM53" s="9"/>
+      <c r="CN53" s="9"/>
+      <c r="CO53" s="9"/>
+      <c r="CP53" s="9"/>
+      <c r="CQ53" s="9"/>
+      <c r="CR53" s="9"/>
+      <c r="CS53" s="9"/>
+      <c r="CT53" s="9"/>
+      <c r="CU53" s="9"/>
+      <c r="DX53" s="9"/>
+      <c r="DY53" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="DZ53" s="9"/>
+      <c r="EA53" s="9"/>
+      <c r="EB53" s="9"/>
+      <c r="EC53" s="9"/>
+      <c r="ED53" s="9"/>
+      <c r="EE53" s="9"/>
+      <c r="EF53" s="9"/>
+      <c r="EG53" s="9"/>
+      <c r="EH53" s="9"/>
+      <c r="EI53" s="9"/>
+      <c r="EJ53" s="9"/>
+      <c r="EK53" s="9"/>
+      <c r="EL53" s="9"/>
+      <c r="FA53" s="9"/>
+      <c r="FB53" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="FC53" s="9"/>
+      <c r="FD53" s="9"/>
+      <c r="FE53" s="9"/>
+      <c r="FF53" s="9"/>
+      <c r="FG53" s="9"/>
+      <c r="FH53" s="9"/>
+      <c r="FI53" s="9"/>
+      <c r="FJ53" s="9"/>
+      <c r="FK53" s="9"/>
+      <c r="FL53" s="9"/>
+      <c r="FM53" s="9"/>
+      <c r="FN53" s="9"/>
+      <c r="FO53" s="9"/>
+      <c r="FP53" s="9"/>
+      <c r="FQ53" s="9"/>
+    </row>
+    <row r="54" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B54" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
+      <c r="W54" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="X54" s="9"/>
+      <c r="Y54" s="9"/>
+      <c r="Z54" s="9"/>
+      <c r="AA54" s="9"/>
+      <c r="AB54" s="9"/>
+      <c r="AC54" s="9"/>
+      <c r="AD54" s="9"/>
+      <c r="AE54" s="9"/>
+      <c r="AF54" s="9"/>
+      <c r="AG54" s="9"/>
+      <c r="AH54" s="9"/>
+      <c r="AI54" s="9"/>
+      <c r="AJ54" s="9"/>
+      <c r="AK54" s="9"/>
+      <c r="BH54" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="BI54" s="9"/>
+      <c r="BJ54" s="9"/>
+      <c r="BK54" s="9"/>
+      <c r="BL54" s="9"/>
+      <c r="BM54" s="9"/>
+      <c r="BN54" s="9"/>
+      <c r="BO54" s="9"/>
+      <c r="BP54" s="9"/>
+      <c r="BQ54" s="9"/>
+      <c r="BR54" s="9"/>
+      <c r="BS54" s="9"/>
+      <c r="BT54" s="9"/>
+      <c r="BU54" s="9"/>
+      <c r="BV54" s="9"/>
+      <c r="BW54" s="53"/>
+      <c r="BX54" s="53"/>
+      <c r="CG54" s="9"/>
+      <c r="CH54" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="CI54" s="9"/>
+      <c r="CJ54" s="9"/>
+      <c r="CK54" s="9"/>
+      <c r="CL54" s="9"/>
+      <c r="CM54" s="9"/>
+      <c r="CN54" s="9"/>
+      <c r="CO54" s="9"/>
+      <c r="CP54" s="9"/>
+      <c r="CQ54" s="9"/>
+      <c r="CR54" s="9"/>
+      <c r="CS54" s="9"/>
+      <c r="CT54" s="9"/>
+      <c r="CU54" s="9"/>
+      <c r="DX54" s="9"/>
+      <c r="DY54" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="DZ54" s="9"/>
+      <c r="EA54" s="9"/>
+      <c r="EB54" s="9"/>
+      <c r="EC54" s="9"/>
+      <c r="ED54" s="9"/>
+      <c r="EE54" s="9"/>
+      <c r="EF54" s="9"/>
+      <c r="EG54" s="9"/>
+      <c r="EH54" s="9"/>
+      <c r="EI54" s="9"/>
+      <c r="EJ54" s="9"/>
+      <c r="EK54" s="9"/>
+      <c r="EL54" s="9"/>
+      <c r="FA54" s="9"/>
+      <c r="FB54" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="FC54" s="9"/>
+      <c r="FD54" s="9"/>
+      <c r="FE54" s="9"/>
+      <c r="FF54" s="9"/>
+      <c r="FG54" s="9"/>
+      <c r="FH54" s="9"/>
+      <c r="FI54" s="9"/>
+      <c r="FJ54" s="9"/>
+      <c r="FK54" s="9"/>
+      <c r="FL54" s="9"/>
+      <c r="FM54" s="9"/>
+      <c r="FN54" s="9"/>
+      <c r="FO54" s="9"/>
+      <c r="FP54" s="9"/>
+      <c r="FQ54" s="9"/>
+    </row>
+    <row r="55" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B55" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+      <c r="W55" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="X55" s="9"/>
+      <c r="Y55" s="9"/>
+      <c r="Z55" s="9"/>
+      <c r="AA55" s="9"/>
+      <c r="AB55" s="9"/>
+      <c r="AC55" s="9"/>
+      <c r="AD55" s="9"/>
+      <c r="AE55" s="9"/>
+      <c r="AF55" s="9"/>
+      <c r="AG55" s="9"/>
+      <c r="AH55" s="9"/>
+      <c r="AI55" s="9"/>
+      <c r="AJ55" s="9"/>
+      <c r="AK55" s="9"/>
+      <c r="BH55" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="BI55" s="9"/>
+      <c r="BJ55" s="9"/>
+      <c r="BK55" s="9"/>
+      <c r="BL55" s="9"/>
+      <c r="BM55" s="9"/>
+      <c r="BN55" s="9"/>
+      <c r="BO55" s="9"/>
+      <c r="BP55" s="9"/>
+      <c r="BQ55" s="9"/>
+      <c r="BR55" s="9"/>
+      <c r="BS55" s="9"/>
+      <c r="BT55" s="9"/>
+      <c r="BU55" s="9"/>
+      <c r="BV55" s="9"/>
+      <c r="BW55" s="53"/>
+      <c r="BX55" s="53"/>
+      <c r="CG55" s="9"/>
+      <c r="CH55" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="CI55" s="9"/>
+      <c r="CJ55" s="9"/>
+      <c r="CK55" s="9"/>
+      <c r="CL55" s="9"/>
+      <c r="CM55" s="9"/>
+      <c r="CN55" s="9"/>
+      <c r="CO55" s="9"/>
+      <c r="CP55" s="9"/>
+      <c r="CQ55" s="9"/>
+      <c r="CR55" s="9"/>
+      <c r="CS55" s="9"/>
+      <c r="CT55" s="9"/>
+      <c r="CU55" s="9"/>
+      <c r="DX55" s="9"/>
+      <c r="DY55" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="DZ55" s="9"/>
+      <c r="EA55" s="9"/>
+      <c r="EB55" s="9"/>
+      <c r="EC55" s="9"/>
+      <c r="ED55" s="9"/>
+      <c r="EE55" s="9"/>
+      <c r="EF55" s="9"/>
+      <c r="EG55" s="9"/>
+      <c r="EH55" s="9"/>
+      <c r="EI55" s="9"/>
+      <c r="EJ55" s="9"/>
+      <c r="EK55" s="9"/>
+      <c r="EL55" s="9"/>
+      <c r="FA55" s="9"/>
+      <c r="FB55" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="FC55" s="9"/>
+      <c r="FD55" s="9"/>
+      <c r="FE55" s="9"/>
+      <c r="FF55" s="9"/>
+      <c r="FG55" s="9"/>
+      <c r="FH55" s="9"/>
+      <c r="FI55" s="9"/>
+      <c r="FJ55" s="9"/>
+      <c r="FK55" s="9"/>
+      <c r="FL55" s="9"/>
+      <c r="FM55" s="9"/>
+      <c r="FN55" s="9"/>
+      <c r="FO55" s="9"/>
+      <c r="FP55" s="9"/>
+      <c r="FQ55" s="9"/>
+    </row>
+    <row r="56" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B56" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
+      <c r="BH56" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="BI56" s="9"/>
+      <c r="BJ56" s="9"/>
+      <c r="BK56" s="9"/>
+      <c r="BL56" s="9"/>
+      <c r="BM56" s="9"/>
+      <c r="BN56" s="9"/>
+      <c r="BO56" s="9"/>
+      <c r="BP56" s="9"/>
+      <c r="BQ56" s="9"/>
+      <c r="BR56" s="9"/>
+      <c r="BS56" s="9"/>
+      <c r="BT56" s="9"/>
+      <c r="BU56" s="9"/>
+      <c r="BV56" s="9"/>
+      <c r="BW56" s="53"/>
+      <c r="BX56" s="53"/>
+      <c r="CG56" s="9"/>
+      <c r="CH56" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="CI56" s="9"/>
+      <c r="CJ56" s="9"/>
+      <c r="CK56" s="9"/>
+      <c r="CL56" s="9"/>
+      <c r="CM56" s="9"/>
+      <c r="CN56" s="9"/>
+      <c r="CO56" s="9"/>
+      <c r="CP56" s="9"/>
+      <c r="CQ56" s="9"/>
+      <c r="CR56" s="9"/>
+      <c r="CS56" s="9"/>
+      <c r="CT56" s="9"/>
+      <c r="CU56" s="9"/>
+      <c r="DX56" s="9"/>
+      <c r="DY56" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="DZ56" s="9"/>
+      <c r="EA56" s="9"/>
+      <c r="EB56" s="9"/>
+      <c r="EC56" s="9"/>
+      <c r="ED56" s="9"/>
+      <c r="EE56" s="9"/>
+      <c r="EF56" s="9"/>
+      <c r="EG56" s="9"/>
+      <c r="EH56" s="9"/>
+      <c r="EI56" s="9"/>
+      <c r="EJ56" s="9"/>
+      <c r="EK56" s="9"/>
+      <c r="EL56" s="9"/>
+      <c r="FA56" s="9"/>
+      <c r="FB56" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="FC56" s="9"/>
+      <c r="FD56" s="9"/>
+      <c r="FE56" s="9"/>
+      <c r="FF56" s="9"/>
+      <c r="FG56" s="9"/>
+      <c r="FH56" s="9"/>
+      <c r="FI56" s="9"/>
+      <c r="FJ56" s="9"/>
+      <c r="FK56" s="9"/>
+      <c r="FL56" s="9"/>
+      <c r="FM56" s="9"/>
+      <c r="FN56" s="9"/>
+      <c r="FO56" s="9"/>
+      <c r="FP56" s="9"/>
+      <c r="FQ56" s="9"/>
+    </row>
+    <row r="57" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B57" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
+      <c r="BH57" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="BI57" s="9"/>
+      <c r="BJ57" s="9"/>
+      <c r="BK57" s="9"/>
+      <c r="BL57" s="9"/>
+      <c r="BM57" s="9"/>
+      <c r="BN57" s="9"/>
+      <c r="BO57" s="9"/>
+      <c r="BP57" s="9"/>
+      <c r="BQ57" s="9"/>
+      <c r="BR57" s="9"/>
+      <c r="BS57" s="9"/>
+      <c r="BT57" s="9"/>
+      <c r="BU57" s="9"/>
+      <c r="BV57" s="9"/>
+      <c r="BW57" s="53"/>
+      <c r="BX57" s="53"/>
+      <c r="CG57" s="9"/>
+      <c r="CH57" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="CI57" s="9"/>
+      <c r="CJ57" s="9"/>
+      <c r="CK57" s="9"/>
+      <c r="CL57" s="9"/>
+      <c r="CM57" s="9"/>
+      <c r="CN57" s="9"/>
+      <c r="CO57" s="9"/>
+      <c r="CP57" s="9"/>
+      <c r="CQ57" s="9"/>
+      <c r="CR57" s="9"/>
+      <c r="CS57" s="9"/>
+      <c r="CT57" s="9"/>
+      <c r="CU57" s="9"/>
+      <c r="DX57" s="9"/>
+      <c r="DY57" s="63" t="s">
+        <v>319</v>
+      </c>
+      <c r="DZ57" s="9"/>
+      <c r="EA57" s="9"/>
+      <c r="EB57" s="9"/>
+      <c r="EC57" s="9"/>
+      <c r="ED57" s="9"/>
+      <c r="EE57" s="9"/>
+      <c r="EF57" s="9"/>
+      <c r="EG57" s="9"/>
+      <c r="EH57" s="9"/>
+      <c r="EI57" s="9"/>
+      <c r="EJ57" s="9"/>
+      <c r="EK57" s="9"/>
+      <c r="EL57" s="9"/>
+      <c r="FA57" s="9"/>
+      <c r="FB57" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="FC57" s="9"/>
+      <c r="FD57" s="9"/>
+      <c r="FE57" s="9"/>
+      <c r="FF57" s="9"/>
+      <c r="FG57" s="9"/>
+      <c r="FH57" s="9"/>
+      <c r="FI57" s="9"/>
+      <c r="FJ57" s="9"/>
+      <c r="FK57" s="9"/>
+      <c r="FL57" s="9"/>
+      <c r="FM57" s="9"/>
+      <c r="FN57" s="9"/>
+      <c r="FO57" s="9"/>
+      <c r="FP57" s="9"/>
+      <c r="FQ57" s="9"/>
+    </row>
+    <row r="58" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B58" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
+      <c r="CG58" s="9"/>
+      <c r="CH58" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="CI58" s="9"/>
+      <c r="CJ58" s="9"/>
+      <c r="CK58" s="9"/>
+      <c r="CL58" s="9"/>
+      <c r="CM58" s="9"/>
+      <c r="CN58" s="9"/>
+      <c r="CO58" s="9"/>
+      <c r="CP58" s="9"/>
+      <c r="CQ58" s="9"/>
+      <c r="CR58" s="9"/>
+      <c r="CS58" s="9"/>
+      <c r="CT58" s="9"/>
+      <c r="CU58" s="9"/>
+      <c r="DX58" s="9"/>
+      <c r="DY58" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="DZ58" s="9"/>
+      <c r="EA58" s="9"/>
+      <c r="EB58" s="9"/>
+      <c r="EC58" s="9"/>
+      <c r="ED58" s="9"/>
+      <c r="EE58" s="9"/>
+      <c r="EF58" s="9"/>
+      <c r="EG58" s="9"/>
+      <c r="EH58" s="9"/>
+      <c r="EI58" s="9"/>
+      <c r="EJ58" s="9"/>
+      <c r="EK58" s="9"/>
+      <c r="EL58" s="9"/>
+      <c r="FA58" s="9"/>
+      <c r="FB58" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="FC58" s="9"/>
+      <c r="FD58" s="9"/>
+      <c r="FE58" s="9"/>
+      <c r="FF58" s="9"/>
+      <c r="FG58" s="9"/>
+      <c r="FH58" s="9"/>
+      <c r="FI58" s="9"/>
+      <c r="FJ58" s="9"/>
+      <c r="FK58" s="9"/>
+      <c r="FL58" s="9"/>
+      <c r="FM58" s="9"/>
+      <c r="FN58" s="9"/>
+      <c r="FO58" s="9"/>
+      <c r="FP58" s="9"/>
+      <c r="FQ58" s="9"/>
+    </row>
+    <row r="59" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B59" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
+      <c r="CG59" s="9"/>
+      <c r="CH59" s="9"/>
+      <c r="CI59" s="9"/>
+      <c r="CJ59" s="9"/>
+      <c r="CK59" s="9"/>
+      <c r="CL59" s="9"/>
+      <c r="CM59" s="9"/>
+      <c r="CN59" s="9"/>
+      <c r="CO59" s="9"/>
+      <c r="CP59" s="9"/>
+      <c r="CQ59" s="9"/>
+      <c r="CR59" s="9"/>
+      <c r="CS59" s="9"/>
+      <c r="CT59" s="9"/>
+      <c r="CU59" s="9"/>
+      <c r="DX59" s="9"/>
+      <c r="DY59" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="DZ59" s="9"/>
+      <c r="EA59" s="9"/>
+      <c r="EB59" s="9"/>
+      <c r="EC59" s="9"/>
+      <c r="ED59" s="9"/>
+      <c r="EE59" s="9"/>
+      <c r="EF59" s="9"/>
+      <c r="EG59" s="9"/>
+      <c r="EH59" s="9"/>
+      <c r="EI59" s="9"/>
+      <c r="EJ59" s="9"/>
+      <c r="EK59" s="9"/>
+      <c r="EL59" s="9"/>
+      <c r="FA59" s="9"/>
+      <c r="FB59" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="FC59" s="9"/>
+      <c r="FD59" s="9"/>
+      <c r="FE59" s="9"/>
+      <c r="FF59" s="9"/>
+      <c r="FG59" s="9"/>
+      <c r="FH59" s="9"/>
+      <c r="FI59" s="9"/>
+      <c r="FJ59" s="9"/>
+      <c r="FK59" s="9"/>
+      <c r="FL59" s="9"/>
+      <c r="FM59" s="9"/>
+      <c r="FN59" s="9"/>
+      <c r="FO59" s="9"/>
+      <c r="FP59" s="9"/>
+      <c r="FQ59" s="9"/>
+    </row>
+    <row r="60" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B60" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
+      <c r="CG60" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="CH60" s="9"/>
+      <c r="CI60" s="9"/>
+      <c r="CJ60" s="9"/>
+      <c r="CK60" s="9"/>
+      <c r="CL60" s="9"/>
+      <c r="CM60" s="9"/>
+      <c r="CN60" s="9"/>
+      <c r="CO60" s="9"/>
+      <c r="CP60" s="9"/>
+      <c r="CQ60" s="9"/>
+      <c r="CR60" s="9"/>
+      <c r="CS60" s="9"/>
+      <c r="CT60" s="9"/>
+      <c r="CU60" s="9"/>
+      <c r="DX60" s="9"/>
+      <c r="DY60" s="9"/>
+      <c r="DZ60" s="9"/>
+      <c r="EA60" s="9"/>
+      <c r="EB60" s="9"/>
+      <c r="EC60" s="9"/>
+      <c r="ED60" s="9"/>
+      <c r="EE60" s="9"/>
+      <c r="EF60" s="9"/>
+      <c r="EG60" s="9"/>
+      <c r="EH60" s="9"/>
+      <c r="EI60" s="9"/>
+      <c r="EJ60" s="9"/>
+      <c r="EK60" s="9"/>
+      <c r="EL60" s="9"/>
+      <c r="FA60" s="9"/>
+      <c r="FB60" s="9"/>
+      <c r="FC60" s="9"/>
+      <c r="FD60" s="9"/>
+      <c r="FE60" s="9"/>
+      <c r="FF60" s="9"/>
+      <c r="FG60" s="9"/>
+      <c r="FH60" s="9"/>
+      <c r="FI60" s="9"/>
+      <c r="FJ60" s="9"/>
+      <c r="FK60" s="9"/>
+      <c r="FL60" s="9"/>
+      <c r="FM60" s="9"/>
+      <c r="FN60" s="9"/>
+      <c r="FO60" s="9"/>
+      <c r="FP60" s="9"/>
+      <c r="FQ60" s="9"/>
+    </row>
+    <row r="61" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B61" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
+      <c r="L61" s="9"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="9"/>
+      <c r="CG61" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="CH61" s="9"/>
+      <c r="CI61" s="9"/>
+      <c r="CJ61" s="9"/>
+      <c r="CK61" s="9"/>
+      <c r="CL61" s="9"/>
+      <c r="CM61" s="9"/>
+      <c r="CN61" s="9"/>
+      <c r="CO61" s="9"/>
+      <c r="CP61" s="9"/>
+      <c r="CQ61" s="9"/>
+      <c r="CR61" s="9"/>
+      <c r="CS61" s="9"/>
+      <c r="CT61" s="9"/>
+      <c r="CU61" s="9"/>
+      <c r="DX61" s="63" t="s">
+        <v>320</v>
+      </c>
+      <c r="DY61" s="64"/>
+      <c r="DZ61" s="9"/>
+      <c r="EA61" s="9"/>
+      <c r="EB61" s="9"/>
+      <c r="EC61" s="9"/>
+      <c r="ED61" s="9"/>
+      <c r="EE61" s="9"/>
+      <c r="EF61" s="9"/>
+      <c r="EG61" s="9"/>
+      <c r="EH61" s="9"/>
+      <c r="EI61" s="9"/>
+      <c r="EJ61" s="9"/>
+      <c r="EK61" s="9"/>
+      <c r="EL61" s="9"/>
+      <c r="FA61" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="FB61" s="9"/>
+      <c r="FC61" s="9"/>
+      <c r="FD61" s="9"/>
+      <c r="FE61" s="9"/>
+      <c r="FF61" s="9"/>
+      <c r="FG61" s="9"/>
+      <c r="FH61" s="9"/>
+      <c r="FI61" s="9"/>
+      <c r="FJ61" s="9"/>
+      <c r="FK61" s="9"/>
+      <c r="FL61" s="9"/>
+      <c r="FM61" s="9"/>
+      <c r="FN61" s="9"/>
+      <c r="FO61" s="9"/>
+      <c r="FP61" s="9"/>
+      <c r="FQ61" s="9"/>
+    </row>
+    <row r="62" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B62" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+      <c r="N62" s="9"/>
+      <c r="CG62" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="CH62" s="9"/>
+      <c r="CI62" s="9"/>
+      <c r="CJ62" s="9"/>
+      <c r="CK62" s="9"/>
+      <c r="CL62" s="9"/>
+      <c r="CM62" s="9"/>
+      <c r="CN62" s="9"/>
+      <c r="CO62" s="9"/>
+      <c r="CP62" s="9"/>
+      <c r="CQ62" s="9"/>
+      <c r="CR62" s="9"/>
+      <c r="CS62" s="9"/>
+      <c r="CT62" s="9"/>
+      <c r="CU62" s="9"/>
+      <c r="DX62" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="DY62" s="9"/>
+      <c r="DZ62" s="9"/>
+      <c r="EA62" s="9"/>
+      <c r="EB62" s="9"/>
+      <c r="EC62" s="9"/>
+      <c r="ED62" s="9"/>
+      <c r="EE62" s="9"/>
+      <c r="EF62" s="9"/>
+      <c r="EG62" s="9"/>
+      <c r="EH62" s="9"/>
+      <c r="EI62" s="9"/>
+      <c r="EJ62" s="9"/>
+      <c r="EK62" s="9"/>
+      <c r="EL62" s="9"/>
+      <c r="FA62" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="FB62" s="9"/>
+      <c r="FC62" s="9"/>
+      <c r="FD62" s="9"/>
+      <c r="FE62" s="9"/>
+      <c r="FF62" s="9"/>
+      <c r="FG62" s="9"/>
+      <c r="FH62" s="9"/>
+      <c r="FI62" s="9"/>
+      <c r="FJ62" s="9"/>
+      <c r="FK62" s="9"/>
+      <c r="FL62" s="9"/>
+      <c r="FM62" s="9"/>
+      <c r="FN62" s="9"/>
+      <c r="FO62" s="9"/>
+      <c r="FP62" s="9"/>
+      <c r="FQ62" s="9"/>
+    </row>
+    <row r="63" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B63" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="9"/>
+      <c r="DX63" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="DY63" s="9"/>
+      <c r="DZ63" s="9"/>
+      <c r="EA63" s="9"/>
+      <c r="EB63" s="9"/>
+      <c r="EC63" s="9"/>
+      <c r="ED63" s="9"/>
+      <c r="EE63" s="9"/>
+      <c r="EF63" s="9"/>
+      <c r="EG63" s="9"/>
+      <c r="EH63" s="9"/>
+      <c r="EI63" s="9"/>
+      <c r="EJ63" s="9"/>
+      <c r="EK63" s="9"/>
+      <c r="EL63" s="9"/>
+      <c r="FA63" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="FB63" s="9"/>
+      <c r="FC63" s="9"/>
+      <c r="FD63" s="9"/>
+      <c r="FE63" s="9"/>
+      <c r="FF63" s="9"/>
+      <c r="FG63" s="9"/>
+      <c r="FH63" s="9"/>
+      <c r="FI63" s="9"/>
+      <c r="FJ63" s="9"/>
+      <c r="FK63" s="9"/>
+      <c r="FL63" s="9"/>
+      <c r="FM63" s="9"/>
+      <c r="FN63" s="9"/>
+      <c r="FO63" s="9"/>
+      <c r="FP63" s="9"/>
+      <c r="FQ63" s="9"/>
+    </row>
+    <row r="64" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B64" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
+      <c r="DX64" s="9"/>
+      <c r="DY64" s="9"/>
+      <c r="DZ64" s="9"/>
+      <c r="EA64" s="9"/>
+      <c r="EB64" s="9"/>
+      <c r="EC64" s="9"/>
+      <c r="ED64" s="9"/>
+      <c r="EE64" s="9"/>
+      <c r="EF64" s="9"/>
+      <c r="EG64" s="9"/>
+      <c r="EH64" s="9"/>
+      <c r="EI64" s="9"/>
+      <c r="EJ64" s="9"/>
+      <c r="EK64" s="9"/>
+      <c r="EL64" s="9"/>
+      <c r="FA64" s="9"/>
+      <c r="FB64" s="9"/>
+      <c r="FC64" s="9"/>
+      <c r="FD64" s="9"/>
+      <c r="FE64" s="9"/>
+      <c r="FF64" s="9"/>
+      <c r="FG64" s="9"/>
+      <c r="FH64" s="9"/>
+      <c r="FI64" s="9"/>
+      <c r="FJ64" s="9"/>
+      <c r="FK64" s="9"/>
+      <c r="FL64" s="9"/>
+      <c r="FM64" s="9"/>
+      <c r="FN64" s="9"/>
+      <c r="FO64" s="9"/>
+      <c r="FP64" s="9"/>
+      <c r="FQ64" s="9"/>
+    </row>
+    <row r="65" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B65" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="9"/>
+      <c r="DX65" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="DY65" s="9"/>
+      <c r="DZ65" s="9"/>
+      <c r="EA65" s="9"/>
+      <c r="EB65" s="9"/>
+      <c r="EC65" s="9"/>
+      <c r="ED65" s="9"/>
+      <c r="EE65" s="9"/>
+      <c r="EF65" s="9"/>
+      <c r="EG65" s="9"/>
+      <c r="EH65" s="9"/>
+      <c r="EI65" s="9"/>
+      <c r="EJ65" s="9"/>
+      <c r="EK65" s="9"/>
+      <c r="EL65" s="9"/>
+      <c r="FA65" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="FB65" s="9"/>
+      <c r="FC65" s="9"/>
+      <c r="FD65" s="9"/>
+      <c r="FE65" s="9"/>
+      <c r="FF65" s="9"/>
+      <c r="FG65" s="9"/>
+      <c r="FH65" s="9"/>
+      <c r="FI65" s="9"/>
+      <c r="FJ65" s="9"/>
+      <c r="FK65" s="9"/>
+      <c r="FL65" s="9"/>
+      <c r="FM65" s="9"/>
+      <c r="FN65" s="9"/>
+      <c r="FO65" s="9"/>
+      <c r="FP65" s="9"/>
+      <c r="FQ65" s="9"/>
+    </row>
+    <row r="66" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B66" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="9"/>
+      <c r="DX66" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="DY66" s="9"/>
+      <c r="DZ66" s="9"/>
+      <c r="EA66" s="9"/>
+      <c r="EB66" s="9"/>
+      <c r="EC66" s="9"/>
+      <c r="ED66" s="9"/>
+      <c r="EE66" s="9"/>
+      <c r="EF66" s="9"/>
+      <c r="EG66" s="9"/>
+      <c r="EH66" s="9"/>
+      <c r="EI66" s="9"/>
+      <c r="EJ66" s="9"/>
+      <c r="EK66" s="9"/>
+      <c r="EL66" s="9"/>
+      <c r="FA66" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="FB66" s="9"/>
+      <c r="FC66" s="9"/>
+      <c r="FD66" s="9"/>
+      <c r="FE66" s="9"/>
+      <c r="FF66" s="9"/>
+      <c r="FG66" s="9"/>
+      <c r="FH66" s="9"/>
+      <c r="FI66" s="9"/>
+      <c r="FJ66" s="9"/>
+      <c r="FK66" s="9"/>
+      <c r="FL66" s="9"/>
+      <c r="FM66" s="9"/>
+      <c r="FN66" s="9"/>
+      <c r="FO66" s="9"/>
+      <c r="FP66" s="9"/>
+      <c r="FQ66" s="9"/>
+      <c r="FR66" s="53" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="67" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="9"/>
+      <c r="DX67" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="DY67" s="9"/>
+      <c r="DZ67" s="9"/>
+      <c r="EA67" s="9"/>
+      <c r="EB67" s="9"/>
+      <c r="EC67" s="9"/>
+      <c r="ED67" s="9"/>
+      <c r="EE67" s="9"/>
+      <c r="EF67" s="9"/>
+      <c r="EG67" s="9"/>
+      <c r="EH67" s="9"/>
+      <c r="EI67" s="9"/>
+      <c r="EJ67" s="9"/>
+      <c r="EK67" s="9"/>
+      <c r="EL67" s="9"/>
+      <c r="FA67" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="FB67" s="9"/>
+      <c r="FC67" s="9"/>
+      <c r="FD67" s="9"/>
+      <c r="FE67" s="9"/>
+      <c r="FF67" s="9"/>
+      <c r="FG67" s="9"/>
+      <c r="FH67" s="9"/>
+      <c r="FI67" s="9"/>
+      <c r="FJ67" s="9"/>
+      <c r="FK67" s="9"/>
+      <c r="FL67" s="9"/>
+      <c r="FM67" s="9"/>
+      <c r="FN67" s="9"/>
+      <c r="FO67" s="9"/>
+      <c r="FP67" s="9"/>
+      <c r="FQ67" s="9"/>
+      <c r="FR67" s="53" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="68" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B68" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
+      <c r="DX68" s="9"/>
+      <c r="DY68" s="9"/>
+      <c r="DZ68" s="9"/>
+      <c r="EA68" s="9"/>
+      <c r="EB68" s="9"/>
+      <c r="EC68" s="9"/>
+      <c r="ED68" s="9"/>
+      <c r="EE68" s="9"/>
+      <c r="EF68" s="9"/>
+      <c r="EG68" s="9"/>
+      <c r="EH68" s="9"/>
+      <c r="EI68" s="9"/>
+      <c r="EJ68" s="9"/>
+      <c r="EK68" s="9"/>
+      <c r="EL68" s="9"/>
+      <c r="FA68" s="9"/>
+      <c r="FB68" s="9"/>
+      <c r="FC68" s="9"/>
+      <c r="FD68" s="9"/>
+      <c r="FE68" s="9"/>
+      <c r="FF68" s="9"/>
+      <c r="FG68" s="9"/>
+      <c r="FH68" s="9"/>
+      <c r="FI68" s="9"/>
+      <c r="FJ68" s="9"/>
+      <c r="FK68" s="9"/>
+      <c r="FL68" s="9"/>
+      <c r="FM68" s="9"/>
+      <c r="FN68" s="9"/>
+      <c r="FO68" s="9"/>
+      <c r="FP68" s="9"/>
+      <c r="FQ68" s="9"/>
+      <c r="FS68" s="53" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="69" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B69" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9"/>
+      <c r="DX69" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="DY69" s="9"/>
+      <c r="DZ69" s="9"/>
+      <c r="EA69" s="9"/>
+      <c r="EB69" s="9"/>
+      <c r="EC69" s="9"/>
+      <c r="ED69" s="9"/>
+      <c r="EE69" s="9"/>
+      <c r="EF69" s="9"/>
+      <c r="EG69" s="9"/>
+      <c r="EH69" s="9"/>
+      <c r="EI69" s="9"/>
+      <c r="EJ69" s="9"/>
+      <c r="EK69" s="9"/>
+      <c r="EL69" s="9"/>
+      <c r="EM69" s="53" t="s">
+        <v>334</v>
+      </c>
+      <c r="FA69" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="FB69" s="9"/>
+      <c r="FC69" s="9"/>
+      <c r="FD69" s="9"/>
+      <c r="FE69" s="9"/>
+      <c r="FF69" s="9"/>
+      <c r="FG69" s="9"/>
+      <c r="FH69" s="9"/>
+      <c r="FI69" s="9"/>
+      <c r="FJ69" s="9"/>
+      <c r="FK69" s="9"/>
+      <c r="FL69" s="9"/>
+      <c r="FM69" s="9"/>
+      <c r="FN69" s="9"/>
+      <c r="FO69" s="9"/>
+      <c r="FP69" s="9"/>
+      <c r="FQ69" s="9"/>
+      <c r="FS69" s="53" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="70" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B70" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="9"/>
+      <c r="DX70" s="9"/>
+      <c r="DY70" s="9"/>
+      <c r="DZ70" s="9"/>
+      <c r="EA70" s="9"/>
+      <c r="EB70" s="9"/>
+      <c r="EC70" s="9"/>
+      <c r="ED70" s="9"/>
+      <c r="EE70" s="9"/>
+      <c r="EF70" s="9"/>
+      <c r="EG70" s="9"/>
+      <c r="EH70" s="9"/>
+      <c r="EI70" s="9"/>
+      <c r="EJ70" s="9"/>
+      <c r="EK70" s="9"/>
+      <c r="EL70" s="9"/>
+      <c r="EM70" s="53"/>
+      <c r="FA70" s="9"/>
+      <c r="FB70" s="9"/>
+      <c r="FC70" s="9"/>
+      <c r="FD70" s="9"/>
+      <c r="FE70" s="9"/>
+      <c r="FF70" s="9"/>
+      <c r="FG70" s="9"/>
+      <c r="FH70" s="9"/>
+      <c r="FI70" s="9"/>
+      <c r="FJ70" s="9"/>
+      <c r="FK70" s="9"/>
+      <c r="FL70" s="9"/>
+      <c r="FM70" s="9"/>
+      <c r="FN70" s="9"/>
+      <c r="FO70" s="9"/>
+      <c r="FP70" s="9"/>
+      <c r="FQ70" s="9"/>
+      <c r="FR70" s="53" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="71" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B71" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="9"/>
+      <c r="DX71" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="DY71" s="9"/>
+      <c r="DZ71" s="9"/>
+      <c r="EA71" s="9"/>
+      <c r="EB71" s="9"/>
+      <c r="EC71" s="9"/>
+      <c r="ED71" s="9"/>
+      <c r="EE71" s="9"/>
+      <c r="EF71" s="9"/>
+      <c r="EG71" s="9"/>
+      <c r="EH71" s="9"/>
+      <c r="EI71" s="9"/>
+      <c r="EJ71" s="9"/>
+      <c r="EK71" s="9"/>
+      <c r="EL71" s="9"/>
+      <c r="EM71" s="53"/>
+      <c r="FA71" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="FB71" s="9"/>
+      <c r="FC71" s="9"/>
+      <c r="FD71" s="9"/>
+      <c r="FE71" s="9"/>
+      <c r="FF71" s="9"/>
+      <c r="FG71" s="9"/>
+      <c r="FH71" s="9"/>
+      <c r="FI71" s="9"/>
+      <c r="FJ71" s="9"/>
+      <c r="FK71" s="9"/>
+      <c r="FL71" s="9"/>
+      <c r="FM71" s="9"/>
+      <c r="FN71" s="9"/>
+      <c r="FO71" s="9"/>
+      <c r="FP71" s="9"/>
+      <c r="FQ71" s="9"/>
+    </row>
+    <row r="72" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B72" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="9"/>
+      <c r="DX72" s="63" t="s">
+        <v>331</v>
+      </c>
+      <c r="DY72" s="9"/>
+      <c r="DZ72" s="9"/>
+      <c r="EA72" s="9"/>
+      <c r="EB72" s="9"/>
+      <c r="EC72" s="9"/>
+      <c r="ED72" s="9"/>
+      <c r="EE72" s="9"/>
+      <c r="EF72" s="9"/>
+      <c r="EG72" s="9"/>
+      <c r="EH72" s="9"/>
+      <c r="EI72" s="9"/>
+      <c r="EJ72" s="9"/>
+      <c r="EK72" s="9"/>
+      <c r="EL72" s="9"/>
+      <c r="EM72" s="53" t="s">
+        <v>335</v>
+      </c>
+      <c r="FA72" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="FB72" s="9"/>
+      <c r="FC72" s="9"/>
+      <c r="FD72" s="9"/>
+      <c r="FE72" s="9"/>
+      <c r="FF72" s="9"/>
+      <c r="FG72" s="9"/>
+      <c r="FH72" s="9"/>
+      <c r="FI72" s="9"/>
+      <c r="FJ72" s="9"/>
+      <c r="FK72" s="9"/>
+      <c r="FL72" s="9"/>
+      <c r="FM72" s="9"/>
+      <c r="FN72" s="9"/>
+      <c r="FO72" s="9"/>
+      <c r="FP72" s="9"/>
+      <c r="FQ72" s="9"/>
+    </row>
+    <row r="73" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="B73" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="9"/>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
+      <c r="DX73" s="63" t="s">
+        <v>332</v>
+      </c>
+      <c r="DY73" s="9"/>
+      <c r="DZ73" s="9"/>
+      <c r="EA73" s="9"/>
+      <c r="EB73" s="9"/>
+      <c r="EC73" s="9"/>
+      <c r="ED73" s="9"/>
+      <c r="EE73" s="9"/>
+      <c r="EF73" s="9"/>
+      <c r="EG73" s="9"/>
+      <c r="EH73" s="9"/>
+      <c r="EI73" s="9"/>
+      <c r="EJ73" s="9"/>
+      <c r="EK73" s="9"/>
+      <c r="EL73" s="9"/>
+      <c r="FA73" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="FB73" s="9"/>
+      <c r="FC73" s="9"/>
+      <c r="FD73" s="9"/>
+      <c r="FE73" s="9"/>
+      <c r="FF73" s="9"/>
+      <c r="FG73" s="9"/>
+      <c r="FH73" s="9"/>
+      <c r="FI73" s="9"/>
+      <c r="FJ73" s="9"/>
+      <c r="FK73" s="9"/>
+      <c r="FL73" s="9"/>
+      <c r="FM73" s="9"/>
+      <c r="FN73" s="9"/>
+      <c r="FO73" s="9"/>
+      <c r="FP73" s="9"/>
+      <c r="FQ73" s="9"/>
+    </row>
+    <row r="74" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="DX74" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="DY74" s="9"/>
+      <c r="DZ74" s="9"/>
+      <c r="EA74" s="9"/>
+      <c r="EB74" s="9"/>
+      <c r="EC74" s="9"/>
+      <c r="ED74" s="9"/>
+      <c r="EE74" s="9"/>
+      <c r="EF74" s="9"/>
+      <c r="EG74" s="9"/>
+      <c r="EH74" s="9"/>
+      <c r="EI74" s="9"/>
+      <c r="EJ74" s="9"/>
+      <c r="EK74" s="9"/>
+      <c r="EL74" s="9"/>
+      <c r="FA74" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="FB74" s="9"/>
+      <c r="FC74" s="9"/>
+      <c r="FD74" s="9"/>
+      <c r="FE74" s="9"/>
+      <c r="FF74" s="9"/>
+      <c r="FG74" s="9"/>
+      <c r="FH74" s="9"/>
+      <c r="FI74" s="9"/>
+      <c r="FJ74" s="9"/>
+      <c r="FK74" s="9"/>
+      <c r="FL74" s="9"/>
+      <c r="FM74" s="9"/>
+      <c r="FN74" s="9"/>
+      <c r="FO74" s="9"/>
+      <c r="FP74" s="9"/>
+      <c r="FQ74" s="9"/>
+    </row>
+    <row r="75" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="DX75" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="DY75" s="9"/>
+      <c r="DZ75" s="9"/>
+      <c r="EA75" s="9"/>
+      <c r="EB75" s="9"/>
+      <c r="EC75" s="9"/>
+      <c r="ED75" s="9"/>
+      <c r="EE75" s="9"/>
+      <c r="EF75" s="9"/>
+      <c r="EG75" s="9"/>
+      <c r="EH75" s="9"/>
+      <c r="EI75" s="9"/>
+      <c r="EJ75" s="9"/>
+      <c r="EK75" s="9"/>
+      <c r="EL75" s="9"/>
+      <c r="FA75" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="FB75" s="9"/>
+      <c r="FC75" s="9"/>
+      <c r="FD75" s="9"/>
+      <c r="FE75" s="9"/>
+      <c r="FF75" s="9"/>
+      <c r="FG75" s="9"/>
+      <c r="FH75" s="9"/>
+      <c r="FI75" s="9"/>
+      <c r="FJ75" s="9"/>
+      <c r="FK75" s="9"/>
+      <c r="FL75" s="9"/>
+      <c r="FM75" s="9"/>
+      <c r="FN75" s="9"/>
+      <c r="FO75" s="9"/>
+      <c r="FP75" s="9"/>
+      <c r="FQ75" s="9"/>
+    </row>
+    <row r="76" spans="2:175" x14ac:dyDescent="0.4">
+      <c r="DX76" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="DY76" s="9"/>
+      <c r="DZ76" s="9"/>
+      <c r="EA76" s="9"/>
+      <c r="EB76" s="9"/>
+      <c r="EC76" s="9"/>
+      <c r="ED76" s="9"/>
+      <c r="EE76" s="9"/>
+      <c r="EF76" s="9"/>
+      <c r="EG76" s="9"/>
+      <c r="EH76" s="9"/>
+      <c r="EI76" s="9"/>
+      <c r="EJ76" s="9"/>
+      <c r="EK76" s="9"/>
+      <c r="EL76" s="9"/>
+      <c r="FA76" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="FB76" s="9"/>
+      <c r="FC76" s="9"/>
+      <c r="FD76" s="9"/>
+      <c r="FE76" s="9"/>
+      <c r="FF76" s="9"/>
+      <c r="FG76" s="9"/>
+      <c r="FH76" s="9"/>
+      <c r="FI76" s="9"/>
+      <c r="FJ76" s="9"/>
+      <c r="FK76" s="9"/>
+      <c r="FL76" s="9"/>
+      <c r="FM76" s="9"/>
+      <c r="FN76" s="9"/>
+      <c r="FO76" s="9"/>
+      <c r="FP76" s="9"/>
+      <c r="FQ76" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{9E8104E2-0B1A-498B-A07D-38DAF385409A}"/>
+    <hyperlink ref="Q43" r:id="rId2" xr:uid="{C9A864E0-135D-4BC6-BAC2-C835A37D8BD6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
doc: 1189. Maximum Number of Balloons
Leetcode problem 1189. Maximum Number of Balloons is solved and the learnings are captured

URL: https://leetcode.com/problems/maximum-number-of-balloons/description/?envType=problem-list-v2&envId=string
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA99734-07CF-4E03-98DF-A1FC6A2FDEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F77FE8-5F24-4F79-81F9-747A65A51E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
   <sheets>
-    <sheet name="A" sheetId="1" r:id="rId1"/>
-    <sheet name="S" sheetId="3" r:id="rId2"/>
-    <sheet name="Format" sheetId="2" r:id="rId3"/>
+    <sheet name="Simple" sheetId="4" r:id="rId1"/>
+    <sheet name="A" sheetId="1" r:id="rId2"/>
+    <sheet name="S" sheetId="3" r:id="rId3"/>
+    <sheet name="Format" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="497">
   <si>
     <t>Title</t>
   </si>
@@ -1628,6 +1629,117 @@
   </si>
   <si>
     <t>2000. Reverse Prefix of Word</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int maxNumberOfBalloons(string text) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int b = 0, a = 0, l = 0, o = 0, n = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int pos;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        for (char ch : text) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            switch (ch) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            case 'b':</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                b++;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                break;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            case 'a':</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                a++;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            case 'l':</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                l++;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            case 'o':</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                o++;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            case 'n':</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                n++;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            default:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            ch='X';</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int min = (b&lt;a)?((b&lt;n)?b:n):((a&lt;n)?a:n);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int res = (l&lt;o)?(((l/2)&lt;min)?(l/2):min):(((o/2)&lt;min)?(o/2):min);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return res;</t>
+  </si>
+  <si>
+    <t>case b wont work</t>
+  </si>
+  <si>
+    <t>we should give in ''</t>
+  </si>
+  <si>
+    <t>int maxNumberOfBalloons(string text) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int b, a, l, o, n;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        b = a = l = o = n = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        for (auto ch : text) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            b += (ch == 'b');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            a += (ch == 'a');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            l += (ch == 'l');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            o += (ch == 'o');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            n += (ch == 'n');</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return min({b, a, l/2, o/2, n});</t>
+  </si>
+  <si>
+    <t>the condition returns 0 is false and 1 if true</t>
+  </si>
+  <si>
+    <t>So the increment can be done in this way</t>
+  </si>
+  <si>
+    <t>1189. Maximum Number of Balloons</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-number-of-balloons/description/?envType=problem-list-v2&amp;envId=string</t>
   </si>
 </sst>
 </file>
@@ -2506,6 +2618,1245 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE91F9C-297C-4D59-9996-90CC520AF8DF}">
+  <dimension ref="B1:AK399"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3:AI14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.77734375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="18" width="4.77734375" style="53"/>
+    <col min="25" max="38" width="4.77734375" style="53"/>
+    <col min="39" max="41" width="4.77734375" style="53" customWidth="1"/>
+    <col min="42" max="16384" width="4.77734375" style="53"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="53" t="s">
+        <v>495</v>
+      </c>
+      <c r="O2" s="62" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="3" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="Y3" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="9"/>
+    </row>
+    <row r="4" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="Y4" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="9"/>
+      <c r="AH4" s="9"/>
+      <c r="AI4" s="9"/>
+    </row>
+    <row r="5" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="Y5" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9"/>
+      <c r="AI5" s="9"/>
+    </row>
+    <row r="6" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="Y6" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
+    </row>
+    <row r="7" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="Y7" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AK7" s="53" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="8" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="Y8" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AK8" s="53" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="9" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="9" t="s">
+        <v>464</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="Y9" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+    </row>
+    <row r="10" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="53" t="s">
+        <v>481</v>
+      </c>
+      <c r="Y10" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+    </row>
+    <row r="11" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="53" t="s">
+        <v>482</v>
+      </c>
+      <c r="Y11" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+    </row>
+    <row r="12" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="Y12" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+    </row>
+    <row r="13" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="Y13" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="9"/>
+    </row>
+    <row r="14" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="Y14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
+      <c r="AG14" s="9"/>
+      <c r="AH14" s="9"/>
+      <c r="AI14" s="9"/>
+    </row>
+    <row r="15" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+    </row>
+    <row r="16" spans="2:37" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+    </row>
+    <row r="17" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+    </row>
+    <row r="18" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+    </row>
+    <row r="19" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+    </row>
+    <row r="20" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+    </row>
+    <row r="21" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+    </row>
+    <row r="22" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+    </row>
+    <row r="23" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+    </row>
+    <row r="24" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+    </row>
+    <row r="25" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+    </row>
+    <row r="26" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+    </row>
+    <row r="27" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+    </row>
+    <row r="28" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+    </row>
+    <row r="29" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B29" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+    </row>
+    <row r="30" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+    </row>
+    <row r="31" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+    </row>
+    <row r="32" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+    </row>
+    <row r="33" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+    </row>
+    <row r="34" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B34" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+    </row>
+    <row r="35" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="37" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="38" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="39" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="40" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="41" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="42" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="43" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="44" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="45" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="46" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="47" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="48" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="49" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="50" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="51" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="52" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="53" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="54" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="55" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="56" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="57" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="58" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="59" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="60" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="61" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="62" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="63" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="64" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="65" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="66" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="67" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="68" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="69" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="70" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="71" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="72" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="73" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="74" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="75" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="76" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="77" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="78" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="79" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="80" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="81" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="82" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="83" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="84" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="85" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="86" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="87" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="88" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="89" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="90" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="91" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="92" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="93" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="94" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="95" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="96" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="97" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="98" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="99" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="100" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="101" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="102" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="103" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="104" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="105" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="106" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="107" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="108" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="109" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="110" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="111" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="112" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="113" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="114" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="115" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="116" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="117" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="118" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="119" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="120" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="121" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="122" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="123" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="124" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="125" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="126" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="127" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="128" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="129" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="130" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="131" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="132" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="133" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="134" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="135" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="136" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="137" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="138" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="139" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="140" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="141" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="142" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="143" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="144" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="145" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="146" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="147" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="148" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="149" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="150" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="151" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="152" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="153" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="154" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="155" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="156" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="157" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="158" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="159" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="160" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="161" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="162" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="163" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="164" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="165" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="166" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="167" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="168" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="169" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="170" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="171" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="172" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="173" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="174" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="175" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="176" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="177" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="178" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="179" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="180" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="181" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="182" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="183" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="184" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="185" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="186" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="187" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="188" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="189" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="190" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="191" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="192" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="193" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="194" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="195" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="196" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="197" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="198" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="199" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="200" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="201" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="202" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="203" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="204" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="205" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="206" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="207" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="208" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="209" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="210" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="211" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="212" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="213" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="214" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="215" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="216" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="217" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="218" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="219" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="220" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="221" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="222" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="223" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="224" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="225" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="226" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="227" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="228" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="229" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="230" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="231" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="232" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="233" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="234" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="235" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="236" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="237" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="238" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="239" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="240" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="241" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="242" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="243" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="244" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="245" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="246" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="247" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="248" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="249" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="250" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="251" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="252" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="253" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="254" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="255" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="256" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="257" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="258" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="259" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="260" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="261" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="262" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="263" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="264" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="265" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="266" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="267" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="268" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="269" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="270" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="271" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="272" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="273" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="274" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="275" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="276" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="277" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="278" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="279" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="280" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="281" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="282" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="283" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="284" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="285" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="286" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="287" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="288" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="289" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="290" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="291" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="292" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="293" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="294" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="295" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="296" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="297" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="298" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="299" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="300" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="301" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="302" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="303" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="304" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="305" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="306" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="307" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="308" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="309" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="310" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="311" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="312" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="313" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="314" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="315" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="316" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="317" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="318" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="319" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="320" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="321" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="322" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="323" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="324" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="325" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="326" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="327" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="328" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="329" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="330" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="331" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="332" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="333" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="334" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="335" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="336" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="337" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="338" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="339" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="340" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="341" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="342" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="343" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="344" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="345" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="346" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="347" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="348" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="349" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="350" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="351" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="352" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="353" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="354" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="355" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="356" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="357" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="358" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="359" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="360" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="361" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="362" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="363" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="364" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="365" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="366" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="367" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="368" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="369" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="370" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="371" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="372" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="373" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="374" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="375" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="376" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="377" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="378" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="379" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="380" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="381" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="382" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="383" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="384" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="385" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="386" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="387" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="388" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="389" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="390" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="391" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="392" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="393" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="394" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="395" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="396" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="397" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="398" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="399" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{33BE294A-425B-4A78-9221-04CE79E267EB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE6A8EE-45F0-4DFE-8B47-A80E55C53C69}">
   <dimension ref="B1:AP399"/>
   <sheetViews>
@@ -7432,12 +8783,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28504ADD-8E4E-436B-849F-525BA36E82D6}">
   <dimension ref="A2:HD127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -16394,7 +17745,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AB2F21-1695-41F3-AD6E-505367934BD2}">
   <dimension ref="B1:AP84"/>
   <sheetViews>

</xml_diff>

<commit_message>
doc: 125. Valid Palindrome
Leetcode problem 125. Valid Palindrome is solved and learnings are documented
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F77FE8-5F24-4F79-81F9-747A65A51E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026E5EFE-6F84-4989-A0B3-CDB585AB5DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="544">
   <si>
     <t>Title</t>
   </si>
@@ -1740,6 +1740,147 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/maximum-number-of-balloons/description/?envType=problem-list-v2&amp;envId=string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    bool isPalindrome(string s) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        std::string smallStr = "";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        for (char ch : s) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            if (((ch &gt;= 48) &amp;&amp; (ch &lt;= 57)) || ((ch &gt;= 97) &amp;&amp; (ch &lt;= 122))) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                smallStr.push_back(ch);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            } else if ((ch &gt;= 65) &amp;&amp; (ch &lt;= 90)) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                smallStr.push_back(ch + 32);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        std::string revStr = smallStr;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        std::reverse(revStr.begin(),revStr.end());</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if(smallStr==revStr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            return true;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        else </t>
+  </si>
+  <si>
+    <t xml:space="preserve">            return false;</t>
+  </si>
+  <si>
+    <t>125. Valid Palindrome</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-palindrome/description/?envType=problem-list-v2&amp;envId=string</t>
+  </si>
+  <si>
+    <t>#include &lt;cctype&gt; // For isalnum and tolower</t>
+  </si>
+  <si>
+    <t>#include &lt;algorithm&gt; // Optional, if you use reverse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    bool isPalindrome(std::string s) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int left = 0, right = s.size() - 1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        while (left &lt; right) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            // Move left to the next alphanumeric character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            while (left &lt; right &amp;&amp; !std::isalnum(s[left])) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                ++left;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            // Move right to the previous alphanumeric character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            while (left &lt; right &amp;&amp; !std::isalnum(s[right])) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                --right;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            // Compare characters (case-insensitive)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            if (std::tolower(s[left]) != std::tolower(s[right])) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                return false;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            ++left;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            --right;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return true;</t>
+  </si>
+  <si>
+    <t>std functions</t>
+  </si>
+  <si>
+    <t>bool isPalindrome(const char* s) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int left = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int right = strlen(s) - 1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    while (left &lt; right) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        // Move left pointer to next alphanumeric character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        while (left &lt; right &amp;&amp; !std::isalnum(s[left])) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        // Move right pointer to previous alphanumeric character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        while (left &lt; right &amp;&amp; !std::isalnum(s[right])) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        // Compare characters (case-insensitive)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (std::tolower(s[left]) != std::tolower(s[right])) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ++left;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        --right;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    return true;</t>
   </si>
 </sst>
 </file>
@@ -2621,7 +2762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE91F9C-297C-4D59-9996-90CC520AF8DF}">
   <dimension ref="B1:AK399"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y3" sqref="Y3:AI14"/>
     </sheetView>
   </sheetViews>
@@ -8785,10 +8926,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28504ADD-8E4E-436B-849F-525BA36E82D6}">
-  <dimension ref="A2:HD127"/>
+  <dimension ref="A2:HD163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="U146" workbookViewId="0">
+      <selection activeCell="AL163" sqref="AL163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -17735,6 +17876,1673 @@
       <c r="CK127" s="9"/>
       <c r="CL127" s="9"/>
     </row>
+    <row r="129" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B129" s="59" t="s">
+        <v>511</v>
+      </c>
+      <c r="N129" s="53" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="131" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B131" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C131" s="9"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="9"/>
+      <c r="G131" s="9"/>
+      <c r="H131" s="9"/>
+      <c r="I131" s="9"/>
+      <c r="J131" s="9"/>
+      <c r="K131" s="9"/>
+      <c r="L131" s="9"/>
+      <c r="M131" s="9"/>
+      <c r="N131" s="9"/>
+      <c r="O131" s="9"/>
+      <c r="P131" s="9"/>
+      <c r="Q131" s="9"/>
+      <c r="R131" s="9"/>
+      <c r="S131" s="9"/>
+      <c r="W131" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="X131" s="9"/>
+      <c r="Y131" s="9"/>
+      <c r="Z131" s="9"/>
+      <c r="AA131" s="9"/>
+      <c r="AB131" s="9"/>
+      <c r="AC131" s="9"/>
+      <c r="AD131" s="9"/>
+      <c r="AE131" s="9"/>
+      <c r="AF131" s="9"/>
+      <c r="AG131" s="9"/>
+      <c r="AH131" s="9"/>
+      <c r="AI131" s="9"/>
+      <c r="AJ131" s="9"/>
+      <c r="AK131" s="9"/>
+      <c r="AL131" s="9"/>
+      <c r="AQ131" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="AR131" s="9"/>
+      <c r="AS131" s="9"/>
+      <c r="AT131" s="9"/>
+      <c r="AU131" s="9"/>
+      <c r="AV131" s="9"/>
+      <c r="AW131" s="9"/>
+      <c r="AX131" s="9"/>
+      <c r="AY131" s="9"/>
+      <c r="AZ131" s="9"/>
+      <c r="BA131" s="9"/>
+      <c r="BB131" s="9"/>
+      <c r="BC131" s="9"/>
+      <c r="BD131" s="9"/>
+      <c r="BE131" s="9"/>
+      <c r="BF131" s="9"/>
+      <c r="BG131" s="9"/>
+    </row>
+    <row r="132" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B132" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C132" s="9"/>
+      <c r="D132" s="9"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="9"/>
+      <c r="G132" s="9"/>
+      <c r="H132" s="9"/>
+      <c r="I132" s="9"/>
+      <c r="J132" s="9"/>
+      <c r="K132" s="9"/>
+      <c r="L132" s="9"/>
+      <c r="M132" s="9"/>
+      <c r="N132" s="9"/>
+      <c r="O132" s="9"/>
+      <c r="P132" s="9"/>
+      <c r="Q132" s="9"/>
+      <c r="R132" s="9"/>
+      <c r="S132" s="9"/>
+      <c r="W132" s="64" t="s">
+        <v>513</v>
+      </c>
+      <c r="X132" s="9"/>
+      <c r="Y132" s="9"/>
+      <c r="Z132" s="9"/>
+      <c r="AA132" s="9"/>
+      <c r="AB132" s="9"/>
+      <c r="AC132" s="9"/>
+      <c r="AD132" s="9"/>
+      <c r="AE132" s="9"/>
+      <c r="AF132" s="9"/>
+      <c r="AG132" s="9"/>
+      <c r="AH132" s="9"/>
+      <c r="AI132" s="9"/>
+      <c r="AJ132" s="9"/>
+      <c r="AK132" s="9"/>
+      <c r="AL132" s="9"/>
+      <c r="AM132" s="53" t="s">
+        <v>530</v>
+      </c>
+      <c r="AQ132" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="AR132" s="9"/>
+      <c r="AS132" s="9"/>
+      <c r="AT132" s="9"/>
+      <c r="AU132" s="9"/>
+      <c r="AV132" s="9"/>
+      <c r="AW132" s="9"/>
+      <c r="AX132" s="9"/>
+      <c r="AY132" s="9"/>
+      <c r="AZ132" s="9"/>
+      <c r="BA132" s="9"/>
+      <c r="BB132" s="9"/>
+      <c r="BC132" s="9"/>
+      <c r="BD132" s="9"/>
+      <c r="BE132" s="9"/>
+      <c r="BF132" s="9"/>
+      <c r="BG132" s="9"/>
+    </row>
+    <row r="133" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B133" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+      <c r="H133" s="9"/>
+      <c r="I133" s="9"/>
+      <c r="J133" s="9"/>
+      <c r="K133" s="9"/>
+      <c r="L133" s="9"/>
+      <c r="M133" s="9"/>
+      <c r="N133" s="9"/>
+      <c r="O133" s="9"/>
+      <c r="P133" s="9"/>
+      <c r="Q133" s="9"/>
+      <c r="R133" s="9"/>
+      <c r="S133" s="9"/>
+      <c r="W133" s="9" t="s">
+        <v>514</v>
+      </c>
+      <c r="X133" s="9"/>
+      <c r="Y133" s="9"/>
+      <c r="Z133" s="9"/>
+      <c r="AA133" s="9"/>
+      <c r="AB133" s="9"/>
+      <c r="AC133" s="9"/>
+      <c r="AD133" s="9"/>
+      <c r="AE133" s="9"/>
+      <c r="AF133" s="9"/>
+      <c r="AG133" s="9"/>
+      <c r="AH133" s="9"/>
+      <c r="AI133" s="9"/>
+      <c r="AJ133" s="9"/>
+      <c r="AK133" s="9"/>
+      <c r="AL133" s="9"/>
+      <c r="AQ133" s="9"/>
+      <c r="AR133" s="9"/>
+      <c r="AS133" s="9"/>
+      <c r="AT133" s="9"/>
+      <c r="AU133" s="9"/>
+      <c r="AV133" s="9"/>
+      <c r="AW133" s="9"/>
+      <c r="AX133" s="9"/>
+      <c r="AY133" s="9"/>
+      <c r="AZ133" s="9"/>
+      <c r="BA133" s="9"/>
+      <c r="BB133" s="9"/>
+      <c r="BC133" s="9"/>
+      <c r="BD133" s="9"/>
+      <c r="BE133" s="9"/>
+      <c r="BF133" s="9"/>
+      <c r="BG133" s="9"/>
+    </row>
+    <row r="134" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B134" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="9"/>
+      <c r="G134" s="9"/>
+      <c r="H134" s="9"/>
+      <c r="I134" s="9"/>
+      <c r="J134" s="9"/>
+      <c r="K134" s="9"/>
+      <c r="L134" s="9"/>
+      <c r="M134" s="9"/>
+      <c r="N134" s="9"/>
+      <c r="O134" s="9"/>
+      <c r="P134" s="9"/>
+      <c r="Q134" s="9"/>
+      <c r="R134" s="9"/>
+      <c r="S134" s="9"/>
+      <c r="W134" s="9"/>
+      <c r="X134" s="9"/>
+      <c r="Y134" s="9"/>
+      <c r="Z134" s="9"/>
+      <c r="AA134" s="9"/>
+      <c r="AB134" s="9"/>
+      <c r="AC134" s="9"/>
+      <c r="AD134" s="9"/>
+      <c r="AE134" s="9"/>
+      <c r="AF134" s="9"/>
+      <c r="AG134" s="9"/>
+      <c r="AH134" s="9"/>
+      <c r="AI134" s="9"/>
+      <c r="AJ134" s="9"/>
+      <c r="AK134" s="9"/>
+      <c r="AL134" s="9"/>
+      <c r="AQ134" s="9"/>
+      <c r="AR134" s="9"/>
+      <c r="AS134" s="9"/>
+      <c r="AT134" s="9"/>
+      <c r="AU134" s="9"/>
+      <c r="AV134" s="9"/>
+      <c r="AW134" s="9"/>
+      <c r="AX134" s="9"/>
+      <c r="AY134" s="9"/>
+      <c r="AZ134" s="9"/>
+      <c r="BA134" s="9"/>
+      <c r="BB134" s="9"/>
+      <c r="BC134" s="9"/>
+      <c r="BD134" s="9"/>
+      <c r="BE134" s="9"/>
+      <c r="BF134" s="9"/>
+      <c r="BG134" s="9"/>
+    </row>
+    <row r="135" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B135" s="9" t="s">
+        <v>499</v>
+      </c>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="9"/>
+      <c r="G135" s="9"/>
+      <c r="H135" s="9"/>
+      <c r="I135" s="9"/>
+      <c r="J135" s="9"/>
+      <c r="K135" s="9"/>
+      <c r="L135" s="9"/>
+      <c r="M135" s="9"/>
+      <c r="N135" s="9"/>
+      <c r="O135" s="9"/>
+      <c r="P135" s="9"/>
+      <c r="Q135" s="9"/>
+      <c r="R135" s="9"/>
+      <c r="S135" s="9"/>
+      <c r="W135" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="X135" s="9"/>
+      <c r="Y135" s="9"/>
+      <c r="Z135" s="9"/>
+      <c r="AA135" s="9"/>
+      <c r="AB135" s="9"/>
+      <c r="AC135" s="9"/>
+      <c r="AD135" s="9"/>
+      <c r="AE135" s="9"/>
+      <c r="AF135" s="9"/>
+      <c r="AG135" s="9"/>
+      <c r="AH135" s="9"/>
+      <c r="AI135" s="9"/>
+      <c r="AJ135" s="9"/>
+      <c r="AK135" s="9"/>
+      <c r="AL135" s="9"/>
+      <c r="AQ135" s="9"/>
+      <c r="AR135" s="9"/>
+      <c r="AS135" s="9"/>
+      <c r="AT135" s="9"/>
+      <c r="AU135" s="9"/>
+      <c r="AV135" s="9"/>
+      <c r="AW135" s="9"/>
+      <c r="AX135" s="9"/>
+      <c r="AY135" s="9"/>
+      <c r="AZ135" s="9"/>
+      <c r="BA135" s="9"/>
+      <c r="BB135" s="9"/>
+      <c r="BC135" s="9"/>
+      <c r="BD135" s="9"/>
+      <c r="BE135" s="9"/>
+      <c r="BF135" s="9"/>
+      <c r="BG135" s="9"/>
+    </row>
+    <row r="136" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B136" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="C136" s="9"/>
+      <c r="D136" s="9"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="9"/>
+      <c r="G136" s="9"/>
+      <c r="H136" s="9"/>
+      <c r="I136" s="9"/>
+      <c r="J136" s="9"/>
+      <c r="K136" s="9"/>
+      <c r="L136" s="9"/>
+      <c r="M136" s="9"/>
+      <c r="N136" s="9"/>
+      <c r="O136" s="9"/>
+      <c r="P136" s="9"/>
+      <c r="Q136" s="9"/>
+      <c r="R136" s="9"/>
+      <c r="S136" s="9"/>
+      <c r="W136" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="X136" s="9"/>
+      <c r="Y136" s="9"/>
+      <c r="Z136" s="9"/>
+      <c r="AA136" s="9"/>
+      <c r="AB136" s="9"/>
+      <c r="AC136" s="9"/>
+      <c r="AD136" s="9"/>
+      <c r="AE136" s="9"/>
+      <c r="AF136" s="9"/>
+      <c r="AG136" s="9"/>
+      <c r="AH136" s="9"/>
+      <c r="AI136" s="9"/>
+      <c r="AJ136" s="9"/>
+      <c r="AK136" s="9"/>
+      <c r="AL136" s="9"/>
+      <c r="AQ136" s="9"/>
+      <c r="AR136" s="9"/>
+      <c r="AS136" s="9"/>
+      <c r="AT136" s="9"/>
+      <c r="AU136" s="9"/>
+      <c r="AV136" s="9"/>
+      <c r="AW136" s="9"/>
+      <c r="AX136" s="9"/>
+      <c r="AY136" s="9"/>
+      <c r="AZ136" s="9"/>
+      <c r="BA136" s="9"/>
+      <c r="BB136" s="9"/>
+      <c r="BC136" s="9"/>
+      <c r="BD136" s="9"/>
+      <c r="BE136" s="9"/>
+      <c r="BF136" s="9"/>
+      <c r="BG136" s="9"/>
+    </row>
+    <row r="137" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B137" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="C137" s="9"/>
+      <c r="D137" s="9"/>
+      <c r="E137" s="9"/>
+      <c r="F137" s="9"/>
+      <c r="G137" s="9"/>
+      <c r="H137" s="9"/>
+      <c r="I137" s="9"/>
+      <c r="J137" s="9"/>
+      <c r="K137" s="9"/>
+      <c r="L137" s="9"/>
+      <c r="M137" s="9"/>
+      <c r="N137" s="9"/>
+      <c r="O137" s="9"/>
+      <c r="P137" s="9"/>
+      <c r="Q137" s="9"/>
+      <c r="R137" s="9"/>
+      <c r="S137" s="9"/>
+      <c r="W137" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="X137" s="9"/>
+      <c r="Y137" s="9"/>
+      <c r="Z137" s="9"/>
+      <c r="AA137" s="9"/>
+      <c r="AB137" s="9"/>
+      <c r="AC137" s="9"/>
+      <c r="AD137" s="9"/>
+      <c r="AE137" s="9"/>
+      <c r="AF137" s="9"/>
+      <c r="AG137" s="9"/>
+      <c r="AH137" s="9"/>
+      <c r="AI137" s="9"/>
+      <c r="AJ137" s="9"/>
+      <c r="AK137" s="9"/>
+      <c r="AL137" s="9"/>
+      <c r="AQ137" s="9" t="s">
+        <v>531</v>
+      </c>
+      <c r="AR137" s="9"/>
+      <c r="AS137" s="9"/>
+      <c r="AT137" s="9"/>
+      <c r="AU137" s="9"/>
+      <c r="AV137" s="9"/>
+      <c r="AW137" s="9"/>
+      <c r="AX137" s="9"/>
+      <c r="AY137" s="9"/>
+      <c r="AZ137" s="9"/>
+      <c r="BA137" s="9"/>
+      <c r="BB137" s="9"/>
+      <c r="BC137" s="9"/>
+      <c r="BD137" s="9"/>
+      <c r="BE137" s="9"/>
+      <c r="BF137" s="9"/>
+      <c r="BG137" s="9"/>
+    </row>
+    <row r="138" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B138" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="C138" s="9"/>
+      <c r="D138" s="9"/>
+      <c r="E138" s="9"/>
+      <c r="F138" s="9"/>
+      <c r="G138" s="9"/>
+      <c r="H138" s="9"/>
+      <c r="I138" s="9"/>
+      <c r="J138" s="9"/>
+      <c r="K138" s="9"/>
+      <c r="L138" s="9"/>
+      <c r="M138" s="9"/>
+      <c r="N138" s="9"/>
+      <c r="O138" s="9"/>
+      <c r="P138" s="9"/>
+      <c r="Q138" s="9"/>
+      <c r="R138" s="9"/>
+      <c r="S138" s="9"/>
+      <c r="W138" s="9" t="s">
+        <v>516</v>
+      </c>
+      <c r="X138" s="9"/>
+      <c r="Y138" s="9"/>
+      <c r="Z138" s="9"/>
+      <c r="AA138" s="9"/>
+      <c r="AB138" s="9"/>
+      <c r="AC138" s="9"/>
+      <c r="AD138" s="9"/>
+      <c r="AE138" s="9"/>
+      <c r="AF138" s="9"/>
+      <c r="AG138" s="9"/>
+      <c r="AH138" s="9"/>
+      <c r="AI138" s="9"/>
+      <c r="AJ138" s="9"/>
+      <c r="AK138" s="9"/>
+      <c r="AL138" s="9"/>
+      <c r="AQ138" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="AR138" s="9"/>
+      <c r="AS138" s="9"/>
+      <c r="AT138" s="9"/>
+      <c r="AU138" s="9"/>
+      <c r="AV138" s="9"/>
+      <c r="AW138" s="9"/>
+      <c r="AX138" s="9"/>
+      <c r="AY138" s="9"/>
+      <c r="AZ138" s="9"/>
+      <c r="BA138" s="9"/>
+      <c r="BB138" s="9"/>
+      <c r="BC138" s="9"/>
+      <c r="BD138" s="9"/>
+      <c r="BE138" s="9"/>
+      <c r="BF138" s="9"/>
+      <c r="BG138" s="9"/>
+    </row>
+    <row r="139" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B139" s="9" t="s">
+        <v>503</v>
+      </c>
+      <c r="C139" s="9"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="9"/>
+      <c r="F139" s="9"/>
+      <c r="G139" s="9"/>
+      <c r="H139" s="9"/>
+      <c r="I139" s="9"/>
+      <c r="J139" s="9"/>
+      <c r="K139" s="9"/>
+      <c r="L139" s="9"/>
+      <c r="M139" s="9"/>
+      <c r="N139" s="9"/>
+      <c r="O139" s="9"/>
+      <c r="P139" s="9"/>
+      <c r="Q139" s="9"/>
+      <c r="R139" s="9"/>
+      <c r="S139" s="9"/>
+      <c r="W139" s="9"/>
+      <c r="X139" s="9"/>
+      <c r="Y139" s="9"/>
+      <c r="Z139" s="9"/>
+      <c r="AA139" s="9"/>
+      <c r="AB139" s="9"/>
+      <c r="AC139" s="9"/>
+      <c r="AD139" s="9"/>
+      <c r="AE139" s="9"/>
+      <c r="AF139" s="9"/>
+      <c r="AG139" s="9"/>
+      <c r="AH139" s="9"/>
+      <c r="AI139" s="9"/>
+      <c r="AJ139" s="9"/>
+      <c r="AK139" s="9"/>
+      <c r="AL139" s="9"/>
+      <c r="AQ139" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="AR139" s="9"/>
+      <c r="AS139" s="9"/>
+      <c r="AT139" s="9"/>
+      <c r="AU139" s="9"/>
+      <c r="AV139" s="9"/>
+      <c r="AW139" s="9"/>
+      <c r="AX139" s="9"/>
+      <c r="AY139" s="9"/>
+      <c r="AZ139" s="9"/>
+      <c r="BA139" s="9"/>
+      <c r="BB139" s="9"/>
+      <c r="BC139" s="9"/>
+      <c r="BD139" s="9"/>
+      <c r="BE139" s="9"/>
+      <c r="BF139" s="9"/>
+      <c r="BG139" s="9"/>
+    </row>
+    <row r="140" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B140" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C140" s="9"/>
+      <c r="D140" s="9"/>
+      <c r="E140" s="9"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="9"/>
+      <c r="H140" s="9"/>
+      <c r="I140" s="9"/>
+      <c r="J140" s="9"/>
+      <c r="K140" s="9"/>
+      <c r="L140" s="9"/>
+      <c r="M140" s="9"/>
+      <c r="N140" s="9"/>
+      <c r="O140" s="9"/>
+      <c r="P140" s="9"/>
+      <c r="Q140" s="9"/>
+      <c r="R140" s="9"/>
+      <c r="S140" s="9"/>
+      <c r="W140" s="9"/>
+      <c r="X140" s="9"/>
+      <c r="Y140" s="9"/>
+      <c r="Z140" s="9"/>
+      <c r="AA140" s="9"/>
+      <c r="AB140" s="9"/>
+      <c r="AC140" s="9"/>
+      <c r="AD140" s="9"/>
+      <c r="AE140" s="9"/>
+      <c r="AF140" s="9"/>
+      <c r="AG140" s="9"/>
+      <c r="AH140" s="9"/>
+      <c r="AI140" s="9"/>
+      <c r="AJ140" s="9"/>
+      <c r="AK140" s="9"/>
+      <c r="AL140" s="9"/>
+      <c r="AQ140" s="9"/>
+      <c r="AR140" s="9"/>
+      <c r="AS140" s="9"/>
+      <c r="AT140" s="9"/>
+      <c r="AU140" s="9"/>
+      <c r="AV140" s="9"/>
+      <c r="AW140" s="9"/>
+      <c r="AX140" s="9"/>
+      <c r="AY140" s="9"/>
+      <c r="AZ140" s="9"/>
+      <c r="BA140" s="9"/>
+      <c r="BB140" s="9"/>
+      <c r="BC140" s="9"/>
+      <c r="BD140" s="9"/>
+      <c r="BE140" s="9"/>
+      <c r="BF140" s="9"/>
+      <c r="BG140" s="9"/>
+    </row>
+    <row r="141" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B141" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="9"/>
+      <c r="H141" s="9"/>
+      <c r="I141" s="9"/>
+      <c r="J141" s="9"/>
+      <c r="K141" s="9"/>
+      <c r="L141" s="9"/>
+      <c r="M141" s="9"/>
+      <c r="N141" s="9"/>
+      <c r="O141" s="9"/>
+      <c r="P141" s="9"/>
+      <c r="Q141" s="9"/>
+      <c r="R141" s="9"/>
+      <c r="S141" s="9"/>
+      <c r="W141" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="X141" s="9"/>
+      <c r="Y141" s="9"/>
+      <c r="Z141" s="9"/>
+      <c r="AA141" s="9"/>
+      <c r="AB141" s="9"/>
+      <c r="AC141" s="9"/>
+      <c r="AD141" s="9"/>
+      <c r="AE141" s="9"/>
+      <c r="AF141" s="9"/>
+      <c r="AG141" s="9"/>
+      <c r="AH141" s="9"/>
+      <c r="AI141" s="9"/>
+      <c r="AJ141" s="9"/>
+      <c r="AK141" s="9"/>
+      <c r="AL141" s="9"/>
+      <c r="AQ141" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="AR141" s="9"/>
+      <c r="AS141" s="9"/>
+      <c r="AT141" s="9"/>
+      <c r="AU141" s="9"/>
+      <c r="AV141" s="9"/>
+      <c r="AW141" s="9"/>
+      <c r="AX141" s="9"/>
+      <c r="AY141" s="9"/>
+      <c r="AZ141" s="9"/>
+      <c r="BA141" s="9"/>
+      <c r="BB141" s="9"/>
+      <c r="BC141" s="9"/>
+      <c r="BD141" s="9"/>
+      <c r="BE141" s="9"/>
+      <c r="BF141" s="9"/>
+      <c r="BG141" s="9"/>
+    </row>
+    <row r="142" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B142" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="C142" s="9"/>
+      <c r="D142" s="9"/>
+      <c r="E142" s="9"/>
+      <c r="F142" s="9"/>
+      <c r="G142" s="9"/>
+      <c r="H142" s="9"/>
+      <c r="I142" s="9"/>
+      <c r="J142" s="9"/>
+      <c r="K142" s="9"/>
+      <c r="L142" s="9"/>
+      <c r="M142" s="9"/>
+      <c r="N142" s="9"/>
+      <c r="O142" s="9"/>
+      <c r="P142" s="9"/>
+      <c r="Q142" s="9"/>
+      <c r="R142" s="9"/>
+      <c r="S142" s="9"/>
+      <c r="W142" s="9" t="s">
+        <v>518</v>
+      </c>
+      <c r="X142" s="9"/>
+      <c r="Y142" s="9"/>
+      <c r="Z142" s="9"/>
+      <c r="AA142" s="9"/>
+      <c r="AB142" s="9"/>
+      <c r="AC142" s="9"/>
+      <c r="AD142" s="9"/>
+      <c r="AE142" s="9"/>
+      <c r="AF142" s="9"/>
+      <c r="AG142" s="9"/>
+      <c r="AH142" s="9"/>
+      <c r="AI142" s="9"/>
+      <c r="AJ142" s="9"/>
+      <c r="AK142" s="9"/>
+      <c r="AL142" s="9"/>
+      <c r="AQ142" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="AR142" s="9"/>
+      <c r="AS142" s="9"/>
+      <c r="AT142" s="9"/>
+      <c r="AU142" s="9"/>
+      <c r="AV142" s="9"/>
+      <c r="AW142" s="9"/>
+      <c r="AX142" s="9"/>
+      <c r="AY142" s="9"/>
+      <c r="AZ142" s="9"/>
+      <c r="BA142" s="9"/>
+      <c r="BB142" s="9"/>
+      <c r="BC142" s="9"/>
+      <c r="BD142" s="9"/>
+      <c r="BE142" s="9"/>
+      <c r="BF142" s="9"/>
+      <c r="BG142" s="9"/>
+    </row>
+    <row r="143" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B143" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="C143" s="9"/>
+      <c r="D143" s="9"/>
+      <c r="E143" s="9"/>
+      <c r="F143" s="9"/>
+      <c r="G143" s="9"/>
+      <c r="H143" s="9"/>
+      <c r="I143" s="9"/>
+      <c r="J143" s="9"/>
+      <c r="K143" s="9"/>
+      <c r="L143" s="9"/>
+      <c r="M143" s="9"/>
+      <c r="N143" s="9"/>
+      <c r="O143" s="9"/>
+      <c r="P143" s="9"/>
+      <c r="Q143" s="9"/>
+      <c r="R143" s="9"/>
+      <c r="S143" s="9"/>
+      <c r="W143" s="9" t="s">
+        <v>519</v>
+      </c>
+      <c r="X143" s="9"/>
+      <c r="Y143" s="9"/>
+      <c r="Z143" s="9"/>
+      <c r="AA143" s="9"/>
+      <c r="AB143" s="9"/>
+      <c r="AC143" s="9"/>
+      <c r="AD143" s="9"/>
+      <c r="AE143" s="9"/>
+      <c r="AF143" s="9"/>
+      <c r="AG143" s="9"/>
+      <c r="AH143" s="9"/>
+      <c r="AI143" s="9"/>
+      <c r="AJ143" s="9"/>
+      <c r="AK143" s="9"/>
+      <c r="AL143" s="9"/>
+      <c r="AQ143" s="9" t="s">
+        <v>536</v>
+      </c>
+      <c r="AR143" s="9"/>
+      <c r="AS143" s="9"/>
+      <c r="AT143" s="9"/>
+      <c r="AU143" s="9"/>
+      <c r="AV143" s="9"/>
+      <c r="AW143" s="9"/>
+      <c r="AX143" s="9"/>
+      <c r="AY143" s="9"/>
+      <c r="AZ143" s="9"/>
+      <c r="BA143" s="9"/>
+      <c r="BB143" s="9"/>
+      <c r="BC143" s="9"/>
+      <c r="BD143" s="9"/>
+      <c r="BE143" s="9"/>
+      <c r="BF143" s="9"/>
+      <c r="BG143" s="9"/>
+    </row>
+    <row r="144" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B144" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="C144" s="9"/>
+      <c r="D144" s="9"/>
+      <c r="E144" s="9"/>
+      <c r="F144" s="9"/>
+      <c r="G144" s="9"/>
+      <c r="H144" s="9"/>
+      <c r="I144" s="9"/>
+      <c r="J144" s="9"/>
+      <c r="K144" s="9"/>
+      <c r="L144" s="9"/>
+      <c r="M144" s="9"/>
+      <c r="N144" s="9"/>
+      <c r="O144" s="9"/>
+      <c r="P144" s="9"/>
+      <c r="Q144" s="9"/>
+      <c r="R144" s="9"/>
+      <c r="S144" s="9"/>
+      <c r="W144" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="X144" s="9"/>
+      <c r="Y144" s="9"/>
+      <c r="Z144" s="9"/>
+      <c r="AA144" s="9"/>
+      <c r="AB144" s="9"/>
+      <c r="AC144" s="9"/>
+      <c r="AD144" s="9"/>
+      <c r="AE144" s="9"/>
+      <c r="AF144" s="9"/>
+      <c r="AG144" s="9"/>
+      <c r="AH144" s="9"/>
+      <c r="AI144" s="9"/>
+      <c r="AJ144" s="9"/>
+      <c r="AK144" s="9"/>
+      <c r="AL144" s="9"/>
+      <c r="AQ144" s="9" t="s">
+        <v>527</v>
+      </c>
+      <c r="AR144" s="9"/>
+      <c r="AS144" s="9"/>
+      <c r="AT144" s="9"/>
+      <c r="AU144" s="9"/>
+      <c r="AV144" s="9"/>
+      <c r="AW144" s="9"/>
+      <c r="AX144" s="9"/>
+      <c r="AY144" s="9"/>
+      <c r="AZ144" s="9"/>
+      <c r="BA144" s="9"/>
+      <c r="BB144" s="9"/>
+      <c r="BC144" s="9"/>
+      <c r="BD144" s="9"/>
+      <c r="BE144" s="9"/>
+      <c r="BF144" s="9"/>
+      <c r="BG144" s="9"/>
+    </row>
+    <row r="145" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B145" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="C145" s="9"/>
+      <c r="D145" s="9"/>
+      <c r="E145" s="9"/>
+      <c r="F145" s="9"/>
+      <c r="G145" s="9"/>
+      <c r="H145" s="9"/>
+      <c r="I145" s="9"/>
+      <c r="J145" s="9"/>
+      <c r="K145" s="9"/>
+      <c r="L145" s="9"/>
+      <c r="M145" s="9"/>
+      <c r="N145" s="9"/>
+      <c r="O145" s="9"/>
+      <c r="P145" s="9"/>
+      <c r="Q145" s="9"/>
+      <c r="R145" s="9"/>
+      <c r="S145" s="9"/>
+      <c r="W145" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="X145" s="9"/>
+      <c r="Y145" s="9"/>
+      <c r="Z145" s="9"/>
+      <c r="AA145" s="9"/>
+      <c r="AB145" s="9"/>
+      <c r="AC145" s="9"/>
+      <c r="AD145" s="9"/>
+      <c r="AE145" s="9"/>
+      <c r="AF145" s="9"/>
+      <c r="AG145" s="9"/>
+      <c r="AH145" s="9"/>
+      <c r="AI145" s="9"/>
+      <c r="AJ145" s="9"/>
+      <c r="AK145" s="9"/>
+      <c r="AL145" s="9"/>
+      <c r="AQ145" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="AR145" s="9"/>
+      <c r="AS145" s="9"/>
+      <c r="AT145" s="9"/>
+      <c r="AU145" s="9"/>
+      <c r="AV145" s="9"/>
+      <c r="AW145" s="9"/>
+      <c r="AX145" s="9"/>
+      <c r="AY145" s="9"/>
+      <c r="AZ145" s="9"/>
+      <c r="BA145" s="9"/>
+      <c r="BB145" s="9"/>
+      <c r="BC145" s="9"/>
+      <c r="BD145" s="9"/>
+      <c r="BE145" s="9"/>
+      <c r="BF145" s="9"/>
+      <c r="BG145" s="9"/>
+    </row>
+    <row r="146" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B146" s="9" t="s">
+        <v>507</v>
+      </c>
+      <c r="C146" s="9"/>
+      <c r="D146" s="9"/>
+      <c r="E146" s="9"/>
+      <c r="F146" s="9"/>
+      <c r="G146" s="9"/>
+      <c r="H146" s="9"/>
+      <c r="I146" s="9"/>
+      <c r="J146" s="9"/>
+      <c r="K146" s="9"/>
+      <c r="L146" s="9"/>
+      <c r="M146" s="9"/>
+      <c r="N146" s="9"/>
+      <c r="O146" s="9"/>
+      <c r="P146" s="9"/>
+      <c r="Q146" s="9"/>
+      <c r="R146" s="9"/>
+      <c r="S146" s="9"/>
+      <c r="W146" s="9"/>
+      <c r="X146" s="9"/>
+      <c r="Y146" s="9"/>
+      <c r="Z146" s="9"/>
+      <c r="AA146" s="9"/>
+      <c r="AB146" s="9"/>
+      <c r="AC146" s="9"/>
+      <c r="AD146" s="9"/>
+      <c r="AE146" s="9"/>
+      <c r="AF146" s="9"/>
+      <c r="AG146" s="9"/>
+      <c r="AH146" s="9"/>
+      <c r="AI146" s="9"/>
+      <c r="AJ146" s="9"/>
+      <c r="AK146" s="9"/>
+      <c r="AL146" s="9"/>
+      <c r="AQ146" s="9"/>
+      <c r="AR146" s="9"/>
+      <c r="AS146" s="9"/>
+      <c r="AT146" s="9"/>
+      <c r="AU146" s="9"/>
+      <c r="AV146" s="9"/>
+      <c r="AW146" s="9"/>
+      <c r="AX146" s="9"/>
+      <c r="AY146" s="9"/>
+      <c r="AZ146" s="9"/>
+      <c r="BA146" s="9"/>
+      <c r="BB146" s="9"/>
+      <c r="BC146" s="9"/>
+      <c r="BD146" s="9"/>
+      <c r="BE146" s="9"/>
+      <c r="BF146" s="9"/>
+      <c r="BG146" s="9"/>
+    </row>
+    <row r="147" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B147" s="9" t="s">
+        <v>508</v>
+      </c>
+      <c r="C147" s="9"/>
+      <c r="D147" s="9"/>
+      <c r="E147" s="9"/>
+      <c r="F147" s="9"/>
+      <c r="G147" s="9"/>
+      <c r="H147" s="9"/>
+      <c r="I147" s="9"/>
+      <c r="J147" s="9"/>
+      <c r="K147" s="9"/>
+      <c r="L147" s="9"/>
+      <c r="M147" s="9"/>
+      <c r="N147" s="9"/>
+      <c r="O147" s="9"/>
+      <c r="P147" s="9"/>
+      <c r="Q147" s="9"/>
+      <c r="R147" s="9"/>
+      <c r="S147" s="9"/>
+      <c r="W147" s="9" t="s">
+        <v>521</v>
+      </c>
+      <c r="X147" s="9"/>
+      <c r="Y147" s="9"/>
+      <c r="Z147" s="9"/>
+      <c r="AA147" s="9"/>
+      <c r="AB147" s="9"/>
+      <c r="AC147" s="9"/>
+      <c r="AD147" s="9"/>
+      <c r="AE147" s="9"/>
+      <c r="AF147" s="9"/>
+      <c r="AG147" s="9"/>
+      <c r="AH147" s="9"/>
+      <c r="AI147" s="9"/>
+      <c r="AJ147" s="9"/>
+      <c r="AK147" s="9"/>
+      <c r="AL147" s="9"/>
+      <c r="AQ147" s="9" t="s">
+        <v>537</v>
+      </c>
+      <c r="AR147" s="9"/>
+      <c r="AS147" s="9"/>
+      <c r="AT147" s="9"/>
+      <c r="AU147" s="9"/>
+      <c r="AV147" s="9"/>
+      <c r="AW147" s="9"/>
+      <c r="AX147" s="9"/>
+      <c r="AY147" s="9"/>
+      <c r="AZ147" s="9"/>
+      <c r="BA147" s="9"/>
+      <c r="BB147" s="9"/>
+      <c r="BC147" s="9"/>
+      <c r="BD147" s="9"/>
+      <c r="BE147" s="9"/>
+      <c r="BF147" s="9"/>
+      <c r="BG147" s="9"/>
+    </row>
+    <row r="148" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B148" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="C148" s="9"/>
+      <c r="D148" s="9"/>
+      <c r="E148" s="9"/>
+      <c r="F148" s="9"/>
+      <c r="G148" s="9"/>
+      <c r="H148" s="9"/>
+      <c r="I148" s="9"/>
+      <c r="J148" s="9"/>
+      <c r="K148" s="9"/>
+      <c r="L148" s="9"/>
+      <c r="M148" s="9"/>
+      <c r="N148" s="9"/>
+      <c r="O148" s="9"/>
+      <c r="P148" s="9"/>
+      <c r="Q148" s="9"/>
+      <c r="R148" s="9"/>
+      <c r="S148" s="9"/>
+      <c r="W148" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="X148" s="9"/>
+      <c r="Y148" s="9"/>
+      <c r="Z148" s="9"/>
+      <c r="AA148" s="9"/>
+      <c r="AB148" s="9"/>
+      <c r="AC148" s="9"/>
+      <c r="AD148" s="9"/>
+      <c r="AE148" s="9"/>
+      <c r="AF148" s="9"/>
+      <c r="AG148" s="9"/>
+      <c r="AH148" s="9"/>
+      <c r="AI148" s="9"/>
+      <c r="AJ148" s="9"/>
+      <c r="AK148" s="9"/>
+      <c r="AL148" s="9"/>
+      <c r="AQ148" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="AR148" s="9"/>
+      <c r="AS148" s="9"/>
+      <c r="AT148" s="9"/>
+      <c r="AU148" s="9"/>
+      <c r="AV148" s="9"/>
+      <c r="AW148" s="9"/>
+      <c r="AX148" s="9"/>
+      <c r="AY148" s="9"/>
+      <c r="AZ148" s="9"/>
+      <c r="BA148" s="9"/>
+      <c r="BB148" s="9"/>
+      <c r="BC148" s="9"/>
+      <c r="BD148" s="9"/>
+      <c r="BE148" s="9"/>
+      <c r="BF148" s="9"/>
+      <c r="BG148" s="9"/>
+    </row>
+    <row r="149" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B149" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+      <c r="E149" s="9"/>
+      <c r="F149" s="9"/>
+      <c r="G149" s="9"/>
+      <c r="H149" s="9"/>
+      <c r="I149" s="9"/>
+      <c r="J149" s="9"/>
+      <c r="K149" s="9"/>
+      <c r="L149" s="9"/>
+      <c r="M149" s="9"/>
+      <c r="N149" s="9"/>
+      <c r="O149" s="9"/>
+      <c r="P149" s="9"/>
+      <c r="Q149" s="9"/>
+      <c r="R149" s="9"/>
+      <c r="S149" s="9"/>
+      <c r="W149" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="X149" s="9"/>
+      <c r="Y149" s="9"/>
+      <c r="Z149" s="9"/>
+      <c r="AA149" s="9"/>
+      <c r="AB149" s="9"/>
+      <c r="AC149" s="9"/>
+      <c r="AD149" s="9"/>
+      <c r="AE149" s="9"/>
+      <c r="AF149" s="9"/>
+      <c r="AG149" s="9"/>
+      <c r="AH149" s="9"/>
+      <c r="AI149" s="9"/>
+      <c r="AJ149" s="9"/>
+      <c r="AK149" s="9"/>
+      <c r="AL149" s="9"/>
+      <c r="AQ149" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="AR149" s="9"/>
+      <c r="AS149" s="9"/>
+      <c r="AT149" s="9"/>
+      <c r="AU149" s="9"/>
+      <c r="AV149" s="9"/>
+      <c r="AW149" s="9"/>
+      <c r="AX149" s="9"/>
+      <c r="AY149" s="9"/>
+      <c r="AZ149" s="9"/>
+      <c r="BA149" s="9"/>
+      <c r="BB149" s="9"/>
+      <c r="BC149" s="9"/>
+      <c r="BD149" s="9"/>
+      <c r="BE149" s="9"/>
+      <c r="BF149" s="9"/>
+      <c r="BG149" s="9"/>
+    </row>
+    <row r="150" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B150" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C150" s="9"/>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
+      <c r="G150" s="9"/>
+      <c r="H150" s="9"/>
+      <c r="I150" s="9"/>
+      <c r="J150" s="9"/>
+      <c r="K150" s="9"/>
+      <c r="L150" s="9"/>
+      <c r="M150" s="9"/>
+      <c r="N150" s="9"/>
+      <c r="O150" s="9"/>
+      <c r="P150" s="9"/>
+      <c r="Q150" s="9"/>
+      <c r="R150" s="9"/>
+      <c r="S150" s="9"/>
+      <c r="W150" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="X150" s="9"/>
+      <c r="Y150" s="9"/>
+      <c r="Z150" s="9"/>
+      <c r="AA150" s="9"/>
+      <c r="AB150" s="9"/>
+      <c r="AC150" s="9"/>
+      <c r="AD150" s="9"/>
+      <c r="AE150" s="9"/>
+      <c r="AF150" s="9"/>
+      <c r="AG150" s="9"/>
+      <c r="AH150" s="9"/>
+      <c r="AI150" s="9"/>
+      <c r="AJ150" s="9"/>
+      <c r="AK150" s="9"/>
+      <c r="AL150" s="9"/>
+      <c r="AQ150" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="AR150" s="9"/>
+      <c r="AS150" s="9"/>
+      <c r="AT150" s="9"/>
+      <c r="AU150" s="9"/>
+      <c r="AV150" s="9"/>
+      <c r="AW150" s="9"/>
+      <c r="AX150" s="9"/>
+      <c r="AY150" s="9"/>
+      <c r="AZ150" s="9"/>
+      <c r="BA150" s="9"/>
+      <c r="BB150" s="9"/>
+      <c r="BC150" s="9"/>
+      <c r="BD150" s="9"/>
+      <c r="BE150" s="9"/>
+      <c r="BF150" s="9"/>
+      <c r="BG150" s="9"/>
+    </row>
+    <row r="151" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="B151" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C151" s="9"/>
+      <c r="D151" s="9"/>
+      <c r="E151" s="9"/>
+      <c r="F151" s="9"/>
+      <c r="G151" s="9"/>
+      <c r="H151" s="9"/>
+      <c r="I151" s="9"/>
+      <c r="J151" s="9"/>
+      <c r="K151" s="9"/>
+      <c r="L151" s="9"/>
+      <c r="M151" s="9"/>
+      <c r="N151" s="9"/>
+      <c r="O151" s="9"/>
+      <c r="P151" s="9"/>
+      <c r="Q151" s="9"/>
+      <c r="R151" s="9"/>
+      <c r="S151" s="9"/>
+      <c r="W151" s="9"/>
+      <c r="X151" s="9"/>
+      <c r="Y151" s="9"/>
+      <c r="Z151" s="9"/>
+      <c r="AA151" s="9"/>
+      <c r="AB151" s="9"/>
+      <c r="AC151" s="9"/>
+      <c r="AD151" s="9"/>
+      <c r="AE151" s="9"/>
+      <c r="AF151" s="9"/>
+      <c r="AG151" s="9"/>
+      <c r="AH151" s="9"/>
+      <c r="AI151" s="9"/>
+      <c r="AJ151" s="9"/>
+      <c r="AK151" s="9"/>
+      <c r="AL151" s="9"/>
+      <c r="AQ151" s="9"/>
+      <c r="AR151" s="9"/>
+      <c r="AS151" s="9"/>
+      <c r="AT151" s="9"/>
+      <c r="AU151" s="9"/>
+      <c r="AV151" s="9"/>
+      <c r="AW151" s="9"/>
+      <c r="AX151" s="9"/>
+      <c r="AY151" s="9"/>
+      <c r="AZ151" s="9"/>
+      <c r="BA151" s="9"/>
+      <c r="BB151" s="9"/>
+      <c r="BC151" s="9"/>
+      <c r="BD151" s="9"/>
+      <c r="BE151" s="9"/>
+      <c r="BF151" s="9"/>
+      <c r="BG151" s="9"/>
+    </row>
+    <row r="152" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="W152" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="X152" s="9"/>
+      <c r="Y152" s="9"/>
+      <c r="Z152" s="9"/>
+      <c r="AA152" s="9"/>
+      <c r="AB152" s="9"/>
+      <c r="AC152" s="9"/>
+      <c r="AD152" s="9"/>
+      <c r="AE152" s="9"/>
+      <c r="AF152" s="9"/>
+      <c r="AG152" s="9"/>
+      <c r="AH152" s="9"/>
+      <c r="AI152" s="9"/>
+      <c r="AJ152" s="9"/>
+      <c r="AK152" s="9"/>
+      <c r="AL152" s="9"/>
+      <c r="AQ152" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="AR152" s="9"/>
+      <c r="AS152" s="9"/>
+      <c r="AT152" s="9"/>
+      <c r="AU152" s="9"/>
+      <c r="AV152" s="9"/>
+      <c r="AW152" s="9"/>
+      <c r="AX152" s="9"/>
+      <c r="AY152" s="9"/>
+      <c r="AZ152" s="9"/>
+      <c r="BA152" s="9"/>
+      <c r="BB152" s="9"/>
+      <c r="BC152" s="9"/>
+      <c r="BD152" s="9"/>
+      <c r="BE152" s="9"/>
+      <c r="BF152" s="9"/>
+      <c r="BG152" s="9"/>
+    </row>
+    <row r="153" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="W153" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="X153" s="9"/>
+      <c r="Y153" s="9"/>
+      <c r="Z153" s="9"/>
+      <c r="AA153" s="9"/>
+      <c r="AB153" s="9"/>
+      <c r="AC153" s="9"/>
+      <c r="AD153" s="9"/>
+      <c r="AE153" s="9"/>
+      <c r="AF153" s="9"/>
+      <c r="AG153" s="9"/>
+      <c r="AH153" s="9"/>
+      <c r="AI153" s="9"/>
+      <c r="AJ153" s="9"/>
+      <c r="AK153" s="9"/>
+      <c r="AL153" s="9"/>
+      <c r="AQ153" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="AR153" s="9"/>
+      <c r="AS153" s="9"/>
+      <c r="AT153" s="9"/>
+      <c r="AU153" s="9"/>
+      <c r="AV153" s="9"/>
+      <c r="AW153" s="9"/>
+      <c r="AX153" s="9"/>
+      <c r="AY153" s="9"/>
+      <c r="AZ153" s="9"/>
+      <c r="BA153" s="9"/>
+      <c r="BB153" s="9"/>
+      <c r="BC153" s="9"/>
+      <c r="BD153" s="9"/>
+      <c r="BE153" s="9"/>
+      <c r="BF153" s="9"/>
+      <c r="BG153" s="9"/>
+    </row>
+    <row r="154" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="W154" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="X154" s="9"/>
+      <c r="Y154" s="9"/>
+      <c r="Z154" s="9"/>
+      <c r="AA154" s="9"/>
+      <c r="AB154" s="9"/>
+      <c r="AC154" s="9"/>
+      <c r="AD154" s="9"/>
+      <c r="AE154" s="9"/>
+      <c r="AF154" s="9"/>
+      <c r="AG154" s="9"/>
+      <c r="AH154" s="9"/>
+      <c r="AI154" s="9"/>
+      <c r="AJ154" s="9"/>
+      <c r="AK154" s="9"/>
+      <c r="AL154" s="9"/>
+      <c r="AQ154" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="AR154" s="9"/>
+      <c r="AS154" s="9"/>
+      <c r="AT154" s="9"/>
+      <c r="AU154" s="9"/>
+      <c r="AV154" s="9"/>
+      <c r="AW154" s="9"/>
+      <c r="AX154" s="9"/>
+      <c r="AY154" s="9"/>
+      <c r="AZ154" s="9"/>
+      <c r="BA154" s="9"/>
+      <c r="BB154" s="9"/>
+      <c r="BC154" s="9"/>
+      <c r="BD154" s="9"/>
+      <c r="BE154" s="9"/>
+      <c r="BF154" s="9"/>
+      <c r="BG154" s="9"/>
+    </row>
+    <row r="155" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="W155" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="X155" s="9"/>
+      <c r="Y155" s="9"/>
+      <c r="Z155" s="9"/>
+      <c r="AA155" s="9"/>
+      <c r="AB155" s="9"/>
+      <c r="AC155" s="9"/>
+      <c r="AD155" s="9"/>
+      <c r="AE155" s="9"/>
+      <c r="AF155" s="9"/>
+      <c r="AG155" s="9"/>
+      <c r="AH155" s="9"/>
+      <c r="AI155" s="9"/>
+      <c r="AJ155" s="9"/>
+      <c r="AK155" s="9"/>
+      <c r="AL155" s="9"/>
+      <c r="AQ155" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="AR155" s="9"/>
+      <c r="AS155" s="9"/>
+      <c r="AT155" s="9"/>
+      <c r="AU155" s="9"/>
+      <c r="AV155" s="9"/>
+      <c r="AW155" s="9"/>
+      <c r="AX155" s="9"/>
+      <c r="AY155" s="9"/>
+      <c r="AZ155" s="9"/>
+      <c r="BA155" s="9"/>
+      <c r="BB155" s="9"/>
+      <c r="BC155" s="9"/>
+      <c r="BD155" s="9"/>
+      <c r="BE155" s="9"/>
+      <c r="BF155" s="9"/>
+      <c r="BG155" s="9"/>
+    </row>
+    <row r="156" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="W156" s="9"/>
+      <c r="X156" s="9"/>
+      <c r="Y156" s="9"/>
+      <c r="Z156" s="9"/>
+      <c r="AA156" s="9"/>
+      <c r="AB156" s="9"/>
+      <c r="AC156" s="9"/>
+      <c r="AD156" s="9"/>
+      <c r="AE156" s="9"/>
+      <c r="AF156" s="9"/>
+      <c r="AG156" s="9"/>
+      <c r="AH156" s="9"/>
+      <c r="AI156" s="9"/>
+      <c r="AJ156" s="9"/>
+      <c r="AK156" s="9"/>
+      <c r="AL156" s="9"/>
+      <c r="AQ156" s="9"/>
+      <c r="AR156" s="9"/>
+      <c r="AS156" s="9"/>
+      <c r="AT156" s="9"/>
+      <c r="AU156" s="9"/>
+      <c r="AV156" s="9"/>
+      <c r="AW156" s="9"/>
+      <c r="AX156" s="9"/>
+      <c r="AY156" s="9"/>
+      <c r="AZ156" s="9"/>
+      <c r="BA156" s="9"/>
+      <c r="BB156" s="9"/>
+      <c r="BC156" s="9"/>
+      <c r="BD156" s="9"/>
+      <c r="BE156" s="9"/>
+      <c r="BF156" s="9"/>
+      <c r="BG156" s="9"/>
+    </row>
+    <row r="157" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="W157" s="9" t="s">
+        <v>527</v>
+      </c>
+      <c r="X157" s="9"/>
+      <c r="Y157" s="9"/>
+      <c r="Z157" s="9"/>
+      <c r="AA157" s="9"/>
+      <c r="AB157" s="9"/>
+      <c r="AC157" s="9"/>
+      <c r="AD157" s="9"/>
+      <c r="AE157" s="9"/>
+      <c r="AF157" s="9"/>
+      <c r="AG157" s="9"/>
+      <c r="AH157" s="9"/>
+      <c r="AI157" s="9"/>
+      <c r="AJ157" s="9"/>
+      <c r="AK157" s="9"/>
+      <c r="AL157" s="9"/>
+      <c r="AQ157" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="AR157" s="9"/>
+      <c r="AS157" s="9"/>
+      <c r="AT157" s="9"/>
+      <c r="AU157" s="9"/>
+      <c r="AV157" s="9"/>
+      <c r="AW157" s="9"/>
+      <c r="AX157" s="9"/>
+      <c r="AY157" s="9"/>
+      <c r="AZ157" s="9"/>
+      <c r="BA157" s="9"/>
+      <c r="BB157" s="9"/>
+      <c r="BC157" s="9"/>
+      <c r="BD157" s="9"/>
+      <c r="BE157" s="9"/>
+      <c r="BF157" s="9"/>
+      <c r="BG157" s="9"/>
+    </row>
+    <row r="158" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="W158" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="X158" s="9"/>
+      <c r="Y158" s="9"/>
+      <c r="Z158" s="9"/>
+      <c r="AA158" s="9"/>
+      <c r="AB158" s="9"/>
+      <c r="AC158" s="9"/>
+      <c r="AD158" s="9"/>
+      <c r="AE158" s="9"/>
+      <c r="AF158" s="9"/>
+      <c r="AG158" s="9"/>
+      <c r="AH158" s="9"/>
+      <c r="AI158" s="9"/>
+      <c r="AJ158" s="9"/>
+      <c r="AK158" s="9"/>
+      <c r="AL158" s="9"/>
+      <c r="AQ158" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="AR158" s="9"/>
+      <c r="AS158" s="9"/>
+      <c r="AT158" s="9"/>
+      <c r="AU158" s="9"/>
+      <c r="AV158" s="9"/>
+      <c r="AW158" s="9"/>
+      <c r="AX158" s="9"/>
+      <c r="AY158" s="9"/>
+      <c r="AZ158" s="9"/>
+      <c r="BA158" s="9"/>
+      <c r="BB158" s="9"/>
+      <c r="BC158" s="9"/>
+      <c r="BD158" s="9"/>
+      <c r="BE158" s="9"/>
+      <c r="BF158" s="9"/>
+      <c r="BG158" s="9"/>
+    </row>
+    <row r="159" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="W159" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="X159" s="9"/>
+      <c r="Y159" s="9"/>
+      <c r="Z159" s="9"/>
+      <c r="AA159" s="9"/>
+      <c r="AB159" s="9"/>
+      <c r="AC159" s="9"/>
+      <c r="AD159" s="9"/>
+      <c r="AE159" s="9"/>
+      <c r="AF159" s="9"/>
+      <c r="AG159" s="9"/>
+      <c r="AH159" s="9"/>
+      <c r="AI159" s="9"/>
+      <c r="AJ159" s="9"/>
+      <c r="AK159" s="9"/>
+      <c r="AL159" s="9"/>
+      <c r="AQ159" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR159" s="9"/>
+      <c r="AS159" s="9"/>
+      <c r="AT159" s="9"/>
+      <c r="AU159" s="9"/>
+      <c r="AV159" s="9"/>
+      <c r="AW159" s="9"/>
+      <c r="AX159" s="9"/>
+      <c r="AY159" s="9"/>
+      <c r="AZ159" s="9"/>
+      <c r="BA159" s="9"/>
+      <c r="BB159" s="9"/>
+      <c r="BC159" s="9"/>
+      <c r="BD159" s="9"/>
+      <c r="BE159" s="9"/>
+      <c r="BF159" s="9"/>
+      <c r="BG159" s="9"/>
+    </row>
+    <row r="160" spans="2:59" x14ac:dyDescent="0.4">
+      <c r="W160" s="9"/>
+      <c r="X160" s="9"/>
+      <c r="Y160" s="9"/>
+      <c r="Z160" s="9"/>
+      <c r="AA160" s="9"/>
+      <c r="AB160" s="9"/>
+      <c r="AC160" s="9"/>
+      <c r="AD160" s="9"/>
+      <c r="AE160" s="9"/>
+      <c r="AF160" s="9"/>
+      <c r="AG160" s="9"/>
+      <c r="AH160" s="9"/>
+      <c r="AI160" s="9"/>
+      <c r="AJ160" s="9"/>
+      <c r="AK160" s="9"/>
+      <c r="AL160" s="9"/>
+      <c r="AQ160" s="9"/>
+      <c r="AR160" s="9"/>
+      <c r="AS160" s="9"/>
+      <c r="AT160" s="9"/>
+      <c r="AU160" s="9"/>
+      <c r="AV160" s="9"/>
+      <c r="AW160" s="9"/>
+      <c r="AX160" s="9"/>
+      <c r="AY160" s="9"/>
+      <c r="AZ160" s="9"/>
+      <c r="BA160" s="9"/>
+      <c r="BB160" s="9"/>
+      <c r="BC160" s="9"/>
+      <c r="BD160" s="9"/>
+      <c r="BE160" s="9"/>
+      <c r="BF160" s="9"/>
+      <c r="BG160" s="9"/>
+    </row>
+    <row r="161" spans="23:59" x14ac:dyDescent="0.4">
+      <c r="W161" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="X161" s="9"/>
+      <c r="Y161" s="9"/>
+      <c r="Z161" s="9"/>
+      <c r="AA161" s="9"/>
+      <c r="AB161" s="9"/>
+      <c r="AC161" s="9"/>
+      <c r="AD161" s="9"/>
+      <c r="AE161" s="9"/>
+      <c r="AF161" s="9"/>
+      <c r="AG161" s="9"/>
+      <c r="AH161" s="9"/>
+      <c r="AI161" s="9"/>
+      <c r="AJ161" s="9"/>
+      <c r="AK161" s="9"/>
+      <c r="AL161" s="9"/>
+      <c r="AQ161" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="AR161" s="9"/>
+      <c r="AS161" s="9"/>
+      <c r="AT161" s="9"/>
+      <c r="AU161" s="9"/>
+      <c r="AV161" s="9"/>
+      <c r="AW161" s="9"/>
+      <c r="AX161" s="9"/>
+      <c r="AY161" s="9"/>
+      <c r="AZ161" s="9"/>
+      <c r="BA161" s="9"/>
+      <c r="BB161" s="9"/>
+      <c r="BC161" s="9"/>
+      <c r="BD161" s="9"/>
+      <c r="BE161" s="9"/>
+      <c r="BF161" s="9"/>
+      <c r="BG161" s="9"/>
+    </row>
+    <row r="162" spans="23:59" x14ac:dyDescent="0.4">
+      <c r="W162" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="X162" s="9"/>
+      <c r="Y162" s="9"/>
+      <c r="Z162" s="9"/>
+      <c r="AA162" s="9"/>
+      <c r="AB162" s="9"/>
+      <c r="AC162" s="9"/>
+      <c r="AD162" s="9"/>
+      <c r="AE162" s="9"/>
+      <c r="AF162" s="9"/>
+      <c r="AG162" s="9"/>
+      <c r="AH162" s="9"/>
+      <c r="AI162" s="9"/>
+      <c r="AJ162" s="9"/>
+      <c r="AK162" s="9"/>
+      <c r="AL162" s="9"/>
+      <c r="AQ162" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR162" s="9"/>
+      <c r="AS162" s="9"/>
+      <c r="AT162" s="9"/>
+      <c r="AU162" s="9"/>
+      <c r="AV162" s="9"/>
+      <c r="AW162" s="9"/>
+      <c r="AX162" s="9"/>
+      <c r="AY162" s="9"/>
+      <c r="AZ162" s="9"/>
+      <c r="BA162" s="9"/>
+      <c r="BB162" s="9"/>
+      <c r="BC162" s="9"/>
+      <c r="BD162" s="9"/>
+      <c r="BE162" s="9"/>
+      <c r="BF162" s="9"/>
+      <c r="BG162" s="9"/>
+    </row>
+    <row r="163" spans="23:59" x14ac:dyDescent="0.4">
+      <c r="W163" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="X163" s="9"/>
+      <c r="Y163" s="9"/>
+      <c r="Z163" s="9"/>
+      <c r="AA163" s="9"/>
+      <c r="AB163" s="9"/>
+      <c r="AC163" s="9"/>
+      <c r="AD163" s="9"/>
+      <c r="AE163" s="9"/>
+      <c r="AF163" s="9"/>
+      <c r="AG163" s="9"/>
+      <c r="AH163" s="9"/>
+      <c r="AI163" s="9"/>
+      <c r="AJ163" s="9"/>
+      <c r="AK163" s="9"/>
+      <c r="AL163" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{9E8104E2-0B1A-498B-A07D-38DAF385409A}"/>

</xml_diff>

<commit_message>
doc: 680. Valid Palindrome II
Leetcode problem 680. Valid Palindrome II is solved and documented
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026E5EFE-6F84-4989-A0B3-CDB585AB5DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBE608C-02B0-40B9-9C20-4F5AAE296032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="557">
   <si>
     <t>Title</t>
   </si>
@@ -1881,6 +1881,45 @@
   </si>
   <si>
     <t xml:space="preserve">    return true;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    bool isValidPalindrome(string&amp; s, int left, int right, bool skipped) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (left &gt;= right)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (s[left] != s[right]) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            if (skipped)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            return isValidPalindrome(s, left + 1, right, true) ||</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   isValidPalindrome(s, left, right - 1, true);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return isValidPalindrome(s, left + 1, right - 1, skipped);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    bool validPalindrome(string s) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int left = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int right = s.length() - 1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return isValidPalindrome(s, left, right, false);</t>
+  </si>
+  <si>
+    <t>680. Valid Palindrome II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/valid-palindrome-ii/description/</t>
   </si>
 </sst>
 </file>
@@ -8926,10 +8965,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28504ADD-8E4E-436B-849F-525BA36E82D6}">
-  <dimension ref="A2:HD163"/>
+  <dimension ref="A2:HD188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U146" workbookViewId="0">
-      <selection activeCell="AL163" sqref="AL163"/>
+    <sheetView tabSelected="1" topLeftCell="U157" workbookViewId="0">
+      <selection activeCell="AT170" sqref="AT170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -19445,7 +19484,7 @@
       <c r="BF160" s="9"/>
       <c r="BG160" s="9"/>
     </row>
-    <row r="161" spans="23:59" x14ac:dyDescent="0.4">
+    <row r="161" spans="22:59" x14ac:dyDescent="0.4">
       <c r="W161" s="9" t="s">
         <v>529</v>
       </c>
@@ -19484,7 +19523,7 @@
       <c r="BF161" s="9"/>
       <c r="BG161" s="9"/>
     </row>
-    <row r="162" spans="23:59" x14ac:dyDescent="0.4">
+    <row r="162" spans="22:59" x14ac:dyDescent="0.4">
       <c r="W162" s="9" t="s">
         <v>48</v>
       </c>
@@ -19523,7 +19562,7 @@
       <c r="BF162" s="9"/>
       <c r="BG162" s="9"/>
     </row>
-    <row r="163" spans="23:59" x14ac:dyDescent="0.4">
+    <row r="163" spans="22:59" x14ac:dyDescent="0.4">
       <c r="W163" s="9" t="s">
         <v>299</v>
       </c>
@@ -19542,6 +19581,512 @@
       <c r="AJ163" s="9"/>
       <c r="AK163" s="9"/>
       <c r="AL163" s="9"/>
+    </row>
+    <row r="165" spans="22:59" x14ac:dyDescent="0.4">
+      <c r="V165" s="59" t="s">
+        <v>555</v>
+      </c>
+      <c r="AK165" s="53" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="166" spans="22:59" x14ac:dyDescent="0.4">
+      <c r="W166" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="X166" s="9"/>
+      <c r="Y166" s="9"/>
+      <c r="Z166" s="9"/>
+      <c r="AA166" s="9"/>
+      <c r="AB166" s="9"/>
+      <c r="AC166" s="9"/>
+      <c r="AD166" s="9"/>
+      <c r="AE166" s="9"/>
+      <c r="AF166" s="9"/>
+      <c r="AG166" s="9"/>
+      <c r="AH166" s="9"/>
+      <c r="AI166" s="9"/>
+      <c r="AJ166" s="9"/>
+      <c r="AK166" s="9"/>
+      <c r="AL166" s="9"/>
+      <c r="AM166" s="9"/>
+      <c r="AN166" s="9"/>
+    </row>
+    <row r="167" spans="22:59" x14ac:dyDescent="0.4">
+      <c r="W167" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="X167" s="9"/>
+      <c r="Y167" s="9"/>
+      <c r="Z167" s="9"/>
+      <c r="AA167" s="9"/>
+      <c r="AB167" s="9"/>
+      <c r="AC167" s="9"/>
+      <c r="AD167" s="9"/>
+      <c r="AE167" s="9"/>
+      <c r="AF167" s="9"/>
+      <c r="AG167" s="9"/>
+      <c r="AH167" s="9"/>
+      <c r="AI167" s="9"/>
+      <c r="AJ167" s="9"/>
+      <c r="AK167" s="9"/>
+      <c r="AL167" s="9"/>
+      <c r="AM167" s="9"/>
+      <c r="AN167" s="9"/>
+    </row>
+    <row r="168" spans="22:59" x14ac:dyDescent="0.4">
+      <c r="W168" s="9" t="s">
+        <v>544</v>
+      </c>
+      <c r="X168" s="9"/>
+      <c r="Y168" s="9"/>
+      <c r="Z168" s="9"/>
+      <c r="AA168" s="9"/>
+      <c r="AB168" s="9"/>
+      <c r="AC168" s="9"/>
+      <c r="AD168" s="9"/>
+      <c r="AE168" s="9"/>
+      <c r="AF168" s="9"/>
+      <c r="AG168" s="9"/>
+      <c r="AH168" s="9"/>
+      <c r="AI168" s="9"/>
+      <c r="AJ168" s="9"/>
+      <c r="AK168" s="9"/>
+      <c r="AL168" s="9"/>
+      <c r="AM168" s="9"/>
+      <c r="AN168" s="9"/>
+    </row>
+    <row r="169" spans="22:59" x14ac:dyDescent="0.4">
+      <c r="W169" s="9"/>
+      <c r="X169" s="9"/>
+      <c r="Y169" s="9"/>
+      <c r="Z169" s="9"/>
+      <c r="AA169" s="9"/>
+      <c r="AB169" s="9"/>
+      <c r="AC169" s="9"/>
+      <c r="AD169" s="9"/>
+      <c r="AE169" s="9"/>
+      <c r="AF169" s="9"/>
+      <c r="AG169" s="9"/>
+      <c r="AH169" s="9"/>
+      <c r="AI169" s="9"/>
+      <c r="AJ169" s="9"/>
+      <c r="AK169" s="9"/>
+      <c r="AL169" s="9"/>
+      <c r="AM169" s="9"/>
+      <c r="AN169" s="9"/>
+    </row>
+    <row r="170" spans="22:59" x14ac:dyDescent="0.4">
+      <c r="W170" s="9" t="s">
+        <v>545</v>
+      </c>
+      <c r="X170" s="9"/>
+      <c r="Y170" s="9"/>
+      <c r="Z170" s="9"/>
+      <c r="AA170" s="9"/>
+      <c r="AB170" s="9"/>
+      <c r="AC170" s="9"/>
+      <c r="AD170" s="9"/>
+      <c r="AE170" s="9"/>
+      <c r="AF170" s="9"/>
+      <c r="AG170" s="9"/>
+      <c r="AH170" s="9"/>
+      <c r="AI170" s="9"/>
+      <c r="AJ170" s="9"/>
+      <c r="AK170" s="9"/>
+      <c r="AL170" s="9"/>
+      <c r="AM170" s="9"/>
+      <c r="AN170" s="9"/>
+    </row>
+    <row r="171" spans="22:59" x14ac:dyDescent="0.4">
+      <c r="W171" s="9" t="s">
+        <v>508</v>
+      </c>
+      <c r="X171" s="9"/>
+      <c r="Y171" s="9"/>
+      <c r="Z171" s="9"/>
+      <c r="AA171" s="9"/>
+      <c r="AB171" s="9"/>
+      <c r="AC171" s="9"/>
+      <c r="AD171" s="9"/>
+      <c r="AE171" s="9"/>
+      <c r="AF171" s="9"/>
+      <c r="AG171" s="9"/>
+      <c r="AH171" s="9"/>
+      <c r="AI171" s="9"/>
+      <c r="AJ171" s="9"/>
+      <c r="AK171" s="9"/>
+      <c r="AL171" s="9"/>
+      <c r="AM171" s="9"/>
+      <c r="AN171" s="9"/>
+    </row>
+    <row r="172" spans="22:59" x14ac:dyDescent="0.4">
+      <c r="W172" s="9"/>
+      <c r="X172" s="9"/>
+      <c r="Y172" s="9"/>
+      <c r="Z172" s="9"/>
+      <c r="AA172" s="9"/>
+      <c r="AB172" s="9"/>
+      <c r="AC172" s="9"/>
+      <c r="AD172" s="9"/>
+      <c r="AE172" s="9"/>
+      <c r="AF172" s="9"/>
+      <c r="AG172" s="9"/>
+      <c r="AH172" s="9"/>
+      <c r="AI172" s="9"/>
+      <c r="AJ172" s="9"/>
+      <c r="AK172" s="9"/>
+      <c r="AL172" s="9"/>
+      <c r="AM172" s="9"/>
+      <c r="AN172" s="9"/>
+    </row>
+    <row r="173" spans="22:59" x14ac:dyDescent="0.4">
+      <c r="W173" s="9" t="s">
+        <v>546</v>
+      </c>
+      <c r="X173" s="9"/>
+      <c r="Y173" s="9"/>
+      <c r="Z173" s="9"/>
+      <c r="AA173" s="9"/>
+      <c r="AB173" s="9"/>
+      <c r="AC173" s="9"/>
+      <c r="AD173" s="9"/>
+      <c r="AE173" s="9"/>
+      <c r="AF173" s="9"/>
+      <c r="AG173" s="9"/>
+      <c r="AH173" s="9"/>
+      <c r="AI173" s="9"/>
+      <c r="AJ173" s="9"/>
+      <c r="AK173" s="9"/>
+      <c r="AL173" s="9"/>
+      <c r="AM173" s="9"/>
+      <c r="AN173" s="9"/>
+    </row>
+    <row r="174" spans="22:59" x14ac:dyDescent="0.4">
+      <c r="W174" s="9" t="s">
+        <v>547</v>
+      </c>
+      <c r="X174" s="9"/>
+      <c r="Y174" s="9"/>
+      <c r="Z174" s="9"/>
+      <c r="AA174" s="9"/>
+      <c r="AB174" s="9"/>
+      <c r="AC174" s="9"/>
+      <c r="AD174" s="9"/>
+      <c r="AE174" s="9"/>
+      <c r="AF174" s="9"/>
+      <c r="AG174" s="9"/>
+      <c r="AH174" s="9"/>
+      <c r="AI174" s="9"/>
+      <c r="AJ174" s="9"/>
+      <c r="AK174" s="9"/>
+      <c r="AL174" s="9"/>
+      <c r="AM174" s="9"/>
+      <c r="AN174" s="9"/>
+    </row>
+    <row r="175" spans="22:59" x14ac:dyDescent="0.4">
+      <c r="W175" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="X175" s="9"/>
+      <c r="Y175" s="9"/>
+      <c r="Z175" s="9"/>
+      <c r="AA175" s="9"/>
+      <c r="AB175" s="9"/>
+      <c r="AC175" s="9"/>
+      <c r="AD175" s="9"/>
+      <c r="AE175" s="9"/>
+      <c r="AF175" s="9"/>
+      <c r="AG175" s="9"/>
+      <c r="AH175" s="9"/>
+      <c r="AI175" s="9"/>
+      <c r="AJ175" s="9"/>
+      <c r="AK175" s="9"/>
+      <c r="AL175" s="9"/>
+      <c r="AM175" s="9"/>
+      <c r="AN175" s="9"/>
+    </row>
+    <row r="176" spans="22:59" x14ac:dyDescent="0.4">
+      <c r="W176" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="X176" s="9"/>
+      <c r="Y176" s="9"/>
+      <c r="Z176" s="9"/>
+      <c r="AA176" s="9"/>
+      <c r="AB176" s="9"/>
+      <c r="AC176" s="9"/>
+      <c r="AD176" s="9"/>
+      <c r="AE176" s="9"/>
+      <c r="AF176" s="9"/>
+      <c r="AG176" s="9"/>
+      <c r="AH176" s="9"/>
+      <c r="AI176" s="9"/>
+      <c r="AJ176" s="9"/>
+      <c r="AK176" s="9"/>
+      <c r="AL176" s="9"/>
+      <c r="AM176" s="9"/>
+      <c r="AN176" s="9"/>
+    </row>
+    <row r="177" spans="23:40" x14ac:dyDescent="0.4">
+      <c r="W177" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="X177" s="9"/>
+      <c r="Y177" s="9"/>
+      <c r="Z177" s="9"/>
+      <c r="AA177" s="9"/>
+      <c r="AB177" s="9"/>
+      <c r="AC177" s="9"/>
+      <c r="AD177" s="9"/>
+      <c r="AE177" s="9"/>
+      <c r="AF177" s="9"/>
+      <c r="AG177" s="9"/>
+      <c r="AH177" s="9"/>
+      <c r="AI177" s="9"/>
+      <c r="AJ177" s="9"/>
+      <c r="AK177" s="9"/>
+      <c r="AL177" s="9"/>
+      <c r="AM177" s="9"/>
+      <c r="AN177" s="9"/>
+    </row>
+    <row r="178" spans="23:40" x14ac:dyDescent="0.4">
+      <c r="W178" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="X178" s="9"/>
+      <c r="Y178" s="9"/>
+      <c r="Z178" s="9"/>
+      <c r="AA178" s="9"/>
+      <c r="AB178" s="9"/>
+      <c r="AC178" s="9"/>
+      <c r="AD178" s="9"/>
+      <c r="AE178" s="9"/>
+      <c r="AF178" s="9"/>
+      <c r="AG178" s="9"/>
+      <c r="AH178" s="9"/>
+      <c r="AI178" s="9"/>
+      <c r="AJ178" s="9"/>
+      <c r="AK178" s="9"/>
+      <c r="AL178" s="9"/>
+      <c r="AM178" s="9"/>
+      <c r="AN178" s="9"/>
+    </row>
+    <row r="179" spans="23:40" x14ac:dyDescent="0.4">
+      <c r="W179" s="9"/>
+      <c r="X179" s="9"/>
+      <c r="Y179" s="9"/>
+      <c r="Z179" s="9"/>
+      <c r="AA179" s="9"/>
+      <c r="AB179" s="9"/>
+      <c r="AC179" s="9"/>
+      <c r="AD179" s="9"/>
+      <c r="AE179" s="9"/>
+      <c r="AF179" s="9"/>
+      <c r="AG179" s="9"/>
+      <c r="AH179" s="9"/>
+      <c r="AI179" s="9"/>
+      <c r="AJ179" s="9"/>
+      <c r="AK179" s="9"/>
+      <c r="AL179" s="9"/>
+      <c r="AM179" s="9"/>
+      <c r="AN179" s="9"/>
+    </row>
+    <row r="180" spans="23:40" x14ac:dyDescent="0.4">
+      <c r="W180" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="X180" s="9"/>
+      <c r="Y180" s="9"/>
+      <c r="Z180" s="9"/>
+      <c r="AA180" s="9"/>
+      <c r="AB180" s="9"/>
+      <c r="AC180" s="9"/>
+      <c r="AD180" s="9"/>
+      <c r="AE180" s="9"/>
+      <c r="AF180" s="9"/>
+      <c r="AG180" s="9"/>
+      <c r="AH180" s="9"/>
+      <c r="AI180" s="9"/>
+      <c r="AJ180" s="9"/>
+      <c r="AK180" s="9"/>
+      <c r="AL180" s="9"/>
+      <c r="AM180" s="9"/>
+      <c r="AN180" s="9"/>
+    </row>
+    <row r="181" spans="23:40" x14ac:dyDescent="0.4">
+      <c r="W181" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="X181" s="9"/>
+      <c r="Y181" s="9"/>
+      <c r="Z181" s="9"/>
+      <c r="AA181" s="9"/>
+      <c r="AB181" s="9"/>
+      <c r="AC181" s="9"/>
+      <c r="AD181" s="9"/>
+      <c r="AE181" s="9"/>
+      <c r="AF181" s="9"/>
+      <c r="AG181" s="9"/>
+      <c r="AH181" s="9"/>
+      <c r="AI181" s="9"/>
+      <c r="AJ181" s="9"/>
+      <c r="AK181" s="9"/>
+      <c r="AL181" s="9"/>
+      <c r="AM181" s="9"/>
+      <c r="AN181" s="9"/>
+    </row>
+    <row r="182" spans="23:40" x14ac:dyDescent="0.4">
+      <c r="W182" s="9"/>
+      <c r="X182" s="9"/>
+      <c r="Y182" s="9"/>
+      <c r="Z182" s="9"/>
+      <c r="AA182" s="9"/>
+      <c r="AB182" s="9"/>
+      <c r="AC182" s="9"/>
+      <c r="AD182" s="9"/>
+      <c r="AE182" s="9"/>
+      <c r="AF182" s="9"/>
+      <c r="AG182" s="9"/>
+      <c r="AH182" s="9"/>
+      <c r="AI182" s="9"/>
+      <c r="AJ182" s="9"/>
+      <c r="AK182" s="9"/>
+      <c r="AL182" s="9"/>
+      <c r="AM182" s="9"/>
+      <c r="AN182" s="9"/>
+    </row>
+    <row r="183" spans="23:40" x14ac:dyDescent="0.4">
+      <c r="W183" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="X183" s="9"/>
+      <c r="Y183" s="9"/>
+      <c r="Z183" s="9"/>
+      <c r="AA183" s="9"/>
+      <c r="AB183" s="9"/>
+      <c r="AC183" s="9"/>
+      <c r="AD183" s="9"/>
+      <c r="AE183" s="9"/>
+      <c r="AF183" s="9"/>
+      <c r="AG183" s="9"/>
+      <c r="AH183" s="9"/>
+      <c r="AI183" s="9"/>
+      <c r="AJ183" s="9"/>
+      <c r="AK183" s="9"/>
+      <c r="AL183" s="9"/>
+      <c r="AM183" s="9"/>
+      <c r="AN183" s="9"/>
+    </row>
+    <row r="184" spans="23:40" x14ac:dyDescent="0.4">
+      <c r="W184" s="9" t="s">
+        <v>552</v>
+      </c>
+      <c r="X184" s="9"/>
+      <c r="Y184" s="9"/>
+      <c r="Z184" s="9"/>
+      <c r="AA184" s="9"/>
+      <c r="AB184" s="9"/>
+      <c r="AC184" s="9"/>
+      <c r="AD184" s="9"/>
+      <c r="AE184" s="9"/>
+      <c r="AF184" s="9"/>
+      <c r="AG184" s="9"/>
+      <c r="AH184" s="9"/>
+      <c r="AI184" s="9"/>
+      <c r="AJ184" s="9"/>
+      <c r="AK184" s="9"/>
+      <c r="AL184" s="9"/>
+      <c r="AM184" s="9"/>
+      <c r="AN184" s="9"/>
+    </row>
+    <row r="185" spans="23:40" x14ac:dyDescent="0.4">
+      <c r="W185" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="X185" s="9"/>
+      <c r="Y185" s="9"/>
+      <c r="Z185" s="9"/>
+      <c r="AA185" s="9"/>
+      <c r="AB185" s="9"/>
+      <c r="AC185" s="9"/>
+      <c r="AD185" s="9"/>
+      <c r="AE185" s="9"/>
+      <c r="AF185" s="9"/>
+      <c r="AG185" s="9"/>
+      <c r="AH185" s="9"/>
+      <c r="AI185" s="9"/>
+      <c r="AJ185" s="9"/>
+      <c r="AK185" s="9"/>
+      <c r="AL185" s="9"/>
+      <c r="AM185" s="9"/>
+      <c r="AN185" s="9"/>
+    </row>
+    <row r="186" spans="23:40" x14ac:dyDescent="0.4">
+      <c r="W186" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="X186" s="9"/>
+      <c r="Y186" s="9"/>
+      <c r="Z186" s="9"/>
+      <c r="AA186" s="9"/>
+      <c r="AB186" s="9"/>
+      <c r="AC186" s="9"/>
+      <c r="AD186" s="9"/>
+      <c r="AE186" s="9"/>
+      <c r="AF186" s="9"/>
+      <c r="AG186" s="9"/>
+      <c r="AH186" s="9"/>
+      <c r="AI186" s="9"/>
+      <c r="AJ186" s="9"/>
+      <c r="AK186" s="9"/>
+      <c r="AL186" s="9"/>
+      <c r="AM186" s="9"/>
+      <c r="AN186" s="9"/>
+    </row>
+    <row r="187" spans="23:40" x14ac:dyDescent="0.4">
+      <c r="W187" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="X187" s="9"/>
+      <c r="Y187" s="9"/>
+      <c r="Z187" s="9"/>
+      <c r="AA187" s="9"/>
+      <c r="AB187" s="9"/>
+      <c r="AC187" s="9"/>
+      <c r="AD187" s="9"/>
+      <c r="AE187" s="9"/>
+      <c r="AF187" s="9"/>
+      <c r="AG187" s="9"/>
+      <c r="AH187" s="9"/>
+      <c r="AI187" s="9"/>
+      <c r="AJ187" s="9"/>
+      <c r="AK187" s="9"/>
+      <c r="AL187" s="9"/>
+      <c r="AM187" s="9"/>
+      <c r="AN187" s="9"/>
+    </row>
+    <row r="188" spans="23:40" x14ac:dyDescent="0.4">
+      <c r="W188" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="X188" s="9"/>
+      <c r="Y188" s="9"/>
+      <c r="Z188" s="9"/>
+      <c r="AA188" s="9"/>
+      <c r="AB188" s="9"/>
+      <c r="AC188" s="9"/>
+      <c r="AD188" s="9"/>
+      <c r="AE188" s="9"/>
+      <c r="AF188" s="9"/>
+      <c r="AG188" s="9"/>
+      <c r="AH188" s="9"/>
+      <c r="AI188" s="9"/>
+      <c r="AJ188" s="9"/>
+      <c r="AK188" s="9"/>
+      <c r="AL188" s="9"/>
+      <c r="AM188" s="9"/>
+      <c r="AN188" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
doc:: 2108. Find First Palindromic String in the Array
leetcode problem 2108. Find First Palindromic String in the Array is solved and captured
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBE608C-02B0-40B9-9C20-4F5AAE296032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C189958-C744-4AE6-A97A-393AF1DC4ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="578">
   <si>
     <t>Title</t>
   </si>
@@ -1920,6 +1920,69 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/valid-palindrome-ii/description/</t>
+  </si>
+  <si>
+    <t>#include &lt;vector&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    std::string firstPalindrome(std::vector&lt;std::string&gt;&amp; words) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        // Define a function to check if a string is a palindrome.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        auto isPalindrome = [](const std::string&amp; s) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            int i = 0, j = s.length() - 1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            // Iterate from both ends towards the center to check for equality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            while (i &lt;= j) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                if (s[i] != s[j]) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    return false;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                i++;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                j--;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        };</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        // Iterate through each word in the vector.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        for (const auto&amp; word : words) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            // If a palindrome is found, return it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            if (isPalindrome(word)) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                return word;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        // If no palindrome is found, return an empty string.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return "";</t>
+  </si>
+  <si>
+    <t>2108. Find First Palindromic String in the Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-first-palindromic-string-in-the-array/description/</t>
   </si>
 </sst>
 </file>
@@ -8965,10 +9028,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28504ADD-8E4E-436B-849F-525BA36E82D6}">
-  <dimension ref="A2:HD188"/>
+  <dimension ref="A2:HD224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U157" workbookViewId="0">
-      <selection activeCell="AT170" sqref="AT170"/>
+    <sheetView tabSelected="1" topLeftCell="U187" workbookViewId="0">
+      <selection activeCell="AL191" sqref="AL191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -19828,7 +19891,7 @@
       <c r="AM176" s="9"/>
       <c r="AN176" s="9"/>
     </row>
-    <row r="177" spans="23:40" x14ac:dyDescent="0.4">
+    <row r="177" spans="22:41" x14ac:dyDescent="0.4">
       <c r="W177" s="9" t="s">
         <v>549</v>
       </c>
@@ -19850,7 +19913,7 @@
       <c r="AM177" s="9"/>
       <c r="AN177" s="9"/>
     </row>
-    <row r="178" spans="23:40" x14ac:dyDescent="0.4">
+    <row r="178" spans="22:41" x14ac:dyDescent="0.4">
       <c r="W178" s="9" t="s">
         <v>202</v>
       </c>
@@ -19872,7 +19935,7 @@
       <c r="AM178" s="9"/>
       <c r="AN178" s="9"/>
     </row>
-    <row r="179" spans="23:40" x14ac:dyDescent="0.4">
+    <row r="179" spans="22:41" x14ac:dyDescent="0.4">
       <c r="W179" s="9"/>
       <c r="X179" s="9"/>
       <c r="Y179" s="9"/>
@@ -19892,7 +19955,7 @@
       <c r="AM179" s="9"/>
       <c r="AN179" s="9"/>
     </row>
-    <row r="180" spans="23:40" x14ac:dyDescent="0.4">
+    <row r="180" spans="22:41" x14ac:dyDescent="0.4">
       <c r="W180" s="9" t="s">
         <v>550</v>
       </c>
@@ -19914,7 +19977,7 @@
       <c r="AM180" s="9"/>
       <c r="AN180" s="9"/>
     </row>
-    <row r="181" spans="23:40" x14ac:dyDescent="0.4">
+    <row r="181" spans="22:41" x14ac:dyDescent="0.4">
       <c r="W181" s="9" t="s">
         <v>48</v>
       </c>
@@ -19936,7 +19999,7 @@
       <c r="AM181" s="9"/>
       <c r="AN181" s="9"/>
     </row>
-    <row r="182" spans="23:40" x14ac:dyDescent="0.4">
+    <row r="182" spans="22:41" x14ac:dyDescent="0.4">
       <c r="W182" s="9"/>
       <c r="X182" s="9"/>
       <c r="Y182" s="9"/>
@@ -19956,7 +20019,7 @@
       <c r="AM182" s="9"/>
       <c r="AN182" s="9"/>
     </row>
-    <row r="183" spans="23:40" x14ac:dyDescent="0.4">
+    <row r="183" spans="22:41" x14ac:dyDescent="0.4">
       <c r="W183" s="9" t="s">
         <v>551</v>
       </c>
@@ -19978,7 +20041,7 @@
       <c r="AM183" s="9"/>
       <c r="AN183" s="9"/>
     </row>
-    <row r="184" spans="23:40" x14ac:dyDescent="0.4">
+    <row r="184" spans="22:41" x14ac:dyDescent="0.4">
       <c r="W184" s="9" t="s">
         <v>552</v>
       </c>
@@ -20000,7 +20063,7 @@
       <c r="AM184" s="9"/>
       <c r="AN184" s="9"/>
     </row>
-    <row r="185" spans="23:40" x14ac:dyDescent="0.4">
+    <row r="185" spans="22:41" x14ac:dyDescent="0.4">
       <c r="W185" s="9" t="s">
         <v>553</v>
       </c>
@@ -20022,7 +20085,7 @@
       <c r="AM185" s="9"/>
       <c r="AN185" s="9"/>
     </row>
-    <row r="186" spans="23:40" x14ac:dyDescent="0.4">
+    <row r="186" spans="22:41" x14ac:dyDescent="0.4">
       <c r="W186" s="9" t="s">
         <v>554</v>
       </c>
@@ -20044,7 +20107,7 @@
       <c r="AM186" s="9"/>
       <c r="AN186" s="9"/>
     </row>
-    <row r="187" spans="23:40" x14ac:dyDescent="0.4">
+    <row r="187" spans="22:41" x14ac:dyDescent="0.4">
       <c r="W187" s="9" t="s">
         <v>48</v>
       </c>
@@ -20066,7 +20129,7 @@
       <c r="AM187" s="9"/>
       <c r="AN187" s="9"/>
     </row>
-    <row r="188" spans="23:40" x14ac:dyDescent="0.4">
+    <row r="188" spans="22:41" x14ac:dyDescent="0.4">
       <c r="W188" s="9" t="s">
         <v>299</v>
       </c>
@@ -20088,13 +20151,795 @@
       <c r="AM188" s="9"/>
       <c r="AN188" s="9"/>
     </row>
+    <row r="190" spans="22:41" x14ac:dyDescent="0.4">
+      <c r="V190" s="53" t="s">
+        <v>576</v>
+      </c>
+      <c r="AL190" s="62" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="191" spans="22:41" x14ac:dyDescent="0.4">
+      <c r="W191" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="X191" s="9"/>
+      <c r="Y191" s="9"/>
+      <c r="Z191" s="9"/>
+      <c r="AA191" s="9"/>
+      <c r="AB191" s="9"/>
+      <c r="AC191" s="9"/>
+      <c r="AD191" s="9"/>
+      <c r="AE191" s="9"/>
+      <c r="AF191" s="9"/>
+      <c r="AG191" s="9"/>
+      <c r="AH191" s="9"/>
+      <c r="AI191" s="9"/>
+      <c r="AJ191" s="9"/>
+      <c r="AK191" s="9"/>
+      <c r="AL191" s="9"/>
+      <c r="AM191" s="9"/>
+      <c r="AN191" s="9"/>
+      <c r="AO191" s="9"/>
+    </row>
+    <row r="192" spans="22:41" x14ac:dyDescent="0.4">
+      <c r="W192" s="9" t="s">
+        <v>557</v>
+      </c>
+      <c r="X192" s="9"/>
+      <c r="Y192" s="9"/>
+      <c r="Z192" s="9"/>
+      <c r="AA192" s="9"/>
+      <c r="AB192" s="9"/>
+      <c r="AC192" s="9"/>
+      <c r="AD192" s="9"/>
+      <c r="AE192" s="9"/>
+      <c r="AF192" s="9"/>
+      <c r="AG192" s="9"/>
+      <c r="AH192" s="9"/>
+      <c r="AI192" s="9"/>
+      <c r="AJ192" s="9"/>
+      <c r="AK192" s="9"/>
+      <c r="AL192" s="9"/>
+      <c r="AM192" s="9"/>
+      <c r="AN192" s="9"/>
+      <c r="AO192" s="9"/>
+    </row>
+    <row r="193" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W193" s="9"/>
+      <c r="X193" s="9"/>
+      <c r="Y193" s="9"/>
+      <c r="Z193" s="9"/>
+      <c r="AA193" s="9"/>
+      <c r="AB193" s="9"/>
+      <c r="AC193" s="9"/>
+      <c r="AD193" s="9"/>
+      <c r="AE193" s="9"/>
+      <c r="AF193" s="9"/>
+      <c r="AG193" s="9"/>
+      <c r="AH193" s="9"/>
+      <c r="AI193" s="9"/>
+      <c r="AJ193" s="9"/>
+      <c r="AK193" s="9"/>
+      <c r="AL193" s="9"/>
+      <c r="AM193" s="9"/>
+      <c r="AN193" s="9"/>
+      <c r="AO193" s="9"/>
+    </row>
+    <row r="194" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W194" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="X194" s="9"/>
+      <c r="Y194" s="9"/>
+      <c r="Z194" s="9"/>
+      <c r="AA194" s="9"/>
+      <c r="AB194" s="9"/>
+      <c r="AC194" s="9"/>
+      <c r="AD194" s="9"/>
+      <c r="AE194" s="9"/>
+      <c r="AF194" s="9"/>
+      <c r="AG194" s="9"/>
+      <c r="AH194" s="9"/>
+      <c r="AI194" s="9"/>
+      <c r="AJ194" s="9"/>
+      <c r="AK194" s="9"/>
+      <c r="AL194" s="9"/>
+      <c r="AM194" s="9"/>
+      <c r="AN194" s="9"/>
+      <c r="AO194" s="9"/>
+    </row>
+    <row r="195" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W195" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="X195" s="9"/>
+      <c r="Y195" s="9"/>
+      <c r="Z195" s="9"/>
+      <c r="AA195" s="9"/>
+      <c r="AB195" s="9"/>
+      <c r="AC195" s="9"/>
+      <c r="AD195" s="9"/>
+      <c r="AE195" s="9"/>
+      <c r="AF195" s="9"/>
+      <c r="AG195" s="9"/>
+      <c r="AH195" s="9"/>
+      <c r="AI195" s="9"/>
+      <c r="AJ195" s="9"/>
+      <c r="AK195" s="9"/>
+      <c r="AL195" s="9"/>
+      <c r="AM195" s="9"/>
+      <c r="AN195" s="9"/>
+      <c r="AO195" s="9"/>
+    </row>
+    <row r="196" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W196" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="X196" s="9"/>
+      <c r="Y196" s="9"/>
+      <c r="Z196" s="9"/>
+      <c r="AA196" s="9"/>
+      <c r="AB196" s="9"/>
+      <c r="AC196" s="9"/>
+      <c r="AD196" s="9"/>
+      <c r="AE196" s="9"/>
+      <c r="AF196" s="9"/>
+      <c r="AG196" s="9"/>
+      <c r="AH196" s="9"/>
+      <c r="AI196" s="9"/>
+      <c r="AJ196" s="9"/>
+      <c r="AK196" s="9"/>
+      <c r="AL196" s="9"/>
+      <c r="AM196" s="9"/>
+      <c r="AN196" s="9"/>
+      <c r="AO196" s="9"/>
+    </row>
+    <row r="197" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W197" s="9" t="s">
+        <v>559</v>
+      </c>
+      <c r="X197" s="9"/>
+      <c r="Y197" s="9"/>
+      <c r="Z197" s="9"/>
+      <c r="AA197" s="9"/>
+      <c r="AB197" s="9"/>
+      <c r="AC197" s="9"/>
+      <c r="AD197" s="9"/>
+      <c r="AE197" s="9"/>
+      <c r="AF197" s="9"/>
+      <c r="AG197" s="9"/>
+      <c r="AH197" s="9"/>
+      <c r="AI197" s="9"/>
+      <c r="AJ197" s="9"/>
+      <c r="AK197" s="9"/>
+      <c r="AL197" s="9"/>
+      <c r="AM197" s="9"/>
+      <c r="AN197" s="9"/>
+      <c r="AO197" s="9"/>
+    </row>
+    <row r="198" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W198" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="X198" s="9"/>
+      <c r="Y198" s="9"/>
+      <c r="Z198" s="9"/>
+      <c r="AA198" s="9"/>
+      <c r="AB198" s="9"/>
+      <c r="AC198" s="9"/>
+      <c r="AD198" s="9"/>
+      <c r="AE198" s="9"/>
+      <c r="AF198" s="9"/>
+      <c r="AG198" s="9"/>
+      <c r="AH198" s="9"/>
+      <c r="AI198" s="9"/>
+      <c r="AJ198" s="9"/>
+      <c r="AK198" s="9"/>
+      <c r="AL198" s="9"/>
+      <c r="AM198" s="9"/>
+      <c r="AN198" s="9"/>
+      <c r="AO198" s="9"/>
+    </row>
+    <row r="199" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W199" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="X199" s="9"/>
+      <c r="Y199" s="9"/>
+      <c r="Z199" s="9"/>
+      <c r="AA199" s="9"/>
+      <c r="AB199" s="9"/>
+      <c r="AC199" s="9"/>
+      <c r="AD199" s="9"/>
+      <c r="AE199" s="9"/>
+      <c r="AF199" s="9"/>
+      <c r="AG199" s="9"/>
+      <c r="AH199" s="9"/>
+      <c r="AI199" s="9"/>
+      <c r="AJ199" s="9"/>
+      <c r="AK199" s="9"/>
+      <c r="AL199" s="9"/>
+      <c r="AM199" s="9"/>
+      <c r="AN199" s="9"/>
+      <c r="AO199" s="9"/>
+    </row>
+    <row r="200" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W200" s="9"/>
+      <c r="X200" s="9"/>
+      <c r="Y200" s="9"/>
+      <c r="Z200" s="9"/>
+      <c r="AA200" s="9"/>
+      <c r="AB200" s="9"/>
+      <c r="AC200" s="9"/>
+      <c r="AD200" s="9"/>
+      <c r="AE200" s="9"/>
+      <c r="AF200" s="9"/>
+      <c r="AG200" s="9"/>
+      <c r="AH200" s="9"/>
+      <c r="AI200" s="9"/>
+      <c r="AJ200" s="9"/>
+      <c r="AK200" s="9"/>
+      <c r="AL200" s="9"/>
+      <c r="AM200" s="9"/>
+      <c r="AN200" s="9"/>
+      <c r="AO200" s="9"/>
+    </row>
+    <row r="201" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W201" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="X201" s="9"/>
+      <c r="Y201" s="9"/>
+      <c r="Z201" s="9"/>
+      <c r="AA201" s="9"/>
+      <c r="AB201" s="9"/>
+      <c r="AC201" s="9"/>
+      <c r="AD201" s="9"/>
+      <c r="AE201" s="9"/>
+      <c r="AF201" s="9"/>
+      <c r="AG201" s="9"/>
+      <c r="AH201" s="9"/>
+      <c r="AI201" s="9"/>
+      <c r="AJ201" s="9"/>
+      <c r="AK201" s="9"/>
+      <c r="AL201" s="9"/>
+      <c r="AM201" s="9"/>
+      <c r="AN201" s="9"/>
+      <c r="AO201" s="9"/>
+    </row>
+    <row r="202" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W202" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="X202" s="9"/>
+      <c r="Y202" s="9"/>
+      <c r="Z202" s="9"/>
+      <c r="AA202" s="9"/>
+      <c r="AB202" s="9"/>
+      <c r="AC202" s="9"/>
+      <c r="AD202" s="9"/>
+      <c r="AE202" s="9"/>
+      <c r="AF202" s="9"/>
+      <c r="AG202" s="9"/>
+      <c r="AH202" s="9"/>
+      <c r="AI202" s="9"/>
+      <c r="AJ202" s="9"/>
+      <c r="AK202" s="9"/>
+      <c r="AL202" s="9"/>
+      <c r="AM202" s="9"/>
+      <c r="AN202" s="9"/>
+      <c r="AO202" s="9"/>
+    </row>
+    <row r="203" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W203" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="X203" s="9"/>
+      <c r="Y203" s="9"/>
+      <c r="Z203" s="9"/>
+      <c r="AA203" s="9"/>
+      <c r="AB203" s="9"/>
+      <c r="AC203" s="9"/>
+      <c r="AD203" s="9"/>
+      <c r="AE203" s="9"/>
+      <c r="AF203" s="9"/>
+      <c r="AG203" s="9"/>
+      <c r="AH203" s="9"/>
+      <c r="AI203" s="9"/>
+      <c r="AJ203" s="9"/>
+      <c r="AK203" s="9"/>
+      <c r="AL203" s="9"/>
+      <c r="AM203" s="9"/>
+      <c r="AN203" s="9"/>
+      <c r="AO203" s="9"/>
+    </row>
+    <row r="204" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W204" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="X204" s="9"/>
+      <c r="Y204" s="9"/>
+      <c r="Z204" s="9"/>
+      <c r="AA204" s="9"/>
+      <c r="AB204" s="9"/>
+      <c r="AC204" s="9"/>
+      <c r="AD204" s="9"/>
+      <c r="AE204" s="9"/>
+      <c r="AF204" s="9"/>
+      <c r="AG204" s="9"/>
+      <c r="AH204" s="9"/>
+      <c r="AI204" s="9"/>
+      <c r="AJ204" s="9"/>
+      <c r="AK204" s="9"/>
+      <c r="AL204" s="9"/>
+      <c r="AM204" s="9"/>
+      <c r="AN204" s="9"/>
+      <c r="AO204" s="9"/>
+    </row>
+    <row r="205" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W205" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="X205" s="9"/>
+      <c r="Y205" s="9"/>
+      <c r="Z205" s="9"/>
+      <c r="AA205" s="9"/>
+      <c r="AB205" s="9"/>
+      <c r="AC205" s="9"/>
+      <c r="AD205" s="9"/>
+      <c r="AE205" s="9"/>
+      <c r="AF205" s="9"/>
+      <c r="AG205" s="9"/>
+      <c r="AH205" s="9"/>
+      <c r="AI205" s="9"/>
+      <c r="AJ205" s="9"/>
+      <c r="AK205" s="9"/>
+      <c r="AL205" s="9"/>
+      <c r="AM205" s="9"/>
+      <c r="AN205" s="9"/>
+      <c r="AO205" s="9"/>
+    </row>
+    <row r="206" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W206" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="X206" s="9"/>
+      <c r="Y206" s="9"/>
+      <c r="Z206" s="9"/>
+      <c r="AA206" s="9"/>
+      <c r="AB206" s="9"/>
+      <c r="AC206" s="9"/>
+      <c r="AD206" s="9"/>
+      <c r="AE206" s="9"/>
+      <c r="AF206" s="9"/>
+      <c r="AG206" s="9"/>
+      <c r="AH206" s="9"/>
+      <c r="AI206" s="9"/>
+      <c r="AJ206" s="9"/>
+      <c r="AK206" s="9"/>
+      <c r="AL206" s="9"/>
+      <c r="AM206" s="9"/>
+      <c r="AN206" s="9"/>
+      <c r="AO206" s="9"/>
+    </row>
+    <row r="207" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W207" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="X207" s="9"/>
+      <c r="Y207" s="9"/>
+      <c r="Z207" s="9"/>
+      <c r="AA207" s="9"/>
+      <c r="AB207" s="9"/>
+      <c r="AC207" s="9"/>
+      <c r="AD207" s="9"/>
+      <c r="AE207" s="9"/>
+      <c r="AF207" s="9"/>
+      <c r="AG207" s="9"/>
+      <c r="AH207" s="9"/>
+      <c r="AI207" s="9"/>
+      <c r="AJ207" s="9"/>
+      <c r="AK207" s="9"/>
+      <c r="AL207" s="9"/>
+      <c r="AM207" s="9"/>
+      <c r="AN207" s="9"/>
+      <c r="AO207" s="9"/>
+    </row>
+    <row r="208" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W208" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="X208" s="9"/>
+      <c r="Y208" s="9"/>
+      <c r="Z208" s="9"/>
+      <c r="AA208" s="9"/>
+      <c r="AB208" s="9"/>
+      <c r="AC208" s="9"/>
+      <c r="AD208" s="9"/>
+      <c r="AE208" s="9"/>
+      <c r="AF208" s="9"/>
+      <c r="AG208" s="9"/>
+      <c r="AH208" s="9"/>
+      <c r="AI208" s="9"/>
+      <c r="AJ208" s="9"/>
+      <c r="AK208" s="9"/>
+      <c r="AL208" s="9"/>
+      <c r="AM208" s="9"/>
+      <c r="AN208" s="9"/>
+      <c r="AO208" s="9"/>
+    </row>
+    <row r="209" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W209" s="9"/>
+      <c r="X209" s="9"/>
+      <c r="Y209" s="9"/>
+      <c r="Z209" s="9"/>
+      <c r="AA209" s="9"/>
+      <c r="AB209" s="9"/>
+      <c r="AC209" s="9"/>
+      <c r="AD209" s="9"/>
+      <c r="AE209" s="9"/>
+      <c r="AF209" s="9"/>
+      <c r="AG209" s="9"/>
+      <c r="AH209" s="9"/>
+      <c r="AI209" s="9"/>
+      <c r="AJ209" s="9"/>
+      <c r="AK209" s="9"/>
+      <c r="AL209" s="9"/>
+      <c r="AM209" s="9"/>
+      <c r="AN209" s="9"/>
+      <c r="AO209" s="9"/>
+    </row>
+    <row r="210" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W210" s="9" t="s">
+        <v>508</v>
+      </c>
+      <c r="X210" s="9"/>
+      <c r="Y210" s="9"/>
+      <c r="Z210" s="9"/>
+      <c r="AA210" s="9"/>
+      <c r="AB210" s="9"/>
+      <c r="AC210" s="9"/>
+      <c r="AD210" s="9"/>
+      <c r="AE210" s="9"/>
+      <c r="AF210" s="9"/>
+      <c r="AG210" s="9"/>
+      <c r="AH210" s="9"/>
+      <c r="AI210" s="9"/>
+      <c r="AJ210" s="9"/>
+      <c r="AK210" s="9"/>
+      <c r="AL210" s="9"/>
+      <c r="AM210" s="9"/>
+      <c r="AN210" s="9"/>
+      <c r="AO210" s="9"/>
+    </row>
+    <row r="211" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W211" s="9" t="s">
+        <v>568</v>
+      </c>
+      <c r="X211" s="9"/>
+      <c r="Y211" s="9"/>
+      <c r="Z211" s="9"/>
+      <c r="AA211" s="9"/>
+      <c r="AB211" s="9"/>
+      <c r="AC211" s="9"/>
+      <c r="AD211" s="9"/>
+      <c r="AE211" s="9"/>
+      <c r="AF211" s="9"/>
+      <c r="AG211" s="9"/>
+      <c r="AH211" s="9"/>
+      <c r="AI211" s="9"/>
+      <c r="AJ211" s="9"/>
+      <c r="AK211" s="9"/>
+      <c r="AL211" s="9"/>
+      <c r="AM211" s="9"/>
+      <c r="AN211" s="9"/>
+      <c r="AO211" s="9"/>
+    </row>
+    <row r="212" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W212" s="9"/>
+      <c r="X212" s="9"/>
+      <c r="Y212" s="9"/>
+      <c r="Z212" s="9"/>
+      <c r="AA212" s="9"/>
+      <c r="AB212" s="9"/>
+      <c r="AC212" s="9"/>
+      <c r="AD212" s="9"/>
+      <c r="AE212" s="9"/>
+      <c r="AF212" s="9"/>
+      <c r="AG212" s="9"/>
+      <c r="AH212" s="9"/>
+      <c r="AI212" s="9"/>
+      <c r="AJ212" s="9"/>
+      <c r="AK212" s="9"/>
+      <c r="AL212" s="9"/>
+      <c r="AM212" s="9"/>
+      <c r="AN212" s="9"/>
+      <c r="AO212" s="9"/>
+    </row>
+    <row r="213" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W213" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="X213" s="9"/>
+      <c r="Y213" s="9"/>
+      <c r="Z213" s="9"/>
+      <c r="AA213" s="9"/>
+      <c r="AB213" s="9"/>
+      <c r="AC213" s="9"/>
+      <c r="AD213" s="9"/>
+      <c r="AE213" s="9"/>
+      <c r="AF213" s="9"/>
+      <c r="AG213" s="9"/>
+      <c r="AH213" s="9"/>
+      <c r="AI213" s="9"/>
+      <c r="AJ213" s="9"/>
+      <c r="AK213" s="9"/>
+      <c r="AL213" s="9"/>
+      <c r="AM213" s="9"/>
+      <c r="AN213" s="9"/>
+      <c r="AO213" s="9"/>
+    </row>
+    <row r="214" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W214" s="9" t="s">
+        <v>570</v>
+      </c>
+      <c r="X214" s="9"/>
+      <c r="Y214" s="9"/>
+      <c r="Z214" s="9"/>
+      <c r="AA214" s="9"/>
+      <c r="AB214" s="9"/>
+      <c r="AC214" s="9"/>
+      <c r="AD214" s="9"/>
+      <c r="AE214" s="9"/>
+      <c r="AF214" s="9"/>
+      <c r="AG214" s="9"/>
+      <c r="AH214" s="9"/>
+      <c r="AI214" s="9"/>
+      <c r="AJ214" s="9"/>
+      <c r="AK214" s="9"/>
+      <c r="AL214" s="9"/>
+      <c r="AM214" s="9"/>
+      <c r="AN214" s="9"/>
+      <c r="AO214" s="9"/>
+    </row>
+    <row r="215" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W215" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="X215" s="9"/>
+      <c r="Y215" s="9"/>
+      <c r="Z215" s="9"/>
+      <c r="AA215" s="9"/>
+      <c r="AB215" s="9"/>
+      <c r="AC215" s="9"/>
+      <c r="AD215" s="9"/>
+      <c r="AE215" s="9"/>
+      <c r="AF215" s="9"/>
+      <c r="AG215" s="9"/>
+      <c r="AH215" s="9"/>
+      <c r="AI215" s="9"/>
+      <c r="AJ215" s="9"/>
+      <c r="AK215" s="9"/>
+      <c r="AL215" s="9"/>
+      <c r="AM215" s="9"/>
+      <c r="AN215" s="9"/>
+      <c r="AO215" s="9"/>
+    </row>
+    <row r="216" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W216" s="9" t="s">
+        <v>572</v>
+      </c>
+      <c r="X216" s="9"/>
+      <c r="Y216" s="9"/>
+      <c r="Z216" s="9"/>
+      <c r="AA216" s="9"/>
+      <c r="AB216" s="9"/>
+      <c r="AC216" s="9"/>
+      <c r="AD216" s="9"/>
+      <c r="AE216" s="9"/>
+      <c r="AF216" s="9"/>
+      <c r="AG216" s="9"/>
+      <c r="AH216" s="9"/>
+      <c r="AI216" s="9"/>
+      <c r="AJ216" s="9"/>
+      <c r="AK216" s="9"/>
+      <c r="AL216" s="9"/>
+      <c r="AM216" s="9"/>
+      <c r="AN216" s="9"/>
+      <c r="AO216" s="9"/>
+    </row>
+    <row r="217" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W217" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="X217" s="9"/>
+      <c r="Y217" s="9"/>
+      <c r="Z217" s="9"/>
+      <c r="AA217" s="9"/>
+      <c r="AB217" s="9"/>
+      <c r="AC217" s="9"/>
+      <c r="AD217" s="9"/>
+      <c r="AE217" s="9"/>
+      <c r="AF217" s="9"/>
+      <c r="AG217" s="9"/>
+      <c r="AH217" s="9"/>
+      <c r="AI217" s="9"/>
+      <c r="AJ217" s="9"/>
+      <c r="AK217" s="9"/>
+      <c r="AL217" s="9"/>
+      <c r="AM217" s="9"/>
+      <c r="AN217" s="9"/>
+      <c r="AO217" s="9"/>
+    </row>
+    <row r="218" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W218" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="X218" s="9"/>
+      <c r="Y218" s="9"/>
+      <c r="Z218" s="9"/>
+      <c r="AA218" s="9"/>
+      <c r="AB218" s="9"/>
+      <c r="AC218" s="9"/>
+      <c r="AD218" s="9"/>
+      <c r="AE218" s="9"/>
+      <c r="AF218" s="9"/>
+      <c r="AG218" s="9"/>
+      <c r="AH218" s="9"/>
+      <c r="AI218" s="9"/>
+      <c r="AJ218" s="9"/>
+      <c r="AK218" s="9"/>
+      <c r="AL218" s="9"/>
+      <c r="AM218" s="9"/>
+      <c r="AN218" s="9"/>
+      <c r="AO218" s="9"/>
+    </row>
+    <row r="219" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W219" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="X219" s="9"/>
+      <c r="Y219" s="9"/>
+      <c r="Z219" s="9"/>
+      <c r="AA219" s="9"/>
+      <c r="AB219" s="9"/>
+      <c r="AC219" s="9"/>
+      <c r="AD219" s="9"/>
+      <c r="AE219" s="9"/>
+      <c r="AF219" s="9"/>
+      <c r="AG219" s="9"/>
+      <c r="AH219" s="9"/>
+      <c r="AI219" s="9"/>
+      <c r="AJ219" s="9"/>
+      <c r="AK219" s="9"/>
+      <c r="AL219" s="9"/>
+      <c r="AM219" s="9"/>
+      <c r="AN219" s="9"/>
+      <c r="AO219" s="9"/>
+    </row>
+    <row r="220" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W220" s="9"/>
+      <c r="X220" s="9"/>
+      <c r="Y220" s="9"/>
+      <c r="Z220" s="9"/>
+      <c r="AA220" s="9"/>
+      <c r="AB220" s="9"/>
+      <c r="AC220" s="9"/>
+      <c r="AD220" s="9"/>
+      <c r="AE220" s="9"/>
+      <c r="AF220" s="9"/>
+      <c r="AG220" s="9"/>
+      <c r="AH220" s="9"/>
+      <c r="AI220" s="9"/>
+      <c r="AJ220" s="9"/>
+      <c r="AK220" s="9"/>
+      <c r="AL220" s="9"/>
+      <c r="AM220" s="9"/>
+      <c r="AN220" s="9"/>
+      <c r="AO220" s="9"/>
+    </row>
+    <row r="221" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W221" s="9" t="s">
+        <v>574</v>
+      </c>
+      <c r="X221" s="9"/>
+      <c r="Y221" s="9"/>
+      <c r="Z221" s="9"/>
+      <c r="AA221" s="9"/>
+      <c r="AB221" s="9"/>
+      <c r="AC221" s="9"/>
+      <c r="AD221" s="9"/>
+      <c r="AE221" s="9"/>
+      <c r="AF221" s="9"/>
+      <c r="AG221" s="9"/>
+      <c r="AH221" s="9"/>
+      <c r="AI221" s="9"/>
+      <c r="AJ221" s="9"/>
+      <c r="AK221" s="9"/>
+      <c r="AL221" s="9"/>
+      <c r="AM221" s="9"/>
+      <c r="AN221" s="9"/>
+      <c r="AO221" s="9"/>
+    </row>
+    <row r="222" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W222" s="9" t="s">
+        <v>575</v>
+      </c>
+      <c r="X222" s="9"/>
+      <c r="Y222" s="9"/>
+      <c r="Z222" s="9"/>
+      <c r="AA222" s="9"/>
+      <c r="AB222" s="9"/>
+      <c r="AC222" s="9"/>
+      <c r="AD222" s="9"/>
+      <c r="AE222" s="9"/>
+      <c r="AF222" s="9"/>
+      <c r="AG222" s="9"/>
+      <c r="AH222" s="9"/>
+      <c r="AI222" s="9"/>
+      <c r="AJ222" s="9"/>
+      <c r="AK222" s="9"/>
+      <c r="AL222" s="9"/>
+      <c r="AM222" s="9"/>
+      <c r="AN222" s="9"/>
+      <c r="AO222" s="9"/>
+    </row>
+    <row r="223" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W223" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="X223" s="9"/>
+      <c r="Y223" s="9"/>
+      <c r="Z223" s="9"/>
+      <c r="AA223" s="9"/>
+      <c r="AB223" s="9"/>
+      <c r="AC223" s="9"/>
+      <c r="AD223" s="9"/>
+      <c r="AE223" s="9"/>
+      <c r="AF223" s="9"/>
+      <c r="AG223" s="9"/>
+      <c r="AH223" s="9"/>
+      <c r="AI223" s="9"/>
+      <c r="AJ223" s="9"/>
+      <c r="AK223" s="9"/>
+      <c r="AL223" s="9"/>
+      <c r="AM223" s="9"/>
+      <c r="AN223" s="9"/>
+      <c r="AO223" s="9"/>
+    </row>
+    <row r="224" spans="23:41" x14ac:dyDescent="0.4">
+      <c r="W224" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="X224" s="9"/>
+      <c r="Y224" s="9"/>
+      <c r="Z224" s="9"/>
+      <c r="AA224" s="9"/>
+      <c r="AB224" s="9"/>
+      <c r="AC224" s="9"/>
+      <c r="AD224" s="9"/>
+      <c r="AE224" s="9"/>
+      <c r="AF224" s="9"/>
+      <c r="AG224" s="9"/>
+      <c r="AH224" s="9"/>
+      <c r="AI224" s="9"/>
+      <c r="AJ224" s="9"/>
+      <c r="AK224" s="9"/>
+      <c r="AL224" s="9"/>
+      <c r="AM224" s="9"/>
+      <c r="AN224" s="9"/>
+      <c r="AO224" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{9E8104E2-0B1A-498B-A07D-38DAF385409A}"/>
     <hyperlink ref="Q43" r:id="rId2" xr:uid="{C9A864E0-135D-4BC6-BAC2-C835A37D8BD6}"/>
     <hyperlink ref="Q75" r:id="rId3" xr:uid="{B187DD11-D8D8-4A05-B2D5-D669573D0B6D}"/>
+    <hyperlink ref="AL190" r:id="rId4" xr:uid="{0ED352F7-3F7F-466D-A86C-3AFB5310436F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
doc:: 9. Palindrome Number
Leetcode problem 9. Palindrome Number is solved and documented
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C189958-C744-4AE6-A97A-393AF1DC4ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7EAA53-3AF3-469B-B62C-93DE4E24B1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="589">
   <si>
     <t>Title</t>
   </si>
@@ -1983,6 +1983,39 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/find-first-palindromic-string-in-the-array/description/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    bool isPalindrome(int x) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (x &lt; 0) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        long long reversed = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        long long temp = x;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        while (temp != 0) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            int digit = temp % 10;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            reversed = reversed * 10 + digit;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            temp /= 10;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return (reversed == x);</t>
+  </si>
+  <si>
+    <t>9. Palindrome Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-number/description/</t>
   </si>
 </sst>
 </file>
@@ -2864,8 +2897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE91F9C-297C-4D59-9996-90CC520AF8DF}">
   <dimension ref="B1:AK399"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3:AI14"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.77734375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -3726,35 +3759,302 @@
       <c r="R34" s="9"/>
     </row>
     <row r="35" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="36" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="59" t="s">
+        <v>587</v>
+      </c>
+      <c r="L36" s="62" t="s">
+        <v>588</v>
+      </c>
+    </row>
     <row r="37" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="38" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="39" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="40" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="42" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="43" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="44" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="45" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="46" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="47" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="48" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="49" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="50" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="51" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="52" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="53" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="54" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="55" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="56" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="57" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="58" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="59" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="60" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="61" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="62" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="63" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="64" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="38" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+    </row>
+    <row r="39" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+    </row>
+    <row r="40" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+    </row>
+    <row r="41" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="9" t="s">
+        <v>579</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+    </row>
+    <row r="42" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+    </row>
+    <row r="43" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+    </row>
+    <row r="44" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+    </row>
+    <row r="45" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="9" t="s">
+        <v>580</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+    </row>
+    <row r="46" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B46" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+    </row>
+    <row r="47" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+    </row>
+    <row r="48" spans="2:18" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B48" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+    </row>
+    <row r="49" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B49" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+    </row>
+    <row r="50" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B50" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+    </row>
+    <row r="51" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B51" s="9" t="s">
+        <v>585</v>
+      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+    </row>
+    <row r="52" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B52" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+    </row>
+    <row r="53" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+    </row>
+    <row r="54" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B54" s="9" t="s">
+        <v>586</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+    </row>
+    <row r="55" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B55" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+    </row>
+    <row r="56" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B56" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+    </row>
+    <row r="57" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="58" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="59" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="60" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="61" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="62" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="63" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="64" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="65" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="66" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="67" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -4093,9 +4393,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{33BE294A-425B-4A78-9221-04CE79E267EB}"/>
+    <hyperlink ref="L36" r:id="rId2" xr:uid="{DB450F9D-0310-4013-8ECA-9DEA9F8AB182}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -9030,8 +9331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28504ADD-8E4E-436B-849F-525BA36E82D6}">
   <dimension ref="A2:HD224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U187" workbookViewId="0">
-      <selection activeCell="AL191" sqref="AL191"/>
+    <sheetView topLeftCell="A222" workbookViewId="0">
+      <selection activeCell="AU178" sqref="AU178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
doc:: 2843. Count Symmetric Integers
leetcode problem 2843. Count Symmetric Integers is solved and documented
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7EAA53-3AF3-469B-B62C-93DE4E24B1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953652EB-3561-4C21-8CED-8424B2786319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="608">
   <si>
     <t>Title</t>
   </si>
@@ -2016,6 +2016,63 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/palindrome-number/description/</t>
+  </si>
+  <si>
+    <t>2843. Count Symmetric Integers</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/count-symmetric-integers/description/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int countSymmetricIntegers(int low, int high) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       int cnt = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        for(int i = low; i &lt;= high; i++)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            string str = to_string(i);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            if(str.size() % 2 == 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                int l = 0 , h = str.size() - 1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                int lS = 0 , hS = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                while(l &lt; h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    lS += (int)str[l];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    hS += (int)str[h];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    l++;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    h--;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                if(lS == hS) cnt++;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return cnt;</t>
   </si>
 </sst>
 </file>
@@ -2408,7 +2465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2580,6 +2637,7 @@
     <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2897,8 +2955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE91F9C-297C-4D59-9996-90CC520AF8DF}">
   <dimension ref="B1:AK399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="Q60" sqref="Q60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.77734375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -3929,7 +3987,7 @@
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
     </row>
-    <row r="49" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B49" s="9" t="s">
         <v>583</v>
       </c>
@@ -3944,7 +4002,7 @@
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
     </row>
-    <row r="50" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B50" s="9" t="s">
         <v>584</v>
       </c>
@@ -3959,7 +4017,7 @@
       <c r="K50" s="9"/>
       <c r="L50" s="9"/>
     </row>
-    <row r="51" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B51" s="9" t="s">
         <v>585</v>
       </c>
@@ -3974,7 +4032,7 @@
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
     </row>
-    <row r="52" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B52" s="9" t="s">
         <v>202</v>
       </c>
@@ -3989,7 +4047,7 @@
       <c r="K52" s="9"/>
       <c r="L52" s="9"/>
     </row>
-    <row r="53" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
@@ -4002,7 +4060,7 @@
       <c r="K53" s="9"/>
       <c r="L53" s="9"/>
     </row>
-    <row r="54" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B54" s="9" t="s">
         <v>586</v>
       </c>
@@ -4017,7 +4075,7 @@
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
     </row>
-    <row r="55" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B55" s="9" t="s">
         <v>48</v>
       </c>
@@ -4032,7 +4090,7 @@
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
     </row>
-    <row r="56" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B56" s="9" t="s">
         <v>299</v>
       </c>
@@ -4047,46 +4105,451 @@
       <c r="K56" s="9"/>
       <c r="L56" s="9"/>
     </row>
-    <row r="57" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="58" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="59" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="60" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="61" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="62" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="63" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="64" spans="2:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="65" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="66" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="67" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="68" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="69" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="70" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="71" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="72" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="73" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="74" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="75" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="76" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="77" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="78" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="79" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="80" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="81" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="82" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="83" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="84" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="85" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="86" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="87" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="88" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="89" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="90" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="91" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="92" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="93" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="94" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="95" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="96" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="57" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="58" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B58" s="65" t="s">
+        <v>589</v>
+      </c>
+      <c r="M58" s="62" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="60" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B60" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
+    </row>
+    <row r="61" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B61" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
+      <c r="L61" s="9"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="9"/>
+    </row>
+    <row r="62" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B62" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+      <c r="N62" s="9"/>
+    </row>
+    <row r="63" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B63" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="9"/>
+    </row>
+    <row r="64" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
+    </row>
+    <row r="65" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B65" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="9"/>
+    </row>
+    <row r="66" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B66" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="9"/>
+    </row>
+    <row r="67" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B67" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="9"/>
+    </row>
+    <row r="68" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B68" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
+    </row>
+    <row r="69" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B69" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9"/>
+    </row>
+    <row r="70" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B70" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="9"/>
+    </row>
+    <row r="71" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B71" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="9"/>
+    </row>
+    <row r="72" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B72" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="9"/>
+    </row>
+    <row r="73" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B73" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="9"/>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
+    </row>
+    <row r="74" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B74" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="9"/>
+      <c r="J74" s="9"/>
+      <c r="K74" s="9"/>
+      <c r="L74" s="9"/>
+      <c r="M74" s="9"/>
+      <c r="N74" s="9"/>
+    </row>
+    <row r="75" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B75" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
+      <c r="J75" s="9"/>
+      <c r="K75" s="9"/>
+      <c r="L75" s="9"/>
+      <c r="M75" s="9"/>
+      <c r="N75" s="9"/>
+    </row>
+    <row r="76" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B76" s="9" t="s">
+        <v>604</v>
+      </c>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9"/>
+      <c r="K76" s="9"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="9"/>
+      <c r="N76" s="9"/>
+    </row>
+    <row r="77" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B77" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="9"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="9"/>
+      <c r="N77" s="9"/>
+    </row>
+    <row r="78" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B78" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="9"/>
+    </row>
+    <row r="79" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B79" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9"/>
+      <c r="K79" s="9"/>
+      <c r="L79" s="9"/>
+      <c r="M79" s="9"/>
+      <c r="N79" s="9"/>
+    </row>
+    <row r="80" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B80" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="9"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="9"/>
+      <c r="M80" s="9"/>
+      <c r="N80" s="9"/>
+    </row>
+    <row r="81" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B81" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="9"/>
+      <c r="K81" s="9"/>
+      <c r="L81" s="9"/>
+      <c r="M81" s="9"/>
+      <c r="N81" s="9"/>
+    </row>
+    <row r="82" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B82" s="9" t="s">
+        <v>607</v>
+      </c>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="9"/>
+      <c r="J82" s="9"/>
+      <c r="K82" s="9"/>
+      <c r="L82" s="9"/>
+      <c r="M82" s="9"/>
+      <c r="N82" s="9"/>
+    </row>
+    <row r="83" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B83" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+      <c r="I83" s="9"/>
+      <c r="J83" s="9"/>
+      <c r="K83" s="9"/>
+      <c r="L83" s="9"/>
+      <c r="M83" s="9"/>
+      <c r="N83" s="9"/>
+    </row>
+    <row r="84" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B84" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+      <c r="I84" s="9"/>
+      <c r="J84" s="9"/>
+      <c r="K84" s="9"/>
+      <c r="L84" s="9"/>
+      <c r="M84" s="9"/>
+      <c r="N84" s="9"/>
+    </row>
+    <row r="85" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="86" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="87" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="88" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="89" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="90" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="91" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="92" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="93" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="94" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="95" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="96" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="97" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="98" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="99" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -4394,9 +4857,10 @@
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{33BE294A-425B-4A78-9221-04CE79E267EB}"/>
     <hyperlink ref="L36" r:id="rId2" xr:uid="{DB450F9D-0310-4013-8ECA-9DEA9F8AB182}"/>
+    <hyperlink ref="M58" r:id="rId3" xr:uid="{D7DFAD62-63DB-4ADD-A243-4CF38BA9FEEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
doc:: 195. Tenth Line
Shell prob is solved
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{953652EB-3561-4C21-8CED-8424B2786319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4694066-F504-46B3-90C8-C3799243F854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple" sheetId="4" r:id="rId1"/>
-    <sheet name="A" sheetId="1" r:id="rId2"/>
-    <sheet name="S" sheetId="3" r:id="rId3"/>
-    <sheet name="Format" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="A" sheetId="1" r:id="rId3"/>
+    <sheet name="S" sheetId="3" r:id="rId4"/>
+    <sheet name="Format" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="611">
   <si>
     <t>Title</t>
   </si>
@@ -2074,12 +2075,41 @@
   <si>
     <t xml:space="preserve">        return cnt;</t>
   </si>
+  <si>
+    <t>195. Tenth Line</t>
+  </si>
+  <si>
+    <t># Read from the file file.txt and output the tenth line to stdout.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'10q;d'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> file.txt</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2260,6 +2290,32 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF6A9955"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="19">
@@ -2465,7 +2521,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2637,7 +2693,13 @@
     <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2955,7 +3017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE91F9C-297C-4D59-9996-90CC520AF8DF}">
   <dimension ref="B1:AK399"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="Q60" sqref="Q60"/>
     </sheetView>
   </sheetViews>
@@ -4107,7 +4169,7 @@
     </row>
     <row r="57" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="58" spans="2:14" ht="22.05" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B58" s="65" t="s">
+      <c r="B58" s="59" t="s">
         <v>589</v>
       </c>
       <c r="M58" s="62" t="s">
@@ -4865,6 +4927,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A920F7B1-1471-4C74-8E69-EC4893BF0553}">
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="65" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="66" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="67" t="s">
+        <v>610</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE6A8EE-45F0-4DFE-8B47-A80E55C53C69}">
   <dimension ref="B1:AP399"/>
   <sheetViews>
@@ -9791,7 +9883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28504ADD-8E4E-436B-849F-525BA36E82D6}">
   <dimension ref="A2:HD224"/>
   <sheetViews>
@@ -21708,7 +21800,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AB2F21-1695-41F3-AD6E-505367934BD2}">
   <dimension ref="B1:AP84"/>
   <sheetViews>

</xml_diff>

<commit_message>
doc:: 193. Valid Phone Numbers
Leetcode problem 193. Valid Phone Numbers is solved and documented
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4694066-F504-46B3-90C8-C3799243F854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2070F5-5E6A-4B10-9C2A-08815E8C062B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="614">
   <si>
     <t>Title</t>
   </si>
@@ -2103,6 +2103,35 @@
       </rPr>
       <t xml:space="preserve"> file.txt</t>
     </r>
+  </si>
+  <si>
+    <t># Read from the file file.txt and output all valid phone numbers to stdout.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">awk </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFCE9178"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'/^([0-9]{3}-|\([0-9]{3}\) )[0-9]{3}-[0-9]{4}$/'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> file.txt</t>
+    </r>
+  </si>
+  <si>
+    <t>193. Valid Phone Numbers</t>
   </si>
 </sst>
 </file>
@@ -4928,10 +4957,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A920F7B1-1471-4C74-8E69-EC4893BF0553}">
-  <dimension ref="B2:B4"/>
+  <dimension ref="B2:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4951,7 +4980,25 @@
         <v>610</v>
       </c>
     </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B6" s="62" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B7" s="66" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B8" s="67" t="s">
+        <v>612</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" display="https://leetcode.com/problems/valid-phone-numbers/" xr:uid="{55113FAE-8B46-4B3C-ACFA-F5E1DEEE61A1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
doc:: 168. Excel Sheet Column Title
Leetcode problem 168. Excel Sheet Column Title is solved and documented
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2070F5-5E6A-4B10-9C2A-08815E8C062B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDC906A-B03C-448A-BE91-F0951B6E995F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="622">
   <si>
     <t>Title</t>
   </si>
@@ -2132,6 +2132,30 @@
   </si>
   <si>
     <t>193. Valid Phone Numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    string convertToTitle(int columnNumber) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        string result = "";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        while (columnNumber &gt; 0) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            columnNumber--;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            result = char(columnNumber % 26 + 'A') + result;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            columnNumber /= 26;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return result;</t>
+  </si>
+  <si>
+    <t>168. Excel Sheet Column Title</t>
   </si>
 </sst>
 </file>
@@ -4959,8 +4983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A920F7B1-1471-4C74-8E69-EC4893BF0553}">
   <dimension ref="B2:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9932,10 +9956,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28504ADD-8E4E-436B-849F-525BA36E82D6}">
-  <dimension ref="A2:HD224"/>
+  <dimension ref="A2:HD239"/>
   <sheetViews>
-    <sheetView topLeftCell="A222" workbookViewId="0">
-      <selection activeCell="AU178" sqref="AU178"/>
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="C226" sqref="C226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -21835,15 +21859,249 @@
       <c r="AN224" s="9"/>
       <c r="AO224" s="9"/>
     </row>
+    <row r="226" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="C226" s="62" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="228" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B228" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C228" s="9"/>
+      <c r="D228" s="9"/>
+      <c r="E228" s="9"/>
+      <c r="F228" s="9"/>
+      <c r="G228" s="9"/>
+      <c r="H228" s="9"/>
+      <c r="I228" s="9"/>
+      <c r="J228" s="9"/>
+      <c r="K228" s="9"/>
+      <c r="L228" s="9"/>
+      <c r="M228" s="9"/>
+      <c r="N228" s="9"/>
+      <c r="O228" s="9"/>
+      <c r="P228" s="9"/>
+    </row>
+    <row r="229" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B229" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C229" s="9"/>
+      <c r="D229" s="9"/>
+      <c r="E229" s="9"/>
+      <c r="F229" s="9"/>
+      <c r="G229" s="9"/>
+      <c r="H229" s="9"/>
+      <c r="I229" s="9"/>
+      <c r="J229" s="9"/>
+      <c r="K229" s="9"/>
+      <c r="L229" s="9"/>
+      <c r="M229" s="9"/>
+      <c r="N229" s="9"/>
+      <c r="O229" s="9"/>
+      <c r="P229" s="9"/>
+    </row>
+    <row r="230" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B230" s="9" t="s">
+        <v>614</v>
+      </c>
+      <c r="C230" s="9"/>
+      <c r="D230" s="9"/>
+      <c r="E230" s="9"/>
+      <c r="F230" s="9"/>
+      <c r="G230" s="9"/>
+      <c r="H230" s="9"/>
+      <c r="I230" s="9"/>
+      <c r="J230" s="9"/>
+      <c r="K230" s="9"/>
+      <c r="L230" s="9"/>
+      <c r="M230" s="9"/>
+      <c r="N230" s="9"/>
+      <c r="O230" s="9"/>
+      <c r="P230" s="9"/>
+    </row>
+    <row r="231" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B231" s="9" t="s">
+        <v>615</v>
+      </c>
+      <c r="C231" s="9"/>
+      <c r="D231" s="9"/>
+      <c r="E231" s="9"/>
+      <c r="F231" s="9"/>
+      <c r="G231" s="9"/>
+      <c r="H231" s="9"/>
+      <c r="I231" s="9"/>
+      <c r="J231" s="9"/>
+      <c r="K231" s="9"/>
+      <c r="L231" s="9"/>
+      <c r="M231" s="9"/>
+      <c r="N231" s="9"/>
+      <c r="O231" s="9"/>
+      <c r="P231" s="9"/>
+    </row>
+    <row r="232" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B232" s="9" t="s">
+        <v>616</v>
+      </c>
+      <c r="C232" s="9"/>
+      <c r="D232" s="9"/>
+      <c r="E232" s="9"/>
+      <c r="F232" s="9"/>
+      <c r="G232" s="9"/>
+      <c r="H232" s="9"/>
+      <c r="I232" s="9"/>
+      <c r="J232" s="9"/>
+      <c r="K232" s="9"/>
+      <c r="L232" s="9"/>
+      <c r="M232" s="9"/>
+      <c r="N232" s="9"/>
+      <c r="O232" s="9"/>
+      <c r="P232" s="9"/>
+    </row>
+    <row r="233" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B233" s="9" t="s">
+        <v>617</v>
+      </c>
+      <c r="C233" s="9"/>
+      <c r="D233" s="9"/>
+      <c r="E233" s="9"/>
+      <c r="F233" s="9"/>
+      <c r="G233" s="9"/>
+      <c r="H233" s="9"/>
+      <c r="I233" s="9"/>
+      <c r="J233" s="9"/>
+      <c r="K233" s="9"/>
+      <c r="L233" s="9"/>
+      <c r="M233" s="9"/>
+      <c r="N233" s="9"/>
+      <c r="O233" s="9"/>
+      <c r="P233" s="9"/>
+    </row>
+    <row r="234" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B234" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="C234" s="9"/>
+      <c r="D234" s="9"/>
+      <c r="E234" s="9"/>
+      <c r="F234" s="9"/>
+      <c r="G234" s="9"/>
+      <c r="H234" s="9"/>
+      <c r="I234" s="9"/>
+      <c r="J234" s="9"/>
+      <c r="K234" s="9"/>
+      <c r="L234" s="9"/>
+      <c r="M234" s="9"/>
+      <c r="N234" s="9"/>
+      <c r="O234" s="9"/>
+      <c r="P234" s="9"/>
+    </row>
+    <row r="235" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B235" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="C235" s="9"/>
+      <c r="D235" s="9"/>
+      <c r="E235" s="9"/>
+      <c r="F235" s="9"/>
+      <c r="G235" s="9"/>
+      <c r="H235" s="9"/>
+      <c r="I235" s="9"/>
+      <c r="J235" s="9"/>
+      <c r="K235" s="9"/>
+      <c r="L235" s="9"/>
+      <c r="M235" s="9"/>
+      <c r="N235" s="9"/>
+      <c r="O235" s="9"/>
+      <c r="P235" s="9"/>
+    </row>
+    <row r="236" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B236" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C236" s="9"/>
+      <c r="D236" s="9"/>
+      <c r="E236" s="9"/>
+      <c r="F236" s="9"/>
+      <c r="G236" s="9"/>
+      <c r="H236" s="9"/>
+      <c r="I236" s="9"/>
+      <c r="J236" s="9"/>
+      <c r="K236" s="9"/>
+      <c r="L236" s="9"/>
+      <c r="M236" s="9"/>
+      <c r="N236" s="9"/>
+      <c r="O236" s="9"/>
+      <c r="P236" s="9"/>
+    </row>
+    <row r="237" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B237" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="C237" s="9"/>
+      <c r="D237" s="9"/>
+      <c r="E237" s="9"/>
+      <c r="F237" s="9"/>
+      <c r="G237" s="9"/>
+      <c r="H237" s="9"/>
+      <c r="I237" s="9"/>
+      <c r="J237" s="9"/>
+      <c r="K237" s="9"/>
+      <c r="L237" s="9"/>
+      <c r="M237" s="9"/>
+      <c r="N237" s="9"/>
+      <c r="O237" s="9"/>
+      <c r="P237" s="9"/>
+    </row>
+    <row r="238" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B238" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C238" s="9"/>
+      <c r="D238" s="9"/>
+      <c r="E238" s="9"/>
+      <c r="F238" s="9"/>
+      <c r="G238" s="9"/>
+      <c r="H238" s="9"/>
+      <c r="I238" s="9"/>
+      <c r="J238" s="9"/>
+      <c r="K238" s="9"/>
+      <c r="L238" s="9"/>
+      <c r="M238" s="9"/>
+      <c r="N238" s="9"/>
+      <c r="O238" s="9"/>
+      <c r="P238" s="9"/>
+    </row>
+    <row r="239" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B239" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C239" s="9"/>
+      <c r="D239" s="9"/>
+      <c r="E239" s="9"/>
+      <c r="F239" s="9"/>
+      <c r="G239" s="9"/>
+      <c r="H239" s="9"/>
+      <c r="I239" s="9"/>
+      <c r="J239" s="9"/>
+      <c r="K239" s="9"/>
+      <c r="L239" s="9"/>
+      <c r="M239" s="9"/>
+      <c r="N239" s="9"/>
+      <c r="O239" s="9"/>
+      <c r="P239" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{9E8104E2-0B1A-498B-A07D-38DAF385409A}"/>
     <hyperlink ref="Q43" r:id="rId2" xr:uid="{C9A864E0-135D-4BC6-BAC2-C835A37D8BD6}"/>
     <hyperlink ref="Q75" r:id="rId3" xr:uid="{B187DD11-D8D8-4A05-B2D5-D669573D0B6D}"/>
     <hyperlink ref="AL190" r:id="rId4" xr:uid="{0ED352F7-3F7F-466D-A86C-3AFB5310436F}"/>
+    <hyperlink ref="C226" r:id="rId5" display="https://leetcode.com/problems/excel-sheet-column-title/" xr:uid="{5EE1CF6B-190D-452F-B940-D9C579EC7E33}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
doc :: 171. Excel Sheet Column Number
Leetcode problem 171. Excel Sheet Column Number is solved and documented
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDC906A-B03C-448A-BE91-F0951B6E995F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145B4C0A-30B4-4D85-9B42-D3EC5640E0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="629">
   <si>
     <t>Title</t>
   </si>
@@ -2156,6 +2156,27 @@
   </si>
   <si>
     <t>168. Excel Sheet Column Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int titleToNumber(string columnTitle) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int result = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        for(char c : columnTitle)</t>
+  </si>
+  <si>
+    <t>//d = s[i](char) - 'A' + 1 (we used  s[i] -  'A' to convert the letter to a number like it's going to be C)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            int d = c - 'A' + 1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            result = result * 26 + d;</t>
+  </si>
+  <si>
+    <t>171. Excel Sheet Column Number</t>
   </si>
 </sst>
 </file>
@@ -9956,10 +9977,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28504ADD-8E4E-436B-849F-525BA36E82D6}">
-  <dimension ref="A2:HD239"/>
+  <dimension ref="A2:HD256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="C226" sqref="C226"/>
+    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="P228" sqref="P228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -21860,7 +21881,7 @@
       <c r="AO224" s="9"/>
     </row>
     <row r="226" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="C226" s="62" t="s">
+      <c r="B226" s="60" t="s">
         <v>621</v>
       </c>
     </row>
@@ -22092,16 +22113,468 @@
       <c r="O239" s="9"/>
       <c r="P239" s="9"/>
     </row>
+    <row r="241" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B241" s="60" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="243" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B243" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C243" s="9"/>
+      <c r="D243" s="9"/>
+      <c r="E243" s="9"/>
+      <c r="F243" s="9"/>
+      <c r="G243" s="9"/>
+      <c r="H243" s="9"/>
+      <c r="I243" s="9"/>
+      <c r="J243" s="9"/>
+      <c r="K243" s="9"/>
+      <c r="L243" s="9"/>
+      <c r="M243" s="9"/>
+      <c r="N243" s="9"/>
+      <c r="O243" s="9"/>
+      <c r="P243" s="9"/>
+      <c r="Q243" s="9"/>
+      <c r="R243" s="9"/>
+      <c r="S243" s="9"/>
+      <c r="T243" s="9"/>
+      <c r="U243" s="9"/>
+      <c r="V243" s="9"/>
+      <c r="W243" s="9"/>
+      <c r="X243" s="9"/>
+      <c r="Y243" s="9"/>
+      <c r="Z243" s="9"/>
+      <c r="AA243" s="9"/>
+      <c r="AB243" s="9"/>
+      <c r="AC243" s="9"/>
+    </row>
+    <row r="244" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B244" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C244" s="9"/>
+      <c r="D244" s="9"/>
+      <c r="E244" s="9"/>
+      <c r="F244" s="9"/>
+      <c r="G244" s="9"/>
+      <c r="H244" s="9"/>
+      <c r="I244" s="9"/>
+      <c r="J244" s="9"/>
+      <c r="K244" s="9"/>
+      <c r="L244" s="9"/>
+      <c r="M244" s="9"/>
+      <c r="N244" s="9"/>
+      <c r="O244" s="9"/>
+      <c r="P244" s="9"/>
+      <c r="Q244" s="9"/>
+      <c r="R244" s="9"/>
+      <c r="S244" s="9"/>
+      <c r="T244" s="9"/>
+      <c r="U244" s="9"/>
+      <c r="V244" s="9"/>
+      <c r="W244" s="9"/>
+      <c r="X244" s="9"/>
+      <c r="Y244" s="9"/>
+      <c r="Z244" s="9"/>
+      <c r="AA244" s="9"/>
+      <c r="AB244" s="9"/>
+      <c r="AC244" s="9"/>
+    </row>
+    <row r="245" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B245" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="C245" s="9"/>
+      <c r="D245" s="9"/>
+      <c r="E245" s="9"/>
+      <c r="F245" s="9"/>
+      <c r="G245" s="9"/>
+      <c r="H245" s="9"/>
+      <c r="I245" s="9"/>
+      <c r="J245" s="9"/>
+      <c r="K245" s="9"/>
+      <c r="L245" s="9"/>
+      <c r="M245" s="9"/>
+      <c r="N245" s="9"/>
+      <c r="O245" s="9"/>
+      <c r="P245" s="9"/>
+      <c r="Q245" s="9"/>
+      <c r="R245" s="9"/>
+      <c r="S245" s="9"/>
+      <c r="T245" s="9"/>
+      <c r="U245" s="9"/>
+      <c r="V245" s="9"/>
+      <c r="W245" s="9"/>
+      <c r="X245" s="9"/>
+      <c r="Y245" s="9"/>
+      <c r="Z245" s="9"/>
+      <c r="AA245" s="9"/>
+      <c r="AB245" s="9"/>
+      <c r="AC245" s="9"/>
+    </row>
+    <row r="246" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B246" s="9" t="s">
+        <v>623</v>
+      </c>
+      <c r="C246" s="9"/>
+      <c r="D246" s="9"/>
+      <c r="E246" s="9"/>
+      <c r="F246" s="9"/>
+      <c r="G246" s="9"/>
+      <c r="H246" s="9"/>
+      <c r="I246" s="9"/>
+      <c r="J246" s="9"/>
+      <c r="K246" s="9"/>
+      <c r="L246" s="9"/>
+      <c r="M246" s="9"/>
+      <c r="N246" s="9"/>
+      <c r="O246" s="9"/>
+      <c r="P246" s="9"/>
+      <c r="Q246" s="9"/>
+      <c r="R246" s="9"/>
+      <c r="S246" s="9"/>
+      <c r="T246" s="9"/>
+      <c r="U246" s="9"/>
+      <c r="V246" s="9"/>
+      <c r="W246" s="9"/>
+      <c r="X246" s="9"/>
+      <c r="Y246" s="9"/>
+      <c r="Z246" s="9"/>
+      <c r="AA246" s="9"/>
+      <c r="AB246" s="9"/>
+      <c r="AC246" s="9"/>
+    </row>
+    <row r="247" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B247" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="C247" s="9"/>
+      <c r="D247" s="9"/>
+      <c r="E247" s="9"/>
+      <c r="F247" s="9"/>
+      <c r="G247" s="9"/>
+      <c r="H247" s="9"/>
+      <c r="I247" s="9"/>
+      <c r="J247" s="9"/>
+      <c r="K247" s="9"/>
+      <c r="L247" s="9"/>
+      <c r="M247" s="9"/>
+      <c r="N247" s="9"/>
+      <c r="O247" s="9"/>
+      <c r="P247" s="9"/>
+      <c r="Q247" s="9"/>
+      <c r="R247" s="9"/>
+      <c r="S247" s="9"/>
+      <c r="T247" s="9"/>
+      <c r="U247" s="9"/>
+      <c r="V247" s="9"/>
+      <c r="W247" s="9"/>
+      <c r="X247" s="9"/>
+      <c r="Y247" s="9"/>
+      <c r="Z247" s="9"/>
+      <c r="AA247" s="9"/>
+      <c r="AB247" s="9"/>
+      <c r="AC247" s="9"/>
+    </row>
+    <row r="248" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B248" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="C248" s="9"/>
+      <c r="D248" s="9"/>
+      <c r="E248" s="9"/>
+      <c r="F248" s="9"/>
+      <c r="G248" s="9"/>
+      <c r="H248" s="9"/>
+      <c r="I248" s="9"/>
+      <c r="J248" s="9"/>
+      <c r="K248" s="9"/>
+      <c r="L248" s="9"/>
+      <c r="M248" s="9"/>
+      <c r="N248" s="9"/>
+      <c r="O248" s="9"/>
+      <c r="P248" s="9"/>
+      <c r="Q248" s="9"/>
+      <c r="R248" s="9"/>
+      <c r="S248" s="9"/>
+      <c r="T248" s="9"/>
+      <c r="U248" s="9"/>
+      <c r="V248" s="9"/>
+      <c r="W248" s="9"/>
+      <c r="X248" s="9"/>
+      <c r="Y248" s="9"/>
+      <c r="Z248" s="9"/>
+      <c r="AA248" s="9"/>
+      <c r="AB248" s="9"/>
+      <c r="AC248" s="9"/>
+    </row>
+    <row r="249" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B249" s="9"/>
+      <c r="C249" s="9"/>
+      <c r="D249" s="9"/>
+      <c r="E249" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="F249" s="9"/>
+      <c r="G249" s="9"/>
+      <c r="H249" s="9"/>
+      <c r="I249" s="9"/>
+      <c r="J249" s="9"/>
+      <c r="K249" s="9"/>
+      <c r="L249" s="9"/>
+      <c r="M249" s="9"/>
+      <c r="N249" s="9"/>
+      <c r="O249" s="9"/>
+      <c r="P249" s="9"/>
+      <c r="Q249" s="9"/>
+      <c r="R249" s="9"/>
+      <c r="S249" s="9"/>
+      <c r="T249" s="9"/>
+      <c r="U249" s="9"/>
+      <c r="V249" s="9"/>
+      <c r="W249" s="9"/>
+      <c r="X249" s="9"/>
+      <c r="Y249" s="9"/>
+      <c r="Z249" s="9"/>
+      <c r="AA249" s="9"/>
+      <c r="AB249" s="9"/>
+      <c r="AC249" s="9"/>
+    </row>
+    <row r="250" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B250" s="9"/>
+      <c r="C250" s="9"/>
+      <c r="D250" s="9"/>
+      <c r="E250" s="9"/>
+      <c r="F250" s="9"/>
+      <c r="G250" s="9"/>
+      <c r="H250" s="9"/>
+      <c r="I250" s="9"/>
+      <c r="J250" s="9"/>
+      <c r="K250" s="9"/>
+      <c r="L250" s="9"/>
+      <c r="M250" s="9"/>
+      <c r="N250" s="9"/>
+      <c r="O250" s="9"/>
+      <c r="P250" s="9"/>
+      <c r="Q250" s="9"/>
+      <c r="R250" s="9"/>
+      <c r="S250" s="9"/>
+      <c r="T250" s="9"/>
+      <c r="U250" s="9"/>
+      <c r="V250" s="9"/>
+      <c r="W250" s="9"/>
+      <c r="X250" s="9"/>
+      <c r="Y250" s="9"/>
+      <c r="Z250" s="9"/>
+      <c r="AA250" s="9"/>
+      <c r="AB250" s="9"/>
+      <c r="AC250" s="9"/>
+    </row>
+    <row r="251" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B251" s="9" t="s">
+        <v>626</v>
+      </c>
+      <c r="C251" s="9"/>
+      <c r="D251" s="9"/>
+      <c r="E251" s="9"/>
+      <c r="F251" s="9"/>
+      <c r="G251" s="9"/>
+      <c r="H251" s="9"/>
+      <c r="I251" s="9"/>
+      <c r="J251" s="9"/>
+      <c r="K251" s="9"/>
+      <c r="L251" s="9"/>
+      <c r="M251" s="9"/>
+      <c r="N251" s="9"/>
+      <c r="O251" s="9"/>
+      <c r="P251" s="9"/>
+      <c r="Q251" s="9"/>
+      <c r="R251" s="9"/>
+      <c r="S251" s="9"/>
+      <c r="T251" s="9"/>
+      <c r="U251" s="9"/>
+      <c r="V251" s="9"/>
+      <c r="W251" s="9"/>
+      <c r="X251" s="9"/>
+      <c r="Y251" s="9"/>
+      <c r="Z251" s="9"/>
+      <c r="AA251" s="9"/>
+      <c r="AB251" s="9"/>
+      <c r="AC251" s="9"/>
+    </row>
+    <row r="252" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B252" s="9" t="s">
+        <v>627</v>
+      </c>
+      <c r="C252" s="9"/>
+      <c r="D252" s="9"/>
+      <c r="E252" s="9"/>
+      <c r="F252" s="9"/>
+      <c r="G252" s="9"/>
+      <c r="H252" s="9"/>
+      <c r="I252" s="9"/>
+      <c r="J252" s="9"/>
+      <c r="K252" s="9"/>
+      <c r="L252" s="9"/>
+      <c r="M252" s="9"/>
+      <c r="N252" s="9"/>
+      <c r="O252" s="9"/>
+      <c r="P252" s="9"/>
+      <c r="Q252" s="9"/>
+      <c r="R252" s="9"/>
+      <c r="S252" s="9"/>
+      <c r="T252" s="9"/>
+      <c r="U252" s="9"/>
+      <c r="V252" s="9"/>
+      <c r="W252" s="9"/>
+      <c r="X252" s="9"/>
+      <c r="Y252" s="9"/>
+      <c r="Z252" s="9"/>
+      <c r="AA252" s="9"/>
+      <c r="AB252" s="9"/>
+      <c r="AC252" s="9"/>
+    </row>
+    <row r="253" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B253" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C253" s="9"/>
+      <c r="D253" s="9"/>
+      <c r="E253" s="9"/>
+      <c r="F253" s="9"/>
+      <c r="G253" s="9"/>
+      <c r="H253" s="9"/>
+      <c r="I253" s="9"/>
+      <c r="J253" s="9"/>
+      <c r="K253" s="9"/>
+      <c r="L253" s="9"/>
+      <c r="M253" s="9"/>
+      <c r="N253" s="9"/>
+      <c r="O253" s="9"/>
+      <c r="P253" s="9"/>
+      <c r="Q253" s="9"/>
+      <c r="R253" s="9"/>
+      <c r="S253" s="9"/>
+      <c r="T253" s="9"/>
+      <c r="U253" s="9"/>
+      <c r="V253" s="9"/>
+      <c r="W253" s="9"/>
+      <c r="X253" s="9"/>
+      <c r="Y253" s="9"/>
+      <c r="Z253" s="9"/>
+      <c r="AA253" s="9"/>
+      <c r="AB253" s="9"/>
+      <c r="AC253" s="9"/>
+    </row>
+    <row r="254" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B254" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="C254" s="9"/>
+      <c r="D254" s="9"/>
+      <c r="E254" s="9"/>
+      <c r="F254" s="9"/>
+      <c r="G254" s="9"/>
+      <c r="H254" s="9"/>
+      <c r="I254" s="9"/>
+      <c r="J254" s="9"/>
+      <c r="K254" s="9"/>
+      <c r="L254" s="9"/>
+      <c r="M254" s="9"/>
+      <c r="N254" s="9"/>
+      <c r="O254" s="9"/>
+      <c r="P254" s="9"/>
+      <c r="Q254" s="9"/>
+      <c r="R254" s="9"/>
+      <c r="S254" s="9"/>
+      <c r="T254" s="9"/>
+      <c r="U254" s="9"/>
+      <c r="V254" s="9"/>
+      <c r="W254" s="9"/>
+      <c r="X254" s="9"/>
+      <c r="Y254" s="9"/>
+      <c r="Z254" s="9"/>
+      <c r="AA254" s="9"/>
+      <c r="AB254" s="9"/>
+      <c r="AC254" s="9"/>
+    </row>
+    <row r="255" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B255" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C255" s="9"/>
+      <c r="D255" s="9"/>
+      <c r="E255" s="9"/>
+      <c r="F255" s="9"/>
+      <c r="G255" s="9"/>
+      <c r="H255" s="9"/>
+      <c r="I255" s="9"/>
+      <c r="J255" s="9"/>
+      <c r="K255" s="9"/>
+      <c r="L255" s="9"/>
+      <c r="M255" s="9"/>
+      <c r="N255" s="9"/>
+      <c r="O255" s="9"/>
+      <c r="P255" s="9"/>
+      <c r="Q255" s="9"/>
+      <c r="R255" s="9"/>
+      <c r="S255" s="9"/>
+      <c r="T255" s="9"/>
+      <c r="U255" s="9"/>
+      <c r="V255" s="9"/>
+      <c r="W255" s="9"/>
+      <c r="X255" s="9"/>
+      <c r="Y255" s="9"/>
+      <c r="Z255" s="9"/>
+      <c r="AA255" s="9"/>
+      <c r="AB255" s="9"/>
+      <c r="AC255" s="9"/>
+    </row>
+    <row r="256" spans="2:29" x14ac:dyDescent="0.4">
+      <c r="B256" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C256" s="9"/>
+      <c r="D256" s="9"/>
+      <c r="E256" s="9"/>
+      <c r="F256" s="9"/>
+      <c r="G256" s="9"/>
+      <c r="H256" s="9"/>
+      <c r="I256" s="9"/>
+      <c r="J256" s="9"/>
+      <c r="K256" s="9"/>
+      <c r="L256" s="9"/>
+      <c r="M256" s="9"/>
+      <c r="N256" s="9"/>
+      <c r="O256" s="9"/>
+      <c r="P256" s="9"/>
+      <c r="Q256" s="9"/>
+      <c r="R256" s="9"/>
+      <c r="S256" s="9"/>
+      <c r="T256" s="9"/>
+      <c r="U256" s="9"/>
+      <c r="V256" s="9"/>
+      <c r="W256" s="9"/>
+      <c r="X256" s="9"/>
+      <c r="Y256" s="9"/>
+      <c r="Z256" s="9"/>
+      <c r="AA256" s="9"/>
+      <c r="AB256" s="9"/>
+      <c r="AC256" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{9E8104E2-0B1A-498B-A07D-38DAF385409A}"/>
     <hyperlink ref="Q43" r:id="rId2" xr:uid="{C9A864E0-135D-4BC6-BAC2-C835A37D8BD6}"/>
     <hyperlink ref="Q75" r:id="rId3" xr:uid="{B187DD11-D8D8-4A05-B2D5-D669573D0B6D}"/>
     <hyperlink ref="AL190" r:id="rId4" xr:uid="{0ED352F7-3F7F-466D-A86C-3AFB5310436F}"/>
-    <hyperlink ref="C226" r:id="rId5" display="https://leetcode.com/problems/excel-sheet-column-title/" xr:uid="{5EE1CF6B-190D-452F-B940-D9C579EC7E33}"/>
+    <hyperlink ref="B226" r:id="rId5" display="https://leetcode.com/problems/excel-sheet-column-title/" xr:uid="{5EE1CF6B-190D-452F-B940-D9C579EC7E33}"/>
+    <hyperlink ref="B241" r:id="rId6" display="https://leetcode.com/problems/excel-sheet-column-number/" xr:uid="{FF4158B6-879F-4726-B999-B1981E542C68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
doc :: 205. Isomorphic Strings
Leetcodeproblem 205. Isomorphic Strings is solved and documented
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145B4C0A-30B4-4D85-9B42-D3EC5640E0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527BEF0B-CF41-4231-9873-805B0A9E0D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="642">
   <si>
     <t>Title</t>
   </si>
@@ -2177,6 +2177,45 @@
   </si>
   <si>
     <t>171. Excel Sheet Column Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    bool isIsomorphic(string s, string t) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        vector&lt;int&gt; indexS(200, 0); // Stores index of characters in string s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        vector&lt;int&gt; indexT(200, 0); // Stores index of characters in string t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int len = s.length(); // Get the length of both strings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if(len != t.length()) { // If the lengths of the two strings are different, they can't be isomorphic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        for(int i = 0; i &lt; len; i++) { // Iterate through each character of the strings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            if(indexS[s[i]] != indexT[t[i]]) { // Check if the index of the current character in string s is different from the index of the corresponding character in string t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                return false; // If different, strings are not isomorphic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">            indexS[s[i]] = i + 1; // updating position of current character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            indexT[t[i]] = i + 1;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return true; // If the loop completes without returning false, strings are isomorphic</t>
+  </si>
+  <si>
+    <t>205. Isomorphic Strings</t>
   </si>
 </sst>
 </file>
@@ -9977,10 +10016,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28504ADD-8E4E-436B-849F-525BA36E82D6}">
-  <dimension ref="A2:HD256"/>
+  <dimension ref="A2:HD282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
-      <selection activeCell="P228" sqref="P228"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="N257" sqref="N257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -22564,6 +22603,1067 @@
       <c r="AB256" s="9"/>
       <c r="AC256" s="9"/>
     </row>
+    <row r="258" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B258" s="60" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="259" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B259" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C259" s="9"/>
+      <c r="D259" s="9"/>
+      <c r="E259" s="9"/>
+      <c r="F259" s="9"/>
+      <c r="G259" s="9"/>
+      <c r="H259" s="9"/>
+      <c r="I259" s="9"/>
+      <c r="J259" s="9"/>
+      <c r="K259" s="9"/>
+      <c r="L259" s="9"/>
+      <c r="M259" s="9"/>
+      <c r="N259" s="9"/>
+      <c r="O259" s="9"/>
+      <c r="P259" s="9"/>
+      <c r="Q259" s="9"/>
+      <c r="R259" s="9"/>
+      <c r="S259" s="9"/>
+      <c r="T259" s="9"/>
+      <c r="U259" s="9"/>
+      <c r="V259" s="9"/>
+      <c r="W259" s="9"/>
+      <c r="X259" s="9"/>
+      <c r="Y259" s="9"/>
+      <c r="Z259" s="9"/>
+      <c r="AA259" s="9"/>
+      <c r="AB259" s="9"/>
+      <c r="AC259" s="9"/>
+      <c r="AD259" s="9"/>
+      <c r="AE259" s="9"/>
+      <c r="AF259" s="9"/>
+      <c r="AG259" s="9"/>
+      <c r="AH259" s="9"/>
+      <c r="AI259" s="9"/>
+      <c r="AJ259" s="9"/>
+      <c r="AK259" s="9"/>
+      <c r="AL259" s="9"/>
+      <c r="AM259" s="9"/>
+      <c r="AN259" s="9"/>
+      <c r="AO259" s="9"/>
+    </row>
+    <row r="260" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B260" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C260" s="9"/>
+      <c r="D260" s="9"/>
+      <c r="E260" s="9"/>
+      <c r="F260" s="9"/>
+      <c r="G260" s="9"/>
+      <c r="H260" s="9"/>
+      <c r="I260" s="9"/>
+      <c r="J260" s="9"/>
+      <c r="K260" s="9"/>
+      <c r="L260" s="9"/>
+      <c r="M260" s="9"/>
+      <c r="N260" s="9"/>
+      <c r="O260" s="9"/>
+      <c r="P260" s="9"/>
+      <c r="Q260" s="9"/>
+      <c r="R260" s="9"/>
+      <c r="S260" s="9"/>
+      <c r="T260" s="9"/>
+      <c r="U260" s="9"/>
+      <c r="V260" s="9"/>
+      <c r="W260" s="9"/>
+      <c r="X260" s="9"/>
+      <c r="Y260" s="9"/>
+      <c r="Z260" s="9"/>
+      <c r="AA260" s="9"/>
+      <c r="AB260" s="9"/>
+      <c r="AC260" s="9"/>
+      <c r="AD260" s="9"/>
+      <c r="AE260" s="9"/>
+      <c r="AF260" s="9"/>
+      <c r="AG260" s="9"/>
+      <c r="AH260" s="9"/>
+      <c r="AI260" s="9"/>
+      <c r="AJ260" s="9"/>
+      <c r="AK260" s="9"/>
+      <c r="AL260" s="9"/>
+      <c r="AM260" s="9"/>
+      <c r="AN260" s="9"/>
+      <c r="AO260" s="9"/>
+    </row>
+    <row r="261" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B261" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="C261" s="9"/>
+      <c r="D261" s="9"/>
+      <c r="E261" s="9"/>
+      <c r="F261" s="9"/>
+      <c r="G261" s="9"/>
+      <c r="H261" s="9"/>
+      <c r="I261" s="9"/>
+      <c r="J261" s="9"/>
+      <c r="K261" s="9"/>
+      <c r="L261" s="9"/>
+      <c r="M261" s="9"/>
+      <c r="N261" s="9"/>
+      <c r="O261" s="9"/>
+      <c r="P261" s="9"/>
+      <c r="Q261" s="9"/>
+      <c r="R261" s="9"/>
+      <c r="S261" s="9"/>
+      <c r="T261" s="9"/>
+      <c r="U261" s="9"/>
+      <c r="V261" s="9"/>
+      <c r="W261" s="9"/>
+      <c r="X261" s="9"/>
+      <c r="Y261" s="9"/>
+      <c r="Z261" s="9"/>
+      <c r="AA261" s="9"/>
+      <c r="AB261" s="9"/>
+      <c r="AC261" s="9"/>
+      <c r="AD261" s="9"/>
+      <c r="AE261" s="9"/>
+      <c r="AF261" s="9"/>
+      <c r="AG261" s="9"/>
+      <c r="AH261" s="9"/>
+      <c r="AI261" s="9"/>
+      <c r="AJ261" s="9"/>
+      <c r="AK261" s="9"/>
+      <c r="AL261" s="9"/>
+      <c r="AM261" s="9"/>
+      <c r="AN261" s="9"/>
+      <c r="AO261" s="9"/>
+    </row>
+    <row r="262" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B262" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="C262" s="9"/>
+      <c r="D262" s="9"/>
+      <c r="E262" s="9"/>
+      <c r="F262" s="9"/>
+      <c r="G262" s="9"/>
+      <c r="H262" s="9"/>
+      <c r="I262" s="9"/>
+      <c r="J262" s="9"/>
+      <c r="K262" s="9"/>
+      <c r="L262" s="9"/>
+      <c r="M262" s="9"/>
+      <c r="N262" s="9"/>
+      <c r="O262" s="9"/>
+      <c r="P262" s="9"/>
+      <c r="Q262" s="9"/>
+      <c r="R262" s="9"/>
+      <c r="S262" s="9"/>
+      <c r="T262" s="9"/>
+      <c r="U262" s="9"/>
+      <c r="V262" s="9"/>
+      <c r="W262" s="9"/>
+      <c r="X262" s="9"/>
+      <c r="Y262" s="9"/>
+      <c r="Z262" s="9"/>
+      <c r="AA262" s="9"/>
+      <c r="AB262" s="9"/>
+      <c r="AC262" s="9"/>
+      <c r="AD262" s="9"/>
+      <c r="AE262" s="9"/>
+      <c r="AF262" s="9"/>
+      <c r="AG262" s="9"/>
+      <c r="AH262" s="9"/>
+      <c r="AI262" s="9"/>
+      <c r="AJ262" s="9"/>
+      <c r="AK262" s="9"/>
+      <c r="AL262" s="9"/>
+      <c r="AM262" s="9"/>
+      <c r="AN262" s="9"/>
+      <c r="AO262" s="9"/>
+    </row>
+    <row r="263" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B263" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="C263" s="9"/>
+      <c r="D263" s="9"/>
+      <c r="E263" s="9"/>
+      <c r="F263" s="9"/>
+      <c r="G263" s="9"/>
+      <c r="H263" s="9"/>
+      <c r="I263" s="9"/>
+      <c r="J263" s="9"/>
+      <c r="K263" s="9"/>
+      <c r="L263" s="9"/>
+      <c r="M263" s="9"/>
+      <c r="N263" s="9"/>
+      <c r="O263" s="9"/>
+      <c r="P263" s="9"/>
+      <c r="Q263" s="9"/>
+      <c r="R263" s="9"/>
+      <c r="S263" s="9"/>
+      <c r="T263" s="9"/>
+      <c r="U263" s="9"/>
+      <c r="V263" s="9"/>
+      <c r="W263" s="9"/>
+      <c r="X263" s="9"/>
+      <c r="Y263" s="9"/>
+      <c r="Z263" s="9"/>
+      <c r="AA263" s="9"/>
+      <c r="AB263" s="9"/>
+      <c r="AC263" s="9"/>
+      <c r="AD263" s="9"/>
+      <c r="AE263" s="9"/>
+      <c r="AF263" s="9"/>
+      <c r="AG263" s="9"/>
+      <c r="AH263" s="9"/>
+      <c r="AI263" s="9"/>
+      <c r="AJ263" s="9"/>
+      <c r="AK263" s="9"/>
+      <c r="AL263" s="9"/>
+      <c r="AM263" s="9"/>
+      <c r="AN263" s="9"/>
+      <c r="AO263" s="9"/>
+    </row>
+    <row r="264" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B264" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="C264" s="9"/>
+      <c r="D264" s="9"/>
+      <c r="E264" s="9"/>
+      <c r="F264" s="9"/>
+      <c r="G264" s="9"/>
+      <c r="H264" s="9"/>
+      <c r="I264" s="9"/>
+      <c r="J264" s="9"/>
+      <c r="K264" s="9"/>
+      <c r="L264" s="9"/>
+      <c r="M264" s="9"/>
+      <c r="N264" s="9"/>
+      <c r="O264" s="9"/>
+      <c r="P264" s="9"/>
+      <c r="Q264" s="9"/>
+      <c r="R264" s="9"/>
+      <c r="S264" s="9"/>
+      <c r="T264" s="9"/>
+      <c r="U264" s="9"/>
+      <c r="V264" s="9"/>
+      <c r="W264" s="9"/>
+      <c r="X264" s="9"/>
+      <c r="Y264" s="9"/>
+      <c r="Z264" s="9"/>
+      <c r="AA264" s="9"/>
+      <c r="AB264" s="9"/>
+      <c r="AC264" s="9"/>
+      <c r="AD264" s="9"/>
+      <c r="AE264" s="9"/>
+      <c r="AF264" s="9"/>
+      <c r="AG264" s="9"/>
+      <c r="AH264" s="9"/>
+      <c r="AI264" s="9"/>
+      <c r="AJ264" s="9"/>
+      <c r="AK264" s="9"/>
+      <c r="AL264" s="9"/>
+      <c r="AM264" s="9"/>
+      <c r="AN264" s="9"/>
+      <c r="AO264" s="9"/>
+    </row>
+    <row r="265" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B265" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="C265" s="9"/>
+      <c r="D265" s="9"/>
+      <c r="E265" s="9"/>
+      <c r="F265" s="9"/>
+      <c r="G265" s="9"/>
+      <c r="H265" s="9"/>
+      <c r="I265" s="9"/>
+      <c r="J265" s="9"/>
+      <c r="K265" s="9"/>
+      <c r="L265" s="9"/>
+      <c r="M265" s="9"/>
+      <c r="N265" s="9"/>
+      <c r="O265" s="9"/>
+      <c r="P265" s="9"/>
+      <c r="Q265" s="9"/>
+      <c r="R265" s="9"/>
+      <c r="S265" s="9"/>
+      <c r="T265" s="9"/>
+      <c r="U265" s="9"/>
+      <c r="V265" s="9"/>
+      <c r="W265" s="9"/>
+      <c r="X265" s="9"/>
+      <c r="Y265" s="9"/>
+      <c r="Z265" s="9"/>
+      <c r="AA265" s="9"/>
+      <c r="AB265" s="9"/>
+      <c r="AC265" s="9"/>
+      <c r="AD265" s="9"/>
+      <c r="AE265" s="9"/>
+      <c r="AF265" s="9"/>
+      <c r="AG265" s="9"/>
+      <c r="AH265" s="9"/>
+      <c r="AI265" s="9"/>
+      <c r="AJ265" s="9"/>
+      <c r="AK265" s="9"/>
+      <c r="AL265" s="9"/>
+      <c r="AM265" s="9"/>
+      <c r="AN265" s="9"/>
+      <c r="AO265" s="9"/>
+    </row>
+    <row r="266" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B266" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="C266" s="9"/>
+      <c r="D266" s="9"/>
+      <c r="E266" s="9"/>
+      <c r="F266" s="9"/>
+      <c r="G266" s="9"/>
+      <c r="H266" s="9"/>
+      <c r="I266" s="9"/>
+      <c r="J266" s="9"/>
+      <c r="K266" s="9"/>
+      <c r="L266" s="9"/>
+      <c r="M266" s="9"/>
+      <c r="N266" s="9"/>
+      <c r="O266" s="9"/>
+      <c r="P266" s="9"/>
+      <c r="Q266" s="9"/>
+      <c r="R266" s="9"/>
+      <c r="S266" s="9"/>
+      <c r="T266" s="9"/>
+      <c r="U266" s="9"/>
+      <c r="V266" s="9"/>
+      <c r="W266" s="9"/>
+      <c r="X266" s="9"/>
+      <c r="Y266" s="9"/>
+      <c r="Z266" s="9"/>
+      <c r="AA266" s="9"/>
+      <c r="AB266" s="9"/>
+      <c r="AC266" s="9"/>
+      <c r="AD266" s="9"/>
+      <c r="AE266" s="9"/>
+      <c r="AF266" s="9"/>
+      <c r="AG266" s="9"/>
+      <c r="AH266" s="9"/>
+      <c r="AI266" s="9"/>
+      <c r="AJ266" s="9"/>
+      <c r="AK266" s="9"/>
+      <c r="AL266" s="9"/>
+      <c r="AM266" s="9"/>
+      <c r="AN266" s="9"/>
+      <c r="AO266" s="9"/>
+    </row>
+    <row r="267" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B267" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="C267" s="9"/>
+      <c r="D267" s="9"/>
+      <c r="E267" s="9"/>
+      <c r="F267" s="9"/>
+      <c r="G267" s="9"/>
+      <c r="H267" s="9"/>
+      <c r="I267" s="9"/>
+      <c r="J267" s="9"/>
+      <c r="K267" s="9"/>
+      <c r="L267" s="9"/>
+      <c r="M267" s="9"/>
+      <c r="N267" s="9"/>
+      <c r="O267" s="9"/>
+      <c r="P267" s="9"/>
+      <c r="Q267" s="9"/>
+      <c r="R267" s="9"/>
+      <c r="S267" s="9"/>
+      <c r="T267" s="9"/>
+      <c r="U267" s="9"/>
+      <c r="V267" s="9"/>
+      <c r="W267" s="9"/>
+      <c r="X267" s="9"/>
+      <c r="Y267" s="9"/>
+      <c r="Z267" s="9"/>
+      <c r="AA267" s="9"/>
+      <c r="AB267" s="9"/>
+      <c r="AC267" s="9"/>
+      <c r="AD267" s="9"/>
+      <c r="AE267" s="9"/>
+      <c r="AF267" s="9"/>
+      <c r="AG267" s="9"/>
+      <c r="AH267" s="9"/>
+      <c r="AI267" s="9"/>
+      <c r="AJ267" s="9"/>
+      <c r="AK267" s="9"/>
+      <c r="AL267" s="9"/>
+      <c r="AM267" s="9"/>
+      <c r="AN267" s="9"/>
+      <c r="AO267" s="9"/>
+    </row>
+    <row r="268" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B268" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="C268" s="9"/>
+      <c r="D268" s="9"/>
+      <c r="E268" s="9"/>
+      <c r="F268" s="9"/>
+      <c r="G268" s="9"/>
+      <c r="H268" s="9"/>
+      <c r="I268" s="9"/>
+      <c r="J268" s="9"/>
+      <c r="K268" s="9"/>
+      <c r="L268" s="9"/>
+      <c r="M268" s="9"/>
+      <c r="N268" s="9"/>
+      <c r="O268" s="9"/>
+      <c r="P268" s="9"/>
+      <c r="Q268" s="9"/>
+      <c r="R268" s="9"/>
+      <c r="S268" s="9"/>
+      <c r="T268" s="9"/>
+      <c r="U268" s="9"/>
+      <c r="V268" s="9"/>
+      <c r="W268" s="9"/>
+      <c r="X268" s="9"/>
+      <c r="Y268" s="9"/>
+      <c r="Z268" s="9"/>
+      <c r="AA268" s="9"/>
+      <c r="AB268" s="9"/>
+      <c r="AC268" s="9"/>
+      <c r="AD268" s="9"/>
+      <c r="AE268" s="9"/>
+      <c r="AF268" s="9"/>
+      <c r="AG268" s="9"/>
+      <c r="AH268" s="9"/>
+      <c r="AI268" s="9"/>
+      <c r="AJ268" s="9"/>
+      <c r="AK268" s="9"/>
+      <c r="AL268" s="9"/>
+      <c r="AM268" s="9"/>
+      <c r="AN268" s="9"/>
+      <c r="AO268" s="9"/>
+    </row>
+    <row r="269" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B269" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C269" s="9"/>
+      <c r="D269" s="9"/>
+      <c r="E269" s="9"/>
+      <c r="F269" s="9"/>
+      <c r="G269" s="9"/>
+      <c r="H269" s="9"/>
+      <c r="I269" s="9"/>
+      <c r="J269" s="9"/>
+      <c r="K269" s="9"/>
+      <c r="L269" s="9"/>
+      <c r="M269" s="9"/>
+      <c r="N269" s="9"/>
+      <c r="O269" s="9"/>
+      <c r="P269" s="9"/>
+      <c r="Q269" s="9"/>
+      <c r="R269" s="9"/>
+      <c r="S269" s="9"/>
+      <c r="T269" s="9"/>
+      <c r="U269" s="9"/>
+      <c r="V269" s="9"/>
+      <c r="W269" s="9"/>
+      <c r="X269" s="9"/>
+      <c r="Y269" s="9"/>
+      <c r="Z269" s="9"/>
+      <c r="AA269" s="9"/>
+      <c r="AB269" s="9"/>
+      <c r="AC269" s="9"/>
+      <c r="AD269" s="9"/>
+      <c r="AE269" s="9"/>
+      <c r="AF269" s="9"/>
+      <c r="AG269" s="9"/>
+      <c r="AH269" s="9"/>
+      <c r="AI269" s="9"/>
+      <c r="AJ269" s="9"/>
+      <c r="AK269" s="9"/>
+      <c r="AL269" s="9"/>
+      <c r="AM269" s="9"/>
+      <c r="AN269" s="9"/>
+      <c r="AO269" s="9"/>
+    </row>
+    <row r="270" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B270" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="C270" s="9"/>
+      <c r="D270" s="9"/>
+      <c r="E270" s="9"/>
+      <c r="F270" s="9"/>
+      <c r="G270" s="9"/>
+      <c r="H270" s="9"/>
+      <c r="I270" s="9"/>
+      <c r="J270" s="9"/>
+      <c r="K270" s="9"/>
+      <c r="L270" s="9"/>
+      <c r="M270" s="9"/>
+      <c r="N270" s="9"/>
+      <c r="O270" s="9"/>
+      <c r="P270" s="9"/>
+      <c r="Q270" s="9"/>
+      <c r="R270" s="9"/>
+      <c r="S270" s="9"/>
+      <c r="T270" s="9"/>
+      <c r="U270" s="9"/>
+      <c r="V270" s="9"/>
+      <c r="W270" s="9"/>
+      <c r="X270" s="9"/>
+      <c r="Y270" s="9"/>
+      <c r="Z270" s="9"/>
+      <c r="AA270" s="9"/>
+      <c r="AB270" s="9"/>
+      <c r="AC270" s="9"/>
+      <c r="AD270" s="9"/>
+      <c r="AE270" s="9"/>
+      <c r="AF270" s="9"/>
+      <c r="AG270" s="9"/>
+      <c r="AH270" s="9"/>
+      <c r="AI270" s="9"/>
+      <c r="AJ270" s="9"/>
+      <c r="AK270" s="9"/>
+      <c r="AL270" s="9"/>
+      <c r="AM270" s="9"/>
+      <c r="AN270" s="9"/>
+      <c r="AO270" s="9"/>
+    </row>
+    <row r="271" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B271" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="C271" s="9"/>
+      <c r="D271" s="9"/>
+      <c r="E271" s="9"/>
+      <c r="F271" s="9"/>
+      <c r="G271" s="9"/>
+      <c r="H271" s="9"/>
+      <c r="I271" s="9"/>
+      <c r="J271" s="9"/>
+      <c r="K271" s="9"/>
+      <c r="L271" s="9"/>
+      <c r="M271" s="9"/>
+      <c r="N271" s="9"/>
+      <c r="O271" s="9"/>
+      <c r="P271" s="9"/>
+      <c r="Q271" s="9"/>
+      <c r="R271" s="9"/>
+      <c r="S271" s="9"/>
+      <c r="T271" s="9"/>
+      <c r="U271" s="9"/>
+      <c r="V271" s="9"/>
+      <c r="W271" s="9"/>
+      <c r="X271" s="9"/>
+      <c r="Y271" s="9"/>
+      <c r="Z271" s="9"/>
+      <c r="AA271" s="9"/>
+      <c r="AB271" s="9"/>
+      <c r="AC271" s="9"/>
+      <c r="AD271" s="9"/>
+      <c r="AE271" s="9"/>
+      <c r="AF271" s="9"/>
+      <c r="AG271" s="9"/>
+      <c r="AH271" s="9"/>
+      <c r="AI271" s="9"/>
+      <c r="AJ271" s="9"/>
+      <c r="AK271" s="9"/>
+      <c r="AL271" s="9"/>
+      <c r="AM271" s="9"/>
+      <c r="AN271" s="9"/>
+      <c r="AO271" s="9"/>
+    </row>
+    <row r="272" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B272" s="9" t="s">
+        <v>635</v>
+      </c>
+      <c r="C272" s="9"/>
+      <c r="D272" s="9"/>
+      <c r="E272" s="9"/>
+      <c r="F272" s="9"/>
+      <c r="G272" s="9"/>
+      <c r="H272" s="9"/>
+      <c r="I272" s="9"/>
+      <c r="J272" s="9"/>
+      <c r="K272" s="9"/>
+      <c r="L272" s="9"/>
+      <c r="M272" s="9"/>
+      <c r="N272" s="9"/>
+      <c r="O272" s="9"/>
+      <c r="P272" s="9"/>
+      <c r="Q272" s="9"/>
+      <c r="R272" s="9"/>
+      <c r="S272" s="9"/>
+      <c r="T272" s="9"/>
+      <c r="U272" s="9"/>
+      <c r="V272" s="9"/>
+      <c r="W272" s="9"/>
+      <c r="X272" s="9"/>
+      <c r="Y272" s="9"/>
+      <c r="Z272" s="9"/>
+      <c r="AA272" s="9"/>
+      <c r="AB272" s="9"/>
+      <c r="AC272" s="9"/>
+      <c r="AD272" s="9"/>
+      <c r="AE272" s="9"/>
+      <c r="AF272" s="9"/>
+      <c r="AG272" s="9"/>
+      <c r="AH272" s="9"/>
+      <c r="AI272" s="9"/>
+      <c r="AJ272" s="9"/>
+      <c r="AK272" s="9"/>
+      <c r="AL272" s="9"/>
+      <c r="AM272" s="9"/>
+      <c r="AN272" s="9"/>
+      <c r="AO272" s="9"/>
+    </row>
+    <row r="273" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B273" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="C273" s="9"/>
+      <c r="D273" s="9"/>
+      <c r="E273" s="9"/>
+      <c r="F273" s="9"/>
+      <c r="G273" s="9"/>
+      <c r="H273" s="9"/>
+      <c r="I273" s="9"/>
+      <c r="J273" s="9"/>
+      <c r="K273" s="9"/>
+      <c r="L273" s="9"/>
+      <c r="M273" s="9"/>
+      <c r="N273" s="9"/>
+      <c r="O273" s="9"/>
+      <c r="P273" s="9"/>
+      <c r="Q273" s="9"/>
+      <c r="R273" s="9"/>
+      <c r="S273" s="9"/>
+      <c r="T273" s="9"/>
+      <c r="U273" s="9"/>
+      <c r="V273" s="9"/>
+      <c r="W273" s="9"/>
+      <c r="X273" s="9"/>
+      <c r="Y273" s="9"/>
+      <c r="Z273" s="9"/>
+      <c r="AA273" s="9"/>
+      <c r="AB273" s="9"/>
+      <c r="AC273" s="9"/>
+      <c r="AD273" s="9"/>
+      <c r="AE273" s="9"/>
+      <c r="AF273" s="9"/>
+      <c r="AG273" s="9"/>
+      <c r="AH273" s="9"/>
+      <c r="AI273" s="9"/>
+      <c r="AJ273" s="9"/>
+      <c r="AK273" s="9"/>
+      <c r="AL273" s="9"/>
+      <c r="AM273" s="9"/>
+      <c r="AN273" s="9"/>
+      <c r="AO273" s="9"/>
+    </row>
+    <row r="274" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B274" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C274" s="9"/>
+      <c r="D274" s="9"/>
+      <c r="E274" s="9"/>
+      <c r="F274" s="9"/>
+      <c r="G274" s="9"/>
+      <c r="H274" s="9"/>
+      <c r="I274" s="9"/>
+      <c r="J274" s="9"/>
+      <c r="K274" s="9"/>
+      <c r="L274" s="9"/>
+      <c r="M274" s="9"/>
+      <c r="N274" s="9"/>
+      <c r="O274" s="9"/>
+      <c r="P274" s="9"/>
+      <c r="Q274" s="9"/>
+      <c r="R274" s="9"/>
+      <c r="S274" s="9"/>
+      <c r="T274" s="9"/>
+      <c r="U274" s="9"/>
+      <c r="V274" s="9"/>
+      <c r="W274" s="9"/>
+      <c r="X274" s="9"/>
+      <c r="Y274" s="9"/>
+      <c r="Z274" s="9"/>
+      <c r="AA274" s="9"/>
+      <c r="AB274" s="9"/>
+      <c r="AC274" s="9"/>
+      <c r="AD274" s="9"/>
+      <c r="AE274" s="9"/>
+      <c r="AF274" s="9"/>
+      <c r="AG274" s="9"/>
+      <c r="AH274" s="9"/>
+      <c r="AI274" s="9"/>
+      <c r="AJ274" s="9"/>
+      <c r="AK274" s="9"/>
+      <c r="AL274" s="9"/>
+      <c r="AM274" s="9"/>
+      <c r="AN274" s="9"/>
+      <c r="AO274" s="9"/>
+    </row>
+    <row r="275" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B275" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="C275" s="9"/>
+      <c r="D275" s="9"/>
+      <c r="E275" s="9"/>
+      <c r="F275" s="9"/>
+      <c r="G275" s="9"/>
+      <c r="H275" s="9"/>
+      <c r="I275" s="9"/>
+      <c r="J275" s="9"/>
+      <c r="K275" s="9"/>
+      <c r="L275" s="9"/>
+      <c r="M275" s="9"/>
+      <c r="N275" s="9"/>
+      <c r="O275" s="9"/>
+      <c r="P275" s="9"/>
+      <c r="Q275" s="9"/>
+      <c r="R275" s="9"/>
+      <c r="S275" s="9"/>
+      <c r="T275" s="9"/>
+      <c r="U275" s="9"/>
+      <c r="V275" s="9"/>
+      <c r="W275" s="9"/>
+      <c r="X275" s="9"/>
+      <c r="Y275" s="9"/>
+      <c r="Z275" s="9"/>
+      <c r="AA275" s="9"/>
+      <c r="AB275" s="9"/>
+      <c r="AC275" s="9"/>
+      <c r="AD275" s="9"/>
+      <c r="AE275" s="9"/>
+      <c r="AF275" s="9"/>
+      <c r="AG275" s="9"/>
+      <c r="AH275" s="9"/>
+      <c r="AI275" s="9"/>
+      <c r="AJ275" s="9"/>
+      <c r="AK275" s="9"/>
+      <c r="AL275" s="9"/>
+      <c r="AM275" s="9"/>
+      <c r="AN275" s="9"/>
+      <c r="AO275" s="9"/>
+    </row>
+    <row r="276" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B276" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="C276" s="9"/>
+      <c r="D276" s="9"/>
+      <c r="E276" s="9"/>
+      <c r="F276" s="9"/>
+      <c r="G276" s="9"/>
+      <c r="H276" s="9"/>
+      <c r="I276" s="9"/>
+      <c r="J276" s="9"/>
+      <c r="K276" s="9"/>
+      <c r="L276" s="9"/>
+      <c r="M276" s="9"/>
+      <c r="N276" s="9"/>
+      <c r="O276" s="9"/>
+      <c r="P276" s="9"/>
+      <c r="Q276" s="9"/>
+      <c r="R276" s="9"/>
+      <c r="S276" s="9"/>
+      <c r="T276" s="9"/>
+      <c r="U276" s="9"/>
+      <c r="V276" s="9"/>
+      <c r="W276" s="9"/>
+      <c r="X276" s="9"/>
+      <c r="Y276" s="9"/>
+      <c r="Z276" s="9"/>
+      <c r="AA276" s="9"/>
+      <c r="AB276" s="9"/>
+      <c r="AC276" s="9"/>
+      <c r="AD276" s="9"/>
+      <c r="AE276" s="9"/>
+      <c r="AF276" s="9"/>
+      <c r="AG276" s="9"/>
+      <c r="AH276" s="9"/>
+      <c r="AI276" s="9"/>
+      <c r="AJ276" s="9"/>
+      <c r="AK276" s="9"/>
+      <c r="AL276" s="9"/>
+      <c r="AM276" s="9"/>
+      <c r="AN276" s="9"/>
+      <c r="AO276" s="9"/>
+    </row>
+    <row r="277" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B277" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="C277" s="9"/>
+      <c r="D277" s="9"/>
+      <c r="E277" s="9"/>
+      <c r="F277" s="9"/>
+      <c r="G277" s="9"/>
+      <c r="H277" s="9"/>
+      <c r="I277" s="9"/>
+      <c r="J277" s="9"/>
+      <c r="K277" s="9"/>
+      <c r="L277" s="9"/>
+      <c r="M277" s="9"/>
+      <c r="N277" s="9"/>
+      <c r="O277" s="9"/>
+      <c r="P277" s="9"/>
+      <c r="Q277" s="9"/>
+      <c r="R277" s="9"/>
+      <c r="S277" s="9"/>
+      <c r="T277" s="9"/>
+      <c r="U277" s="9"/>
+      <c r="V277" s="9"/>
+      <c r="W277" s="9"/>
+      <c r="X277" s="9"/>
+      <c r="Y277" s="9"/>
+      <c r="Z277" s="9"/>
+      <c r="AA277" s="9"/>
+      <c r="AB277" s="9"/>
+      <c r="AC277" s="9"/>
+      <c r="AD277" s="9"/>
+      <c r="AE277" s="9"/>
+      <c r="AF277" s="9"/>
+      <c r="AG277" s="9"/>
+      <c r="AH277" s="9"/>
+      <c r="AI277" s="9"/>
+      <c r="AJ277" s="9"/>
+      <c r="AK277" s="9"/>
+      <c r="AL277" s="9"/>
+      <c r="AM277" s="9"/>
+      <c r="AN277" s="9"/>
+      <c r="AO277" s="9"/>
+    </row>
+    <row r="278" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B278" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C278" s="9"/>
+      <c r="D278" s="9"/>
+      <c r="E278" s="9"/>
+      <c r="F278" s="9"/>
+      <c r="G278" s="9"/>
+      <c r="H278" s="9"/>
+      <c r="I278" s="9"/>
+      <c r="J278" s="9"/>
+      <c r="K278" s="9"/>
+      <c r="L278" s="9"/>
+      <c r="M278" s="9"/>
+      <c r="N278" s="9"/>
+      <c r="O278" s="9"/>
+      <c r="P278" s="9"/>
+      <c r="Q278" s="9"/>
+      <c r="R278" s="9"/>
+      <c r="S278" s="9"/>
+      <c r="T278" s="9"/>
+      <c r="U278" s="9"/>
+      <c r="V278" s="9"/>
+      <c r="W278" s="9"/>
+      <c r="X278" s="9"/>
+      <c r="Y278" s="9"/>
+      <c r="Z278" s="9"/>
+      <c r="AA278" s="9"/>
+      <c r="AB278" s="9"/>
+      <c r="AC278" s="9"/>
+      <c r="AD278" s="9"/>
+      <c r="AE278" s="9"/>
+      <c r="AF278" s="9"/>
+      <c r="AG278" s="9"/>
+      <c r="AH278" s="9"/>
+      <c r="AI278" s="9"/>
+      <c r="AJ278" s="9"/>
+      <c r="AK278" s="9"/>
+      <c r="AL278" s="9"/>
+      <c r="AM278" s="9"/>
+      <c r="AN278" s="9"/>
+      <c r="AO278" s="9"/>
+    </row>
+    <row r="279" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B279" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="C279" s="9"/>
+      <c r="D279" s="9"/>
+      <c r="E279" s="9"/>
+      <c r="F279" s="9"/>
+      <c r="G279" s="9"/>
+      <c r="H279" s="9"/>
+      <c r="I279" s="9"/>
+      <c r="J279" s="9"/>
+      <c r="K279" s="9"/>
+      <c r="L279" s="9"/>
+      <c r="M279" s="9"/>
+      <c r="N279" s="9"/>
+      <c r="O279" s="9"/>
+      <c r="P279" s="9"/>
+      <c r="Q279" s="9"/>
+      <c r="R279" s="9"/>
+      <c r="S279" s="9"/>
+      <c r="T279" s="9"/>
+      <c r="U279" s="9"/>
+      <c r="V279" s="9"/>
+      <c r="W279" s="9"/>
+      <c r="X279" s="9"/>
+      <c r="Y279" s="9"/>
+      <c r="Z279" s="9"/>
+      <c r="AA279" s="9"/>
+      <c r="AB279" s="9"/>
+      <c r="AC279" s="9"/>
+      <c r="AD279" s="9"/>
+      <c r="AE279" s="9"/>
+      <c r="AF279" s="9"/>
+      <c r="AG279" s="9"/>
+      <c r="AH279" s="9"/>
+      <c r="AI279" s="9"/>
+      <c r="AJ279" s="9"/>
+      <c r="AK279" s="9"/>
+      <c r="AL279" s="9"/>
+      <c r="AM279" s="9"/>
+      <c r="AN279" s="9"/>
+      <c r="AO279" s="9"/>
+    </row>
+    <row r="280" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B280" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="C280" s="9"/>
+      <c r="D280" s="9"/>
+      <c r="E280" s="9"/>
+      <c r="F280" s="9"/>
+      <c r="G280" s="9"/>
+      <c r="H280" s="9"/>
+      <c r="I280" s="9"/>
+      <c r="J280" s="9"/>
+      <c r="K280" s="9"/>
+      <c r="L280" s="9"/>
+      <c r="M280" s="9"/>
+      <c r="N280" s="9"/>
+      <c r="O280" s="9"/>
+      <c r="P280" s="9"/>
+      <c r="Q280" s="9"/>
+      <c r="R280" s="9"/>
+      <c r="S280" s="9"/>
+      <c r="T280" s="9"/>
+      <c r="U280" s="9"/>
+      <c r="V280" s="9"/>
+      <c r="W280" s="9"/>
+      <c r="X280" s="9"/>
+      <c r="Y280" s="9"/>
+      <c r="Z280" s="9"/>
+      <c r="AA280" s="9"/>
+      <c r="AB280" s="9"/>
+      <c r="AC280" s="9"/>
+      <c r="AD280" s="9"/>
+      <c r="AE280" s="9"/>
+      <c r="AF280" s="9"/>
+      <c r="AG280" s="9"/>
+      <c r="AH280" s="9"/>
+      <c r="AI280" s="9"/>
+      <c r="AJ280" s="9"/>
+      <c r="AK280" s="9"/>
+      <c r="AL280" s="9"/>
+      <c r="AM280" s="9"/>
+      <c r="AN280" s="9"/>
+      <c r="AO280" s="9"/>
+    </row>
+    <row r="281" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B281" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C281" s="9"/>
+      <c r="D281" s="9"/>
+      <c r="E281" s="9"/>
+      <c r="F281" s="9"/>
+      <c r="G281" s="9"/>
+      <c r="H281" s="9"/>
+      <c r="I281" s="9"/>
+      <c r="J281" s="9"/>
+      <c r="K281" s="9"/>
+      <c r="L281" s="9"/>
+      <c r="M281" s="9"/>
+      <c r="N281" s="9"/>
+      <c r="O281" s="9"/>
+      <c r="P281" s="9"/>
+      <c r="Q281" s="9"/>
+      <c r="R281" s="9"/>
+      <c r="S281" s="9"/>
+      <c r="T281" s="9"/>
+      <c r="U281" s="9"/>
+      <c r="V281" s="9"/>
+      <c r="W281" s="9"/>
+      <c r="X281" s="9"/>
+      <c r="Y281" s="9"/>
+      <c r="Z281" s="9"/>
+      <c r="AA281" s="9"/>
+      <c r="AB281" s="9"/>
+      <c r="AC281" s="9"/>
+      <c r="AD281" s="9"/>
+      <c r="AE281" s="9"/>
+      <c r="AF281" s="9"/>
+      <c r="AG281" s="9"/>
+      <c r="AH281" s="9"/>
+      <c r="AI281" s="9"/>
+      <c r="AJ281" s="9"/>
+      <c r="AK281" s="9"/>
+      <c r="AL281" s="9"/>
+      <c r="AM281" s="9"/>
+      <c r="AN281" s="9"/>
+      <c r="AO281" s="9"/>
+    </row>
+    <row r="282" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B282" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C282" s="9"/>
+      <c r="D282" s="9"/>
+      <c r="E282" s="9"/>
+      <c r="F282" s="9"/>
+      <c r="G282" s="9"/>
+      <c r="H282" s="9"/>
+      <c r="I282" s="9"/>
+      <c r="J282" s="9"/>
+      <c r="K282" s="9"/>
+      <c r="L282" s="9"/>
+      <c r="M282" s="9"/>
+      <c r="N282" s="9"/>
+      <c r="O282" s="9"/>
+      <c r="P282" s="9"/>
+      <c r="Q282" s="9"/>
+      <c r="R282" s="9"/>
+      <c r="S282" s="9"/>
+      <c r="T282" s="9"/>
+      <c r="U282" s="9"/>
+      <c r="V282" s="9"/>
+      <c r="W282" s="9"/>
+      <c r="X282" s="9"/>
+      <c r="Y282" s="9"/>
+      <c r="Z282" s="9"/>
+      <c r="AA282" s="9"/>
+      <c r="AB282" s="9"/>
+      <c r="AC282" s="9"/>
+      <c r="AD282" s="9"/>
+      <c r="AE282" s="9"/>
+      <c r="AF282" s="9"/>
+      <c r="AG282" s="9"/>
+      <c r="AH282" s="9"/>
+      <c r="AI282" s="9"/>
+      <c r="AJ282" s="9"/>
+      <c r="AK282" s="9"/>
+      <c r="AL282" s="9"/>
+      <c r="AM282" s="9"/>
+      <c r="AN282" s="9"/>
+      <c r="AO282" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{9E8104E2-0B1A-498B-A07D-38DAF385409A}"/>
@@ -22572,9 +23672,10 @@
     <hyperlink ref="AL190" r:id="rId4" xr:uid="{0ED352F7-3F7F-466D-A86C-3AFB5310436F}"/>
     <hyperlink ref="B226" r:id="rId5" display="https://leetcode.com/problems/excel-sheet-column-title/" xr:uid="{5EE1CF6B-190D-452F-B940-D9C579EC7E33}"/>
     <hyperlink ref="B241" r:id="rId6" display="https://leetcode.com/problems/excel-sheet-column-number/" xr:uid="{FF4158B6-879F-4726-B999-B1981E542C68}"/>
+    <hyperlink ref="B258" r:id="rId7" display="https://leetcode.com/problems/isomorphic-strings/" xr:uid="{6590CC4B-CD8A-42F0-A21C-DF5796D0F918}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
doc:: 58. Length of Last Word
Leetcode Problem 58. Length of Last Word is solved and documented
</commit_message>
<xml_diff>
--- a/11-C++/leetcode.xlsx
+++ b/11-C++/leetcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LEARNING\11-C++\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527BEF0B-CF41-4231-9873-805B0A9E0D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE633DB-ABCF-4F22-9CE6-0788384CD315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{8FBBEE65-962B-405C-9512-844F8D7DE21A}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="652">
   <si>
     <t>Title</t>
   </si>
@@ -2216,6 +2216,36 @@
   </si>
   <si>
     <t>205. Isomorphic Strings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int lengthOfLastWord(string s) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        int length = 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        bool counting = false;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        for (int i = s.length() - 1; i &gt;= 0; i--) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            if (s[i] != ' ') {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                counting = true;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                length++;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            else if (counting) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return length;</t>
+  </si>
+  <si>
+    <t>58. Length of Last Word</t>
   </si>
 </sst>
 </file>
@@ -10016,10 +10046,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28504ADD-8E4E-436B-849F-525BA36E82D6}">
-  <dimension ref="A2:HD282"/>
+  <dimension ref="A2:HD303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
-      <selection activeCell="N257" sqref="N257"/>
+    <sheetView tabSelected="1" topLeftCell="A273" workbookViewId="0">
+      <selection activeCell="P281" sqref="P281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -23664,6 +23694,296 @@
       <c r="AN282" s="9"/>
       <c r="AO282" s="9"/>
     </row>
+    <row r="284" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B284" s="60" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="285" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B285" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="C285" s="9"/>
+      <c r="D285" s="9"/>
+      <c r="E285" s="9"/>
+      <c r="F285" s="9"/>
+      <c r="G285" s="9"/>
+      <c r="H285" s="9"/>
+      <c r="I285" s="9"/>
+      <c r="J285" s="9"/>
+      <c r="K285" s="9"/>
+      <c r="L285" s="9"/>
+    </row>
+    <row r="286" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B286" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C286" s="9"/>
+      <c r="D286" s="9"/>
+      <c r="E286" s="9"/>
+      <c r="F286" s="9"/>
+      <c r="G286" s="9"/>
+      <c r="H286" s="9"/>
+      <c r="I286" s="9"/>
+      <c r="J286" s="9"/>
+      <c r="K286" s="9"/>
+      <c r="L286" s="9"/>
+    </row>
+    <row r="287" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B287" s="9" t="s">
+        <v>642</v>
+      </c>
+      <c r="C287" s="9"/>
+      <c r="D287" s="9"/>
+      <c r="E287" s="9"/>
+      <c r="F287" s="9"/>
+      <c r="G287" s="9"/>
+      <c r="H287" s="9"/>
+      <c r="I287" s="9"/>
+      <c r="J287" s="9"/>
+      <c r="K287" s="9"/>
+      <c r="L287" s="9"/>
+    </row>
+    <row r="288" spans="2:41" x14ac:dyDescent="0.4">
+      <c r="B288" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="C288" s="9"/>
+      <c r="D288" s="9"/>
+      <c r="E288" s="9"/>
+      <c r="F288" s="9"/>
+      <c r="G288" s="9"/>
+      <c r="H288" s="9"/>
+      <c r="I288" s="9"/>
+      <c r="J288" s="9"/>
+      <c r="K288" s="9"/>
+      <c r="L288" s="9"/>
+    </row>
+    <row r="289" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B289" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="C289" s="9"/>
+      <c r="D289" s="9"/>
+      <c r="E289" s="9"/>
+      <c r="F289" s="9"/>
+      <c r="G289" s="9"/>
+      <c r="H289" s="9"/>
+      <c r="I289" s="9"/>
+      <c r="J289" s="9"/>
+      <c r="K289" s="9"/>
+      <c r="L289" s="9"/>
+    </row>
+    <row r="290" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B290" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="C290" s="9"/>
+      <c r="D290" s="9"/>
+      <c r="E290" s="9"/>
+      <c r="F290" s="9"/>
+      <c r="G290" s="9"/>
+      <c r="H290" s="9"/>
+      <c r="I290" s="9"/>
+      <c r="J290" s="9"/>
+      <c r="K290" s="9"/>
+      <c r="L290" s="9"/>
+    </row>
+    <row r="291" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B291" s="9" t="s">
+        <v>645</v>
+      </c>
+      <c r="C291" s="9"/>
+      <c r="D291" s="9"/>
+      <c r="E291" s="9"/>
+      <c r="F291" s="9"/>
+      <c r="G291" s="9"/>
+      <c r="H291" s="9"/>
+      <c r="I291" s="9"/>
+      <c r="J291" s="9"/>
+      <c r="K291" s="9"/>
+      <c r="L291" s="9"/>
+    </row>
+    <row r="292" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B292" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="C292" s="9"/>
+      <c r="D292" s="9"/>
+      <c r="E292" s="9"/>
+      <c r="F292" s="9"/>
+      <c r="G292" s="9"/>
+      <c r="H292" s="9"/>
+      <c r="I292" s="9"/>
+      <c r="J292" s="9"/>
+      <c r="K292" s="9"/>
+      <c r="L292" s="9"/>
+    </row>
+    <row r="293" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B293" s="9" t="s">
+        <v>647</v>
+      </c>
+      <c r="C293" s="9"/>
+      <c r="D293" s="9"/>
+      <c r="E293" s="9"/>
+      <c r="F293" s="9"/>
+      <c r="G293" s="9"/>
+      <c r="H293" s="9"/>
+      <c r="I293" s="9"/>
+      <c r="J293" s="9"/>
+      <c r="K293" s="9"/>
+      <c r="L293" s="9"/>
+    </row>
+    <row r="294" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B294" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="C294" s="9"/>
+      <c r="D294" s="9"/>
+      <c r="E294" s="9"/>
+      <c r="F294" s="9"/>
+      <c r="G294" s="9"/>
+      <c r="H294" s="9"/>
+      <c r="I294" s="9"/>
+      <c r="J294" s="9"/>
+      <c r="K294" s="9"/>
+      <c r="L294" s="9"/>
+    </row>
+    <row r="295" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B295" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C295" s="9"/>
+      <c r="D295" s="9"/>
+      <c r="E295" s="9"/>
+      <c r="F295" s="9"/>
+      <c r="G295" s="9"/>
+      <c r="H295" s="9"/>
+      <c r="I295" s="9"/>
+      <c r="J295" s="9"/>
+      <c r="K295" s="9"/>
+      <c r="L295" s="9"/>
+    </row>
+    <row r="296" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B296" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="C296" s="9"/>
+      <c r="D296" s="9"/>
+      <c r="E296" s="9"/>
+      <c r="F296" s="9"/>
+      <c r="G296" s="9"/>
+      <c r="H296" s="9"/>
+      <c r="I296" s="9"/>
+      <c r="J296" s="9"/>
+      <c r="K296" s="9"/>
+      <c r="L296" s="9"/>
+    </row>
+    <row r="297" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B297" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="C297" s="9"/>
+      <c r="D297" s="9"/>
+      <c r="E297" s="9"/>
+      <c r="F297" s="9"/>
+      <c r="G297" s="9"/>
+      <c r="H297" s="9"/>
+      <c r="I297" s="9"/>
+      <c r="J297" s="9"/>
+      <c r="K297" s="9"/>
+      <c r="L297" s="9"/>
+    </row>
+    <row r="298" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B298" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="C298" s="9"/>
+      <c r="D298" s="9"/>
+      <c r="E298" s="9"/>
+      <c r="F298" s="9"/>
+      <c r="G298" s="9"/>
+      <c r="H298" s="9"/>
+      <c r="I298" s="9"/>
+      <c r="J298" s="9"/>
+      <c r="K298" s="9"/>
+      <c r="L298" s="9"/>
+    </row>
+    <row r="299" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B299" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C299" s="9"/>
+      <c r="D299" s="9"/>
+      <c r="E299" s="9"/>
+      <c r="F299" s="9"/>
+      <c r="G299" s="9"/>
+      <c r="H299" s="9"/>
+      <c r="I299" s="9"/>
+      <c r="J299" s="9"/>
+      <c r="K299" s="9"/>
+      <c r="L299" s="9"/>
+    </row>
+    <row r="300" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B300" s="9" t="s">
+        <v>504</v>
+      </c>
+      <c r="C300" s="9"/>
+      <c r="D300" s="9"/>
+      <c r="E300" s="9"/>
+      <c r="F300" s="9"/>
+      <c r="G300" s="9"/>
+      <c r="H300" s="9"/>
+      <c r="I300" s="9"/>
+      <c r="J300" s="9"/>
+      <c r="K300" s="9"/>
+      <c r="L300" s="9"/>
+    </row>
+    <row r="301" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B301" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="C301" s="9"/>
+      <c r="D301" s="9"/>
+      <c r="E301" s="9"/>
+      <c r="F301" s="9"/>
+      <c r="G301" s="9"/>
+      <c r="H301" s="9"/>
+      <c r="I301" s="9"/>
+      <c r="J301" s="9"/>
+      <c r="K301" s="9"/>
+      <c r="L301" s="9"/>
+    </row>
+    <row r="302" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B302" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C302" s="9"/>
+      <c r="D302" s="9"/>
+      <c r="E302" s="9"/>
+      <c r="F302" s="9"/>
+      <c r="G302" s="9"/>
+      <c r="H302" s="9"/>
+      <c r="I302" s="9"/>
+      <c r="J302" s="9"/>
+      <c r="K302" s="9"/>
+      <c r="L302" s="9"/>
+    </row>
+    <row r="303" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B303" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="C303" s="9"/>
+      <c r="D303" s="9"/>
+      <c r="E303" s="9"/>
+      <c r="F303" s="9"/>
+      <c r="G303" s="9"/>
+      <c r="H303" s="9"/>
+      <c r="I303" s="9"/>
+      <c r="J303" s="9"/>
+      <c r="K303" s="9"/>
+      <c r="L303" s="9"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{9E8104E2-0B1A-498B-A07D-38DAF385409A}"/>
@@ -23673,9 +23993,10 @@
     <hyperlink ref="B226" r:id="rId5" display="https://leetcode.com/problems/excel-sheet-column-title/" xr:uid="{5EE1CF6B-190D-452F-B940-D9C579EC7E33}"/>
     <hyperlink ref="B241" r:id="rId6" display="https://leetcode.com/problems/excel-sheet-column-number/" xr:uid="{FF4158B6-879F-4726-B999-B1981E542C68}"/>
     <hyperlink ref="B258" r:id="rId7" display="https://leetcode.com/problems/isomorphic-strings/" xr:uid="{6590CC4B-CD8A-42F0-A21C-DF5796D0F918}"/>
+    <hyperlink ref="B284" r:id="rId8" display="https://leetcode.com/problems/length-of-last-word/" xr:uid="{C4952CAC-CCFD-46F4-BBD9-754F7E47C88C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>